<commit_message>
EUR 3M curve bootstrap - work in progress - fix EUR_YC3MRH_FUT3MM4
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC3MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -309,7 +309,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="192">
   <si>
     <t>Error</t>
   </si>
@@ -883,6 +883,9 @@
   <si>
     <t>EUR_YCRH_SwapsFromBasis</t>
   </si>
+  <si>
+    <t>incorrectly selected in old build because of bug in setting futures quotes</t>
+  </si>
 </sst>
 </file>
 
@@ -1031,7 +1034,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1090,6 +1093,12 @@
       <patternFill patternType="gray0625">
         <fgColor indexed="22"/>
         <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1559,7 +1568,7 @@
     <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -2029,6 +2038,13 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2038,13 +2054,6 @@
     <xf numFmtId="0" fontId="19" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2060,6 +2069,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2605,7 +2618,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AG95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2630,19 +2643,19 @@
       </c>
     </row>
     <row r="2" spans="1:33" s="53" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="220" t="s">
+      <c r="B2" s="217" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="221"/>
-      <c r="D2" s="221"/>
-      <c r="E2" s="221"/>
-      <c r="F2" s="222"/>
-      <c r="K2" s="217" t="s">
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="219"/>
+      <c r="K2" s="220" t="s">
         <v>163</v>
       </c>
-      <c r="L2" s="218"/>
-      <c r="M2" s="218"/>
-      <c r="N2" s="219"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="222"/>
     </row>
     <row r="3" spans="1:33" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="53"/>
@@ -3000,7 +3013,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="86">
-        <v>41646.136203703703</v>
+        <v>41646.188391203701</v>
       </c>
       <c r="E11" s="58"/>
       <c r="F11" s="57"/>
@@ -3047,12 +3060,12 @@
       <c r="H12" s="53"/>
       <c r="I12" s="53"/>
       <c r="J12" s="53"/>
-      <c r="K12" s="217" t="s">
+      <c r="K12" s="220" t="s">
         <v>159</v>
       </c>
-      <c r="L12" s="218"/>
-      <c r="M12" s="218"/>
-      <c r="N12" s="219"/>
+      <c r="L12" s="221"/>
+      <c r="M12" s="221"/>
+      <c r="N12" s="222"/>
       <c r="O12" s="53"/>
       <c r="P12" s="53"/>
       <c r="Q12" s="53"/>
@@ -3116,7 +3129,7 @@
       </c>
       <c r="D14" s="83" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYC3M#0000</v>
+        <v>_EURYC3M#0008</v>
       </c>
       <c r="E14" s="58"/>
       <c r="F14" s="57"/>
@@ -3331,12 +3344,12 @@
       <c r="H19" s="53"/>
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
-      <c r="K19" s="217" t="s">
+      <c r="K19" s="220" t="s">
         <v>163</v>
       </c>
-      <c r="L19" s="218"/>
-      <c r="M19" s="218"/>
-      <c r="N19" s="219"/>
+      <c r="L19" s="221"/>
+      <c r="M19" s="221"/>
+      <c r="N19" s="222"/>
       <c r="O19" s="53"/>
       <c r="P19" s="53"/>
       <c r="Q19" s="53"/>
@@ -3752,7 +3765,7 @@
       </c>
       <c r="D29" s="59" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v>qlPiecewiseYieldCurveData - 1st instrument (maturity: January 23rd, 2014) has an invalid quote</v>
+        <v>qlPiecewiseYieldCurveData - 13th instrument (maturity: January 9th, 2017) has an invalid quote</v>
       </c>
       <c r="E29" s="58"/>
       <c r="F29" s="57"/>
@@ -3760,12 +3773,12 @@
       <c r="H29" s="53"/>
       <c r="I29" s="53"/>
       <c r="J29" s="53"/>
-      <c r="K29" s="217" t="s">
+      <c r="K29" s="220" t="s">
         <v>159</v>
       </c>
-      <c r="L29" s="218"/>
-      <c r="M29" s="218"/>
-      <c r="N29" s="219"/>
+      <c r="L29" s="221"/>
+      <c r="M29" s="221"/>
+      <c r="N29" s="222"/>
       <c r="O29" s="53"/>
       <c r="P29" s="53"/>
       <c r="Q29" s="53"/>
@@ -4019,12 +4032,12 @@
       <c r="H36" s="53"/>
       <c r="I36" s="53"/>
       <c r="J36" s="53"/>
-      <c r="K36" s="217" t="s">
+      <c r="K36" s="220" t="s">
         <v>163</v>
       </c>
-      <c r="L36" s="218"/>
-      <c r="M36" s="218"/>
-      <c r="N36" s="219"/>
+      <c r="L36" s="221"/>
+      <c r="M36" s="221"/>
+      <c r="N36" s="222"/>
       <c r="O36" s="53"/>
       <c r="P36" s="53"/>
       <c r="Q36" s="53"/>
@@ -4394,12 +4407,12 @@
       <c r="H46" s="53"/>
       <c r="I46" s="53"/>
       <c r="J46" s="53"/>
-      <c r="K46" s="217" t="s">
+      <c r="K46" s="220" t="s">
         <v>159</v>
       </c>
-      <c r="L46" s="218"/>
-      <c r="M46" s="218"/>
-      <c r="N46" s="219"/>
+      <c r="L46" s="221"/>
+      <c r="M46" s="221"/>
+      <c r="N46" s="222"/>
       <c r="O46" s="53"/>
       <c r="P46" s="53"/>
       <c r="Q46" s="53"/>
@@ -4653,12 +4666,12 @@
       <c r="H53" s="53"/>
       <c r="I53" s="53"/>
       <c r="J53" s="53"/>
-      <c r="K53" s="217" t="s">
+      <c r="K53" s="220" t="s">
         <v>163</v>
       </c>
-      <c r="L53" s="218"/>
-      <c r="M53" s="218"/>
-      <c r="N53" s="219"/>
+      <c r="L53" s="221"/>
+      <c r="M53" s="221"/>
+      <c r="N53" s="222"/>
       <c r="O53" s="53"/>
       <c r="P53" s="53"/>
       <c r="Q53" s="53"/>
@@ -5028,12 +5041,12 @@
       <c r="H63" s="53"/>
       <c r="I63" s="53"/>
       <c r="J63" s="53"/>
-      <c r="K63" s="217" t="s">
+      <c r="K63" s="220" t="s">
         <v>159</v>
       </c>
-      <c r="L63" s="218"/>
-      <c r="M63" s="218"/>
-      <c r="N63" s="219"/>
+      <c r="L63" s="221"/>
+      <c r="M63" s="221"/>
+      <c r="N63" s="222"/>
       <c r="O63" s="53"/>
       <c r="P63" s="53"/>
       <c r="Q63" s="53"/>
@@ -5295,12 +5308,12 @@
     </row>
     <row r="74" spans="1:33" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K75" s="217" t="s">
+      <c r="K75" s="220" t="s">
         <v>163</v>
       </c>
-      <c r="L75" s="218"/>
-      <c r="M75" s="218"/>
-      <c r="N75" s="219"/>
+      <c r="L75" s="221"/>
+      <c r="M75" s="221"/>
+      <c r="N75" s="222"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.2">
       <c r="K76" s="136"/>
@@ -5380,12 +5393,12 @@
       <c r="N84" s="121"/>
     </row>
     <row r="85" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K85" s="217" t="s">
+      <c r="K85" s="220" t="s">
         <v>159</v>
       </c>
-      <c r="L85" s="218"/>
-      <c r="M85" s="218"/>
-      <c r="N85" s="219"/>
+      <c r="L85" s="221"/>
+      <c r="M85" s="221"/>
+      <c r="N85" s="222"/>
     </row>
     <row r="86" spans="11:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K86" s="128"/>
@@ -5483,17 +5496,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K29:N29"/>
     <mergeCell ref="K85:N85"/>
     <mergeCell ref="K36:N36"/>
     <mergeCell ref="K46:N46"/>
     <mergeCell ref="K53:N53"/>
     <mergeCell ref="K63:N63"/>
     <mergeCell ref="K75:N75"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K29:N29"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 IZ25 SV25 ACR25 AMN25 AWJ25 BGF25 BQB25 BZX25 CJT25 CTP25 DDL25 DNH25 DXD25 EGZ25 EQV25 FAR25 FKN25 FUJ25 GEF25 GOB25 GXX25 HHT25 HRP25 IBL25 ILH25 IVD25 JEZ25 JOV25 JYR25 KIN25 KSJ25 LCF25 LMB25 LVX25 MFT25 MPP25 MZL25 NJH25 NTD25 OCZ25 OMV25 OWR25 PGN25 PQJ25 QAF25 QKB25 QTX25 RDT25 RNP25 RXL25 SHH25 SRD25 TAZ25 TKV25 TUR25 UEN25 UOJ25 UYF25 VIB25 VRX25 WBT25 WLP25 WVL25 D65561 IZ65561 SV65561 ACR65561 AMN65561 AWJ65561 BGF65561 BQB65561 BZX65561 CJT65561 CTP65561 DDL65561 DNH65561 DXD65561 EGZ65561 EQV65561 FAR65561 FKN65561 FUJ65561 GEF65561 GOB65561 GXX65561 HHT65561 HRP65561 IBL65561 ILH65561 IVD65561 JEZ65561 JOV65561 JYR65561 KIN65561 KSJ65561 LCF65561 LMB65561 LVX65561 MFT65561 MPP65561 MZL65561 NJH65561 NTD65561 OCZ65561 OMV65561 OWR65561 PGN65561 PQJ65561 QAF65561 QKB65561 QTX65561 RDT65561 RNP65561 RXL65561 SHH65561 SRD65561 TAZ65561 TKV65561 TUR65561 UEN65561 UOJ65561 UYF65561 VIB65561 VRX65561 WBT65561 WLP65561 WVL65561 D131097 IZ131097 SV131097 ACR131097 AMN131097 AWJ131097 BGF131097 BQB131097 BZX131097 CJT131097 CTP131097 DDL131097 DNH131097 DXD131097 EGZ131097 EQV131097 FAR131097 FKN131097 FUJ131097 GEF131097 GOB131097 GXX131097 HHT131097 HRP131097 IBL131097 ILH131097 IVD131097 JEZ131097 JOV131097 JYR131097 KIN131097 KSJ131097 LCF131097 LMB131097 LVX131097 MFT131097 MPP131097 MZL131097 NJH131097 NTD131097 OCZ131097 OMV131097 OWR131097 PGN131097 PQJ131097 QAF131097 QKB131097 QTX131097 RDT131097 RNP131097 RXL131097 SHH131097 SRD131097 TAZ131097 TKV131097 TUR131097 UEN131097 UOJ131097 UYF131097 VIB131097 VRX131097 WBT131097 WLP131097 WVL131097 D196633 IZ196633 SV196633 ACR196633 AMN196633 AWJ196633 BGF196633 BQB196633 BZX196633 CJT196633 CTP196633 DDL196633 DNH196633 DXD196633 EGZ196633 EQV196633 FAR196633 FKN196633 FUJ196633 GEF196633 GOB196633 GXX196633 HHT196633 HRP196633 IBL196633 ILH196633 IVD196633 JEZ196633 JOV196633 JYR196633 KIN196633 KSJ196633 LCF196633 LMB196633 LVX196633 MFT196633 MPP196633 MZL196633 NJH196633 NTD196633 OCZ196633 OMV196633 OWR196633 PGN196633 PQJ196633 QAF196633 QKB196633 QTX196633 RDT196633 RNP196633 RXL196633 SHH196633 SRD196633 TAZ196633 TKV196633 TUR196633 UEN196633 UOJ196633 UYF196633 VIB196633 VRX196633 WBT196633 WLP196633 WVL196633 D262169 IZ262169 SV262169 ACR262169 AMN262169 AWJ262169 BGF262169 BQB262169 BZX262169 CJT262169 CTP262169 DDL262169 DNH262169 DXD262169 EGZ262169 EQV262169 FAR262169 FKN262169 FUJ262169 GEF262169 GOB262169 GXX262169 HHT262169 HRP262169 IBL262169 ILH262169 IVD262169 JEZ262169 JOV262169 JYR262169 KIN262169 KSJ262169 LCF262169 LMB262169 LVX262169 MFT262169 MPP262169 MZL262169 NJH262169 NTD262169 OCZ262169 OMV262169 OWR262169 PGN262169 PQJ262169 QAF262169 QKB262169 QTX262169 RDT262169 RNP262169 RXL262169 SHH262169 SRD262169 TAZ262169 TKV262169 TUR262169 UEN262169 UOJ262169 UYF262169 VIB262169 VRX262169 WBT262169 WLP262169 WVL262169 D327705 IZ327705 SV327705 ACR327705 AMN327705 AWJ327705 BGF327705 BQB327705 BZX327705 CJT327705 CTP327705 DDL327705 DNH327705 DXD327705 EGZ327705 EQV327705 FAR327705 FKN327705 FUJ327705 GEF327705 GOB327705 GXX327705 HHT327705 HRP327705 IBL327705 ILH327705 IVD327705 JEZ327705 JOV327705 JYR327705 KIN327705 KSJ327705 LCF327705 LMB327705 LVX327705 MFT327705 MPP327705 MZL327705 NJH327705 NTD327705 OCZ327705 OMV327705 OWR327705 PGN327705 PQJ327705 QAF327705 QKB327705 QTX327705 RDT327705 RNP327705 RXL327705 SHH327705 SRD327705 TAZ327705 TKV327705 TUR327705 UEN327705 UOJ327705 UYF327705 VIB327705 VRX327705 WBT327705 WLP327705 WVL327705 D393241 IZ393241 SV393241 ACR393241 AMN393241 AWJ393241 BGF393241 BQB393241 BZX393241 CJT393241 CTP393241 DDL393241 DNH393241 DXD393241 EGZ393241 EQV393241 FAR393241 FKN393241 FUJ393241 GEF393241 GOB393241 GXX393241 HHT393241 HRP393241 IBL393241 ILH393241 IVD393241 JEZ393241 JOV393241 JYR393241 KIN393241 KSJ393241 LCF393241 LMB393241 LVX393241 MFT393241 MPP393241 MZL393241 NJH393241 NTD393241 OCZ393241 OMV393241 OWR393241 PGN393241 PQJ393241 QAF393241 QKB393241 QTX393241 RDT393241 RNP393241 RXL393241 SHH393241 SRD393241 TAZ393241 TKV393241 TUR393241 UEN393241 UOJ393241 UYF393241 VIB393241 VRX393241 WBT393241 WLP393241 WVL393241 D458777 IZ458777 SV458777 ACR458777 AMN458777 AWJ458777 BGF458777 BQB458777 BZX458777 CJT458777 CTP458777 DDL458777 DNH458777 DXD458777 EGZ458777 EQV458777 FAR458777 FKN458777 FUJ458777 GEF458777 GOB458777 GXX458777 HHT458777 HRP458777 IBL458777 ILH458777 IVD458777 JEZ458777 JOV458777 JYR458777 KIN458777 KSJ458777 LCF458777 LMB458777 LVX458777 MFT458777 MPP458777 MZL458777 NJH458777 NTD458777 OCZ458777 OMV458777 OWR458777 PGN458777 PQJ458777 QAF458777 QKB458777 QTX458777 RDT458777 RNP458777 RXL458777 SHH458777 SRD458777 TAZ458777 TKV458777 TUR458777 UEN458777 UOJ458777 UYF458777 VIB458777 VRX458777 WBT458777 WLP458777 WVL458777 D524313 IZ524313 SV524313 ACR524313 AMN524313 AWJ524313 BGF524313 BQB524313 BZX524313 CJT524313 CTP524313 DDL524313 DNH524313 DXD524313 EGZ524313 EQV524313 FAR524313 FKN524313 FUJ524313 GEF524313 GOB524313 GXX524313 HHT524313 HRP524313 IBL524313 ILH524313 IVD524313 JEZ524313 JOV524313 JYR524313 KIN524313 KSJ524313 LCF524313 LMB524313 LVX524313 MFT524313 MPP524313 MZL524313 NJH524313 NTD524313 OCZ524313 OMV524313 OWR524313 PGN524313 PQJ524313 QAF524313 QKB524313 QTX524313 RDT524313 RNP524313 RXL524313 SHH524313 SRD524313 TAZ524313 TKV524313 TUR524313 UEN524313 UOJ524313 UYF524313 VIB524313 VRX524313 WBT524313 WLP524313 WVL524313 D589849 IZ589849 SV589849 ACR589849 AMN589849 AWJ589849 BGF589849 BQB589849 BZX589849 CJT589849 CTP589849 DDL589849 DNH589849 DXD589849 EGZ589849 EQV589849 FAR589849 FKN589849 FUJ589849 GEF589849 GOB589849 GXX589849 HHT589849 HRP589849 IBL589849 ILH589849 IVD589849 JEZ589849 JOV589849 JYR589849 KIN589849 KSJ589849 LCF589849 LMB589849 LVX589849 MFT589849 MPP589849 MZL589849 NJH589849 NTD589849 OCZ589849 OMV589849 OWR589849 PGN589849 PQJ589849 QAF589849 QKB589849 QTX589849 RDT589849 RNP589849 RXL589849 SHH589849 SRD589849 TAZ589849 TKV589849 TUR589849 UEN589849 UOJ589849 UYF589849 VIB589849 VRX589849 WBT589849 WLP589849 WVL589849 D655385 IZ655385 SV655385 ACR655385 AMN655385 AWJ655385 BGF655385 BQB655385 BZX655385 CJT655385 CTP655385 DDL655385 DNH655385 DXD655385 EGZ655385 EQV655385 FAR655385 FKN655385 FUJ655385 GEF655385 GOB655385 GXX655385 HHT655385 HRP655385 IBL655385 ILH655385 IVD655385 JEZ655385 JOV655385 JYR655385 KIN655385 KSJ655385 LCF655385 LMB655385 LVX655385 MFT655385 MPP655385 MZL655385 NJH655385 NTD655385 OCZ655385 OMV655385 OWR655385 PGN655385 PQJ655385 QAF655385 QKB655385 QTX655385 RDT655385 RNP655385 RXL655385 SHH655385 SRD655385 TAZ655385 TKV655385 TUR655385 UEN655385 UOJ655385 UYF655385 VIB655385 VRX655385 WBT655385 WLP655385 WVL655385 D720921 IZ720921 SV720921 ACR720921 AMN720921 AWJ720921 BGF720921 BQB720921 BZX720921 CJT720921 CTP720921 DDL720921 DNH720921 DXD720921 EGZ720921 EQV720921 FAR720921 FKN720921 FUJ720921 GEF720921 GOB720921 GXX720921 HHT720921 HRP720921 IBL720921 ILH720921 IVD720921 JEZ720921 JOV720921 JYR720921 KIN720921 KSJ720921 LCF720921 LMB720921 LVX720921 MFT720921 MPP720921 MZL720921 NJH720921 NTD720921 OCZ720921 OMV720921 OWR720921 PGN720921 PQJ720921 QAF720921 QKB720921 QTX720921 RDT720921 RNP720921 RXL720921 SHH720921 SRD720921 TAZ720921 TKV720921 TUR720921 UEN720921 UOJ720921 UYF720921 VIB720921 VRX720921 WBT720921 WLP720921 WVL720921 D786457 IZ786457 SV786457 ACR786457 AMN786457 AWJ786457 BGF786457 BQB786457 BZX786457 CJT786457 CTP786457 DDL786457 DNH786457 DXD786457 EGZ786457 EQV786457 FAR786457 FKN786457 FUJ786457 GEF786457 GOB786457 GXX786457 HHT786457 HRP786457 IBL786457 ILH786457 IVD786457 JEZ786457 JOV786457 JYR786457 KIN786457 KSJ786457 LCF786457 LMB786457 LVX786457 MFT786457 MPP786457 MZL786457 NJH786457 NTD786457 OCZ786457 OMV786457 OWR786457 PGN786457 PQJ786457 QAF786457 QKB786457 QTX786457 RDT786457 RNP786457 RXL786457 SHH786457 SRD786457 TAZ786457 TKV786457 TUR786457 UEN786457 UOJ786457 UYF786457 VIB786457 VRX786457 WBT786457 WLP786457 WVL786457 D851993 IZ851993 SV851993 ACR851993 AMN851993 AWJ851993 BGF851993 BQB851993 BZX851993 CJT851993 CTP851993 DDL851993 DNH851993 DXD851993 EGZ851993 EQV851993 FAR851993 FKN851993 FUJ851993 GEF851993 GOB851993 GXX851993 HHT851993 HRP851993 IBL851993 ILH851993 IVD851993 JEZ851993 JOV851993 JYR851993 KIN851993 KSJ851993 LCF851993 LMB851993 LVX851993 MFT851993 MPP851993 MZL851993 NJH851993 NTD851993 OCZ851993 OMV851993 OWR851993 PGN851993 PQJ851993 QAF851993 QKB851993 QTX851993 RDT851993 RNP851993 RXL851993 SHH851993 SRD851993 TAZ851993 TKV851993 TUR851993 UEN851993 UOJ851993 UYF851993 VIB851993 VRX851993 WBT851993 WLP851993 WVL851993 D917529 IZ917529 SV917529 ACR917529 AMN917529 AWJ917529 BGF917529 BQB917529 BZX917529 CJT917529 CTP917529 DDL917529 DNH917529 DXD917529 EGZ917529 EQV917529 FAR917529 FKN917529 FUJ917529 GEF917529 GOB917529 GXX917529 HHT917529 HRP917529 IBL917529 ILH917529 IVD917529 JEZ917529 JOV917529 JYR917529 KIN917529 KSJ917529 LCF917529 LMB917529 LVX917529 MFT917529 MPP917529 MZL917529 NJH917529 NTD917529 OCZ917529 OMV917529 OWR917529 PGN917529 PQJ917529 QAF917529 QKB917529 QTX917529 RDT917529 RNP917529 RXL917529 SHH917529 SRD917529 TAZ917529 TKV917529 TUR917529 UEN917529 UOJ917529 UYF917529 VIB917529 VRX917529 WBT917529 WLP917529 WVL917529 D983065 IZ983065 SV983065 ACR983065 AMN983065 AWJ983065 BGF983065 BQB983065 BZX983065 CJT983065 CTP983065 DDL983065 DNH983065 DXD983065 EGZ983065 EQV983065 FAR983065 FKN983065 FUJ983065 GEF983065 GOB983065 GXX983065 HHT983065 HRP983065 IBL983065 ILH983065 IVD983065 JEZ983065 JOV983065 JYR983065 KIN983065 KSJ983065 LCF983065 LMB983065 LVX983065 MFT983065 MPP983065 MZL983065 NJH983065 NTD983065 OCZ983065 OMV983065 OWR983065 PGN983065 PQJ983065 QAF983065 QKB983065 QTX983065 RDT983065 RNP983065 RXL983065 SHH983065 SRD983065 TAZ983065 TKV983065 TUR983065 UEN983065 UOJ983065 UYF983065 VIB983065 VRX983065 WBT983065 WLP983065 WVL983065">
@@ -5537,7 +5550,7 @@
   <dimension ref="A1:N169"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5679,9 +5692,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_SND</v>
       </c>
-      <c r="F4" s="33" t="e">
+      <c r="F4" s="33">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.8940000000000001E-3</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="32" t="b">
@@ -5718,9 +5731,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_SWD</v>
       </c>
-      <c r="F5" s="33" t="e">
+      <c r="F5" s="33">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.9819999999999998E-3</v>
       </c>
       <c r="G5" s="33"/>
       <c r="H5" s="32" t="b">
@@ -5757,9 +5770,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_2WD</v>
       </c>
-      <c r="F6" s="33" t="e">
+      <c r="F6" s="33">
         <f>_xll.qlRateHelperQuoteValue($E6,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.977E-3</v>
       </c>
       <c r="G6" s="33"/>
       <c r="H6" s="32" t="b">
@@ -5796,9 +5809,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_3WD</v>
       </c>
-      <c r="F7" s="33" t="e">
+      <c r="F7" s="33">
         <f>_xll.qlRateHelperQuoteValue($E7,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.9919999999999998E-3</v>
       </c>
       <c r="G7" s="33"/>
       <c r="H7" s="32" t="b">
@@ -5835,9 +5848,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_1MD</v>
       </c>
-      <c r="F8" s="33" t="e">
+      <c r="F8" s="33">
         <f>_xll.qlRateHelperQuoteValue($E8,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.013E-3</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="32" t="b">
@@ -5874,9 +5887,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_2MD</v>
       </c>
-      <c r="F9" s="33" t="e">
+      <c r="F9" s="33">
         <f>_xll.qlRateHelperQuoteValue($E9,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.1280000000000001E-3</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="32" t="b">
@@ -5907,9 +5920,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_3MD</v>
       </c>
-      <c r="F10" s="33" t="e">
+      <c r="F10" s="33">
         <f>_xll.qlRateHelperQuoteValue($E10,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.2360000000000001E-3</v>
       </c>
       <c r="G10" s="33"/>
       <c r="H10" s="32" t="b">
@@ -6113,9 +6126,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_T3F1</v>
       </c>
-      <c r="F16" s="41" t="e">
+      <c r="F16" s="41">
         <f>_xll.qlRateHelperQuoteValue($E16,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.2500000000000003E-3</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="40" t="b">
@@ -6151,9 +6164,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_TOM3F1</v>
       </c>
-      <c r="F17" s="26" t="e">
+      <c r="F17" s="26">
         <f>_xll.qlRateHelperQuoteValue($E17,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.2500000000000003E-3</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="25" t="b">
@@ -6189,9 +6202,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_1x4F</v>
       </c>
-      <c r="F18" s="33" t="e">
+      <c r="F18" s="33">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.4499999999999999E-3</v>
       </c>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="b">
@@ -6227,9 +6240,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_2x5F</v>
       </c>
-      <c r="F19" s="33" t="e">
+      <c r="F19" s="33">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.6800000000000001E-3</v>
       </c>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="b">
@@ -6265,9 +6278,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_3x6F</v>
       </c>
-      <c r="F20" s="33" t="e">
+      <c r="F20" s="33">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.9400000000000003E-3</v>
       </c>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="b">
@@ -6303,9 +6316,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_4x7F</v>
       </c>
-      <c r="F21" s="33" t="e">
+      <c r="F21" s="33">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.1099999999999999E-3</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="b">
@@ -6341,9 +6354,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_5x8F</v>
       </c>
-      <c r="F22" s="33" t="e">
+      <c r="F22" s="33">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.3199999999999996E-3</v>
       </c>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="b">
@@ -6379,9 +6392,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YC3MRH_6x9F</v>
       </c>
-      <c r="F23" s="33" t="e">
+      <c r="F23" s="33">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.5199999999999997E-3</v>
       </c>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="b">
@@ -6744,7 +6757,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B33" s="36">
         <v>16</v>
       </c>
@@ -6782,7 +6795,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B34" s="36">
         <v>17</v>
       </c>
@@ -6820,7 +6833,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B35" s="29">
         <v>18</v>
       </c>
@@ -6858,7 +6871,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="43" t="b">
         <v>0</v>
       </c>
@@ -6901,7 +6914,7 @@
         <v>41744</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="b">
         <v>0</v>
       </c>
@@ -6943,7 +6956,7 @@
         <v>41778</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="35" t="b">
         <v>0</v>
       </c>
@@ -6985,7 +6998,7 @@
         <v>41809</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="35" t="b">
         <v>0</v>
       </c>
@@ -7009,8 +7022,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E39,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H39" s="32" t="b">
-        <v>1</v>
+      <c r="H39" s="228" t="b">
+        <v>0</v>
       </c>
       <c r="I39" s="32">
         <v>60</v>
@@ -7026,8 +7039,11 @@
         <f>_xll.qlRateHelperLatestDate($E39,Trigger)</f>
         <v>41836</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N39" s="229" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="b">
         <v>0</v>
       </c>
@@ -7069,7 +7085,7 @@
         <v>41872</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="b">
         <v>0</v>
       </c>
@@ -7093,8 +7109,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E41,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H41" s="32" t="b">
-        <v>1</v>
+      <c r="H41" s="228" t="b">
+        <v>0</v>
       </c>
       <c r="I41" s="32">
         <v>60</v>
@@ -7111,7 +7127,7 @@
         <v>41900</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="35" t="b">
         <v>0</v>
       </c>
@@ -7135,8 +7151,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E42,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H42" s="32" t="b">
-        <v>1</v>
+      <c r="H42" s="228" t="b">
+        <v>0</v>
       </c>
       <c r="I42" s="32">
         <v>60</v>
@@ -7153,7 +7169,7 @@
         <v>41928</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="35" t="b">
         <v>0</v>
       </c>
@@ -7195,7 +7211,7 @@
         <v>41963</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="b">
         <v>0</v>
       </c>
@@ -7219,8 +7235,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E44,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H44" s="32" t="b">
-        <v>1</v>
+      <c r="H44" s="228" t="b">
+        <v>0</v>
       </c>
       <c r="I44" s="32">
         <v>60</v>
@@ -7237,7 +7253,7 @@
         <v>41990</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="b">
         <v>0</v>
       </c>
@@ -7261,8 +7277,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E45,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H45" s="32" t="b">
-        <v>1</v>
+      <c r="H45" s="228" t="b">
+        <v>0</v>
       </c>
       <c r="I45" s="32">
         <v>60</v>
@@ -7279,7 +7295,7 @@
         <v>42019</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="b">
         <v>0</v>
       </c>
@@ -7321,7 +7337,7 @@
         <v>42054</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="b">
         <v>0</v>
       </c>
@@ -7345,8 +7361,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E47,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H47" s="32" t="b">
-        <v>1</v>
+      <c r="H47" s="228" t="b">
+        <v>0</v>
       </c>
       <c r="I47" s="32">
         <v>60</v>
@@ -7363,7 +7379,7 @@
         <v>42080</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="b">
         <v>1</v>
       </c>
@@ -12582,7 +12598,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -12635,9 +12651,9 @@
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
         <v>EUR_YC3MRH_2WD</v>
       </c>
-      <c r="E2" s="10" t="e">
+      <c r="E2" s="10">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>#NUM!</v>
+        <v>1.977E-3</v>
       </c>
       <c r="F2" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -12671,9 +12687,9 @@
       <c r="D3" s="11" t="str">
         <v>EUR_YC3MRH_3WD</v>
       </c>
-      <c r="E3" s="10" t="e">
+      <c r="E3" s="10">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>#NUM!</v>
+        <v>1.9919999999999998E-3</v>
       </c>
       <c r="F3" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -12707,9 +12723,9 @@
       <c r="D4" s="11" t="str">
         <v>EUR_YC3MRH_1MD</v>
       </c>
-      <c r="E4" s="10" t="e">
+      <c r="E4" s="10">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>#NUM!</v>
+        <v>2.013E-3</v>
       </c>
       <c r="F4" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -12743,9 +12759,9 @@
       <c r="D5" s="11" t="str">
         <v>EUR_YC3MRH_2MD</v>
       </c>
-      <c r="E5" s="10" t="e">
+      <c r="E5" s="10">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>#NUM!</v>
+        <v>2.1280000000000001E-3</v>
       </c>
       <c r="F5" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -12780,9 +12796,9 @@
       <c r="D6" s="11" t="str">
         <v>EUR_YC3MRH_TOM3F1</v>
       </c>
-      <c r="E6" s="10" t="e">
+      <c r="E6" s="10">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>#NUM!</v>
+        <v>2.2500000000000003E-3</v>
       </c>
       <c r="F6" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -12809,7 +12825,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="str">
         <f>_xll.ohGroup(,_xll.ohPack(D2:D126),Permanent,,ObjectOverwrite)</f>
-        <v>obj_0065a#0000</v>
+        <v>obj_0065a#0008</v>
       </c>
       <c r="B7" s="12" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -12846,28 +12862,28 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MM4</v>
-      </c>
-      <c r="E8" s="10" t="e">
+        <v>EUR_YC3MRH_FUT3MH5</v>
+      </c>
+      <c r="E8" s="10">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F8" s="10" t="str">
+        <v>5.1250000000000462E-3</v>
+      </c>
+      <c r="F8" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="G8" s="9">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41808</v>
+        <v>42081</v>
       </c>
       <c r="H8" s="8">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41900</v>
+        <v>42173</v>
       </c>
       <c r="I8" s="3" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="229" t="s">
         <v>122</v>
       </c>
       <c r="L8" s="46">
@@ -12876,28 +12892,28 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MU4</v>
-      </c>
-      <c r="E9" s="10" t="e">
+        <v>EUR_YC3MRH_FUT3MM5</v>
+      </c>
+      <c r="E9" s="10">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F9" s="10" t="str">
+        <v>5.8249999999999691E-3</v>
+      </c>
+      <c r="F9" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="G9" s="9">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41899</v>
+        <v>42172</v>
       </c>
       <c r="H9" s="8">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41990</v>
+        <v>42264</v>
       </c>
       <c r="I9" s="3" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="229" t="s">
         <v>123</v>
       </c>
       <c r="L9" s="46">
@@ -12906,28 +12922,28 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D10" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MZ4</v>
-      </c>
-      <c r="E10" s="10" t="e">
+        <v>EUR_YC3MRH_FUT3MU5</v>
+      </c>
+      <c r="E10" s="10">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F10" s="10" t="str">
+        <v>6.525000000000003E-3</v>
+      </c>
+      <c r="F10" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="G10" s="9">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41990</v>
+        <v>42263</v>
       </c>
       <c r="H10" s="8">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42080</v>
+        <v>42354</v>
       </c>
       <c r="I10" s="3" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="229" t="s">
         <v>124</v>
       </c>
       <c r="L10" s="46">
@@ -12936,11 +12952,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MH5</v>
+        <v>EUR_YC3MRH_FUT3MZ5</v>
       </c>
       <c r="E11" s="10">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>5.1250000000000462E-3</v>
+        <v>7.3250000000000259E-3</v>
       </c>
       <c r="F11" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -12948,11 +12964,11 @@
       </c>
       <c r="G11" s="9">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42081</v>
+        <v>42354</v>
       </c>
       <c r="H11" s="8">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42173</v>
+        <v>42445</v>
       </c>
       <c r="I11" s="3" t="e">
         <v>#NUM!</v>
@@ -12966,11 +12982,11 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MM5</v>
+        <v>EUR_YC3MRH_FUT3MH6</v>
       </c>
       <c r="E12" s="10">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>5.8249999999999691E-3</v>
+        <v>8.1749999999999323E-3</v>
       </c>
       <c r="F12" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -12978,11 +12994,11 @@
       </c>
       <c r="G12" s="9">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42172</v>
+        <v>42445</v>
       </c>
       <c r="H12" s="8">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42264</v>
+        <v>42537</v>
       </c>
       <c r="I12" s="3" t="e">
         <v>#NUM!</v>
@@ -12996,11 +13012,11 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D13" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MU5</v>
+        <v>EUR_YC3MRH_FUT3MM6</v>
       </c>
       <c r="E13" s="10">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>6.525000000000003E-3</v>
+        <v>9.2500000000000915E-3</v>
       </c>
       <c r="F13" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -13008,11 +13024,11 @@
       </c>
       <c r="G13" s="9">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42263</v>
+        <v>42536</v>
       </c>
       <c r="H13" s="8">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42354</v>
+        <v>42628</v>
       </c>
       <c r="I13" s="3" t="e">
         <v>#NUM!</v>
@@ -13026,11 +13042,11 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D14" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MZ5</v>
-      </c>
-      <c r="E14" s="10">
+        <v>EUR_YC3MRH_AB3E3Y</v>
+      </c>
+      <c r="E14" s="10" t="e">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>7.3250000000000259E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F14" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -13038,11 +13054,11 @@
       </c>
       <c r="G14" s="9">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>42354</v>
+        <v>41648</v>
       </c>
       <c r="H14" s="8">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42445</v>
+        <v>42744</v>
       </c>
       <c r="I14" s="3" t="e">
         <v>#NUM!</v>
@@ -13056,7 +13072,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E3Y</v>
+        <v>EUR_YC3MRH_AB3E4Y</v>
       </c>
       <c r="E15" s="10" t="e">
         <f>_xll.qlRateHelperRate($D15)</f>
@@ -13072,7 +13088,7 @@
       </c>
       <c r="H15" s="8">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42744</v>
+        <v>43109</v>
       </c>
       <c r="I15" s="3" t="e">
         <v>#NUM!</v>
@@ -13086,7 +13102,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E4Y</v>
+        <v>EUR_YC3MRH_AB3E5Y</v>
       </c>
       <c r="E16" s="10" t="e">
         <f>_xll.qlRateHelperRate($D16)</f>
@@ -13102,7 +13118,7 @@
       </c>
       <c r="H16" s="8">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>43109</v>
+        <v>43474</v>
       </c>
       <c r="I16" s="3" t="e">
         <v>#NUM!</v>
@@ -13116,7 +13132,7 @@
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D17" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E5Y</v>
+        <v>EUR_YC3MRH_AB3E6Y</v>
       </c>
       <c r="E17" s="10" t="e">
         <f>_xll.qlRateHelperRate($D17)</f>
@@ -13132,7 +13148,7 @@
       </c>
       <c r="H17" s="8">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>43474</v>
+        <v>43839</v>
       </c>
       <c r="I17" s="3" t="e">
         <v>#NUM!</v>
@@ -13146,7 +13162,7 @@
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D18" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E6Y</v>
+        <v>EUR_YC3MRH_AB3E7Y</v>
       </c>
       <c r="E18" s="10" t="e">
         <f>_xll.qlRateHelperRate($D18)</f>
@@ -13162,7 +13178,7 @@
       </c>
       <c r="H18" s="8">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>43839</v>
+        <v>44207</v>
       </c>
       <c r="I18" s="3" t="e">
         <v>#NUM!</v>
@@ -13176,7 +13192,7 @@
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D19" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E7Y</v>
+        <v>EUR_YC3MRH_AB3E8Y</v>
       </c>
       <c r="E19" s="10" t="e">
         <f>_xll.qlRateHelperRate($D19)</f>
@@ -13192,7 +13208,7 @@
       </c>
       <c r="H19" s="8">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>44207</v>
+        <v>44571</v>
       </c>
       <c r="I19" s="3" t="e">
         <v>#NUM!</v>
@@ -13206,7 +13222,7 @@
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D20" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E8Y</v>
+        <v>EUR_YC3MRH_AB3E9Y</v>
       </c>
       <c r="E20" s="10" t="e">
         <f>_xll.qlRateHelperRate($D20)</f>
@@ -13222,7 +13238,7 @@
       </c>
       <c r="H20" s="8">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>44571</v>
+        <v>44935</v>
       </c>
       <c r="I20" s="3" t="e">
         <v>#NUM!</v>
@@ -13236,7 +13252,7 @@
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D21" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E9Y</v>
+        <v>EUR_YC3MRH_AB3E10Y</v>
       </c>
       <c r="E21" s="10" t="e">
         <f>_xll.qlRateHelperRate($D21)</f>
@@ -13252,7 +13268,7 @@
       </c>
       <c r="H21" s="8">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>44935</v>
+        <v>45300</v>
       </c>
       <c r="I21" s="3" t="e">
         <v>#NUM!</v>
@@ -13266,7 +13282,7 @@
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D22" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E10Y</v>
+        <v>EUR_YC3MRH_AB3E12Y</v>
       </c>
       <c r="E22" s="10" t="e">
         <f>_xll.qlRateHelperRate($D22)</f>
@@ -13282,7 +13298,7 @@
       </c>
       <c r="H22" s="8">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>45300</v>
+        <v>46031</v>
       </c>
       <c r="I22" s="3" t="e">
         <v>#NUM!</v>
@@ -13296,7 +13312,7 @@
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D23" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E12Y</v>
+        <v>EUR_YC3MRH_AB3E15Y</v>
       </c>
       <c r="E23" s="10" t="e">
         <f>_xll.qlRateHelperRate($D23)</f>
@@ -13312,7 +13328,7 @@
       </c>
       <c r="H23" s="8">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>46031</v>
+        <v>47127</v>
       </c>
       <c r="I23" s="3" t="e">
         <v>#NUM!</v>
@@ -13326,7 +13342,7 @@
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D24" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E15Y</v>
+        <v>EUR_YC3MRH_AB3E20Y</v>
       </c>
       <c r="E24" s="10" t="e">
         <f>_xll.qlRateHelperRate($D24)</f>
@@ -13342,7 +13358,7 @@
       </c>
       <c r="H24" s="8">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>47127</v>
+        <v>48953</v>
       </c>
       <c r="I24" s="3" t="e">
         <v>#NUM!</v>
@@ -13356,7 +13372,7 @@
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D25" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E20Y</v>
+        <v>EUR_YC3MRH_AB3E25Y</v>
       </c>
       <c r="E25" s="10" t="e">
         <f>_xll.qlRateHelperRate($D25)</f>
@@ -13372,7 +13388,7 @@
       </c>
       <c r="H25" s="8">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>48953</v>
+        <v>50780</v>
       </c>
       <c r="I25" s="3" t="e">
         <v>#NUM!</v>
@@ -13386,7 +13402,7 @@
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D26" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E25Y</v>
+        <v>EUR_YC3MRH_AB3E30Y</v>
       </c>
       <c r="E26" s="10" t="e">
         <f>_xll.qlRateHelperRate($D26)</f>
@@ -13402,7 +13418,7 @@
       </c>
       <c r="H26" s="8">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>50780</v>
+        <v>52607</v>
       </c>
       <c r="I26" s="3" t="e">
         <v>#NUM!</v>
@@ -13416,11 +13432,11 @@
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D27" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E30Y</v>
-      </c>
-      <c r="E27" s="10" t="e">
+        <v>EUR_YC3MRH_AB3EBASIS35Y</v>
+      </c>
+      <c r="E27" s="10">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>#NUM!</v>
+        <v>2.4505000000000002E-2</v>
       </c>
       <c r="F27" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -13432,7 +13448,7 @@
       </c>
       <c r="H27" s="8">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>52607</v>
+        <v>54434</v>
       </c>
       <c r="I27" s="3" t="e">
         <v>#NUM!</v>
@@ -13446,11 +13462,11 @@
     </row>
     <row r="28" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D28" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS35Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS40Y</v>
       </c>
       <c r="E28" s="10">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.4505000000000002E-2</v>
+        <v>2.4820000000000002E-2</v>
       </c>
       <c r="F28" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -13462,7 +13478,7 @@
       </c>
       <c r="H28" s="8">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>54434</v>
+        <v>56258</v>
       </c>
       <c r="I28" s="3" t="e">
         <v>#NUM!</v>
@@ -13476,11 +13492,11 @@
     </row>
     <row r="29" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D29" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS40Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS50Y</v>
       </c>
       <c r="E29" s="10">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.4820000000000002E-2</v>
+        <v>2.5305000000000001E-2</v>
       </c>
       <c r="F29" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -13492,7 +13508,7 @@
       </c>
       <c r="H29" s="8">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>56258</v>
+        <v>59910</v>
       </c>
       <c r="I29" s="3" t="e">
         <v>#NUM!</v>
@@ -13506,11 +13522,11 @@
     </row>
     <row r="30" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D30" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS50Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS60Y</v>
       </c>
       <c r="E30" s="10">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.5305000000000001E-2</v>
+        <v>2.564E-2</v>
       </c>
       <c r="F30" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -13522,7 +13538,7 @@
       </c>
       <c r="H30" s="8">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>59910</v>
+        <v>63563</v>
       </c>
       <c r="I30" s="3" t="e">
         <v>#NUM!</v>
@@ -13535,24 +13551,24 @@
       </c>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D31" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS60Y</v>
-      </c>
-      <c r="E31" s="10">
+      <c r="D31" s="11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E31" s="10" t="e">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.564E-2</v>
-      </c>
-      <c r="F31" s="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F31" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="9">
+        <v>--</v>
+      </c>
+      <c r="G31" s="9" t="e">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41648</v>
-      </c>
-      <c r="H31" s="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H31" s="8" t="e">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>63563</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I31" s="3" t="e">
         <v>#NUM!</v>
@@ -15936,7 +15952,7 @@
       </c>
       <c r="F3" s="109" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_SND#0001</v>
+        <v>EUR_YC3MRH_SND#0002</v>
       </c>
       <c r="G3" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -15963,7 +15979,7 @@
       </c>
       <c r="F4" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_SWD#0001</v>
+        <v>EUR_YC3MRH_SWD#0002</v>
       </c>
       <c r="G4" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -15990,7 +16006,7 @@
       </c>
       <c r="F5" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2WD#0001</v>
+        <v>EUR_YC3MRH_2WD#0002</v>
       </c>
       <c r="G5" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -16017,7 +16033,7 @@
       </c>
       <c r="F6" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3WD#0001</v>
+        <v>EUR_YC3MRH_3WD#0002</v>
       </c>
       <c r="G6" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -16044,7 +16060,7 @@
       </c>
       <c r="F7" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1MD#0001</v>
+        <v>EUR_YC3MRH_1MD#0002</v>
       </c>
       <c r="G7" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -16071,7 +16087,7 @@
       </c>
       <c r="F8" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2MD#0001</v>
+        <v>EUR_YC3MRH_2MD#0002</v>
       </c>
       <c r="G8" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -16098,7 +16114,7 @@
       </c>
       <c r="F9" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3MD#0001</v>
+        <v>EUR_YC3MRH_3MD#0002</v>
       </c>
       <c r="G9" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -16217,7 +16233,7 @@
       </c>
       <c r="H3" s="152" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_T3F1#0001</v>
+        <v>EUR_YC3MRH_T3F1#0002</v>
       </c>
       <c r="I3" s="151" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -16251,7 +16267,7 @@
       </c>
       <c r="H4" s="144" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_TOM3F1#0001</v>
+        <v>EUR_YC3MRH_TOM3F1#0002</v>
       </c>
       <c r="I4" s="150" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -16286,7 +16302,7 @@
       </c>
       <c r="H5" s="147" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1x4F#0001</v>
+        <v>EUR_YC3MRH_1x4F#0002</v>
       </c>
       <c r="I5" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -16321,7 +16337,7 @@
       </c>
       <c r="H6" s="147" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2x5F#0001</v>
+        <v>EUR_YC3MRH_2x5F#0002</v>
       </c>
       <c r="I6" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -16356,7 +16372,7 @@
       </c>
       <c r="H7" s="147" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3x6F#0001</v>
+        <v>EUR_YC3MRH_3x6F#0002</v>
       </c>
       <c r="I7" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -16391,7 +16407,7 @@
       </c>
       <c r="H8" s="147" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_4x7F#0001</v>
+        <v>EUR_YC3MRH_4x7F#0002</v>
       </c>
       <c r="I8" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -16426,7 +16442,7 @@
       </c>
       <c r="H9" s="147" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_5x8F#0001</v>
+        <v>EUR_YC3MRH_5x8F#0002</v>
       </c>
       <c r="I9" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -16461,7 +16477,7 @@
       </c>
       <c r="H10" s="144" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_6x9F#0001</v>
+        <v>EUR_YC3MRH_6x9F#0002</v>
       </c>
       <c r="I10" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -16600,7 +16616,7 @@
       </c>
       <c r="I3" s="174" t="str">
         <f>_xll.qlFuturesRateHelper(H3,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MF4#0001</v>
+        <v>EUR_YC3MRH_FUT3MF4#0002</v>
       </c>
       <c r="J3" s="173" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -16638,7 +16654,7 @@
       </c>
       <c r="I4" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H4,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MG4#0001</v>
+        <v>EUR_YC3MRH_FUT3MG4#0002</v>
       </c>
       <c r="J4" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -16676,7 +16692,7 @@
       </c>
       <c r="I5" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H5,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH4#0001</v>
+        <v>EUR_YC3MRH_FUT3MH4#0002</v>
       </c>
       <c r="J5" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -16714,7 +16730,7 @@
       </c>
       <c r="I6" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H6,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MJ4#0001</v>
+        <v>EUR_YC3MRH_FUT3MJ4#0002</v>
       </c>
       <c r="J6" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -16752,7 +16768,7 @@
       </c>
       <c r="I7" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H7,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MK4#0001</v>
+        <v>EUR_YC3MRH_FUT3MK4#0002</v>
       </c>
       <c r="J7" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -16790,7 +16806,7 @@
       </c>
       <c r="I8" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H8,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM4#0001</v>
+        <v>EUR_YC3MRH_FUT3MM4#0002</v>
       </c>
       <c r="J8" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -16828,7 +16844,7 @@
       </c>
       <c r="I9" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H9,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MN4#0001</v>
+        <v>EUR_YC3MRH_FUT3MN4#0002</v>
       </c>
       <c r="J9" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -16866,7 +16882,7 @@
       </c>
       <c r="I10" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H10,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MQ4#0001</v>
+        <v>EUR_YC3MRH_FUT3MQ4#0002</v>
       </c>
       <c r="J10" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -16904,7 +16920,7 @@
       </c>
       <c r="I11" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H11,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU4#0001</v>
+        <v>EUR_YC3MRH_FUT3MU4#0002</v>
       </c>
       <c r="J11" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -16942,7 +16958,7 @@
       </c>
       <c r="I12" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H12,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MV4#0001</v>
+        <v>EUR_YC3MRH_FUT3MV4#0002</v>
       </c>
       <c r="J12" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -16980,7 +16996,7 @@
       </c>
       <c r="I13" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H13,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MX4#0001</v>
+        <v>EUR_YC3MRH_FUT3MX4#0002</v>
       </c>
       <c r="J13" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -17018,7 +17034,7 @@
       </c>
       <c r="I14" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H14,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ4#0001</v>
+        <v>EUR_YC3MRH_FUT3MZ4#0002</v>
       </c>
       <c r="J14" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -17132,7 +17148,7 @@
       </c>
       <c r="I17" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H17,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH5#0001</v>
+        <v>EUR_YC3MRH_FUT3MH5#0002</v>
       </c>
       <c r="J17" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -17246,7 +17262,7 @@
       </c>
       <c r="I20" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H20,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM5#0001</v>
+        <v>EUR_YC3MRH_FUT3MM5#0002</v>
       </c>
       <c r="J20" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -17360,7 +17376,7 @@
       </c>
       <c r="I23" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H23,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU5#0001</v>
+        <v>EUR_YC3MRH_FUT3MU5#0002</v>
       </c>
       <c r="J23" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
@@ -17474,7 +17490,7 @@
       </c>
       <c r="I26" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H26,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ5#0001</v>
+        <v>EUR_YC3MRH_FUT3MZ5#0002</v>
       </c>
       <c r="J26" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
@@ -17588,7 +17604,7 @@
       </c>
       <c r="I29" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H29,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH6#0001</v>
+        <v>EUR_YC3MRH_FUT3MH6#0002</v>
       </c>
       <c r="J29" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
@@ -17702,7 +17718,7 @@
       </c>
       <c r="I32" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H32,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM6#0001</v>
+        <v>EUR_YC3MRH_FUT3MM6#0002</v>
       </c>
       <c r="J32" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
@@ -17816,7 +17832,7 @@
       </c>
       <c r="I35" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H35,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU6#0001</v>
+        <v>EUR_YC3MRH_FUT3MU6#0002</v>
       </c>
       <c r="J35" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
@@ -17930,7 +17946,7 @@
       </c>
       <c r="I38" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H38,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ6#0001</v>
+        <v>EUR_YC3MRH_FUT3MZ6#0002</v>
       </c>
       <c r="J38" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
@@ -18043,7 +18059,7 @@
       </c>
       <c r="I41" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H41,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH7#0001</v>
+        <v>EUR_YC3MRH_FUT3MH7#0002</v>
       </c>
       <c r="J41" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
@@ -18154,7 +18170,7 @@
       </c>
       <c r="I44" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H44,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM7#0001</v>
+        <v>EUR_YC3MRH_FUT3MM7#0002</v>
       </c>
       <c r="J44" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I44)</f>
@@ -18265,7 +18281,7 @@
       </c>
       <c r="I47" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H47,$F47,$D47,$E47,$G47,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU7#0001</v>
+        <v>EUR_YC3MRH_FUT3MU7#0002</v>
       </c>
       <c r="J47" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I47)</f>
@@ -18376,7 +18392,7 @@
       </c>
       <c r="I50" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H50,$F50,$D50,$E50,$G50,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ7#0001</v>
+        <v>EUR_YC3MRH_FUT3MZ7#0002</v>
       </c>
       <c r="J50" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I50)</f>
@@ -18487,7 +18503,7 @@
       </c>
       <c r="I53" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H53,$F53,$D53,$E53,$G53,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH8#0001</v>
+        <v>EUR_YC3MRH_FUT3MH8#0002</v>
       </c>
       <c r="J53" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I53)</f>
@@ -18598,7 +18614,7 @@
       </c>
       <c r="I56" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H56,$F56,$D56,$E56,$G56,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM8#0001</v>
+        <v>EUR_YC3MRH_FUT3MM8#0002</v>
       </c>
       <c r="J56" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I56)</f>
@@ -18709,7 +18725,7 @@
       </c>
       <c r="I59" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H59,$F59,$D59,$E59,$G59,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU8#0001</v>
+        <v>EUR_YC3MRH_FUT3MU8#0002</v>
       </c>
       <c r="J59" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I59)</f>
@@ -18820,7 +18836,7 @@
       </c>
       <c r="I62" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H62,$F62,$D62,$E62,$G62,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ8#0001</v>
+        <v>EUR_YC3MRH_FUT3MZ8#0002</v>
       </c>
       <c r="J62" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I62)</f>
@@ -18931,7 +18947,7 @@
       </c>
       <c r="I65" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H65,$F65,$D65,$E65,$G65,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH9#0001</v>
+        <v>EUR_YC3MRH_FUT3MH9#0002</v>
       </c>
       <c r="J65" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I65)</f>
@@ -19042,7 +19058,7 @@
       </c>
       <c r="I68" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H68,$F68,$D68,$E68,$G68,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM9#0001</v>
+        <v>EUR_YC3MRH_FUT3MM9#0002</v>
       </c>
       <c r="J68" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I68)</f>
@@ -19153,7 +19169,7 @@
       </c>
       <c r="I71" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H71,$F71,$D71,$E71,$G71,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU9#0001</v>
+        <v>EUR_YC3MRH_FUT3MU9#0002</v>
       </c>
       <c r="J71" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I71)</f>
@@ -19264,7 +19280,7 @@
       </c>
       <c r="I74" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H74,$F74,$D74,$E74,$G74,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ9#0001</v>
+        <v>EUR_YC3MRH_FUT3MZ9#0002</v>
       </c>
       <c r="J74" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I74)</f>
@@ -19375,7 +19391,7 @@
       </c>
       <c r="I77" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H77,$F77,$D77,$E77,$G77,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH0#0001</v>
+        <v>EUR_YC3MRH_FUT3MH0#0002</v>
       </c>
       <c r="J77" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I77)</f>
@@ -19486,7 +19502,7 @@
       </c>
       <c r="I80" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H80,$F80,$D80,$E80,$G80,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM0#0001</v>
+        <v>EUR_YC3MRH_FUT3MM0#0002</v>
       </c>
       <c r="J80" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I80)</f>
@@ -19597,7 +19613,7 @@
       </c>
       <c r="I83" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H83,$F83,$D83,$E83,$G83,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU0#0001</v>
+        <v>EUR_YC3MRH_FUT3MU0#0002</v>
       </c>
       <c r="J83" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I83)</f>
@@ -19708,7 +19724,7 @@
       </c>
       <c r="I86" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H86,$F86,$D86,$E86,$G86,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ0#0001</v>
+        <v>EUR_YC3MRH_FUT3MZ0#0002</v>
       </c>
       <c r="J86" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I86)</f>
@@ -19819,7 +19835,7 @@
       </c>
       <c r="I89" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H89,$F89,$D89,$E89,$G89,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH1#0001</v>
+        <v>EUR_YC3MRH_FUT3MH1#0002</v>
       </c>
       <c r="J89" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I89)</f>
@@ -19930,7 +19946,7 @@
       </c>
       <c r="I92" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H92,$F92,$D92,$E92,$G92,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM1#0001</v>
+        <v>EUR_YC3MRH_FUT3MM1#0002</v>
       </c>
       <c r="J92" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I92)</f>
@@ -20041,7 +20057,7 @@
       </c>
       <c r="I95" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H95,$F95,$D95,$E95,$G95,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU1#0001</v>
+        <v>EUR_YC3MRH_FUT3MU1#0002</v>
       </c>
       <c r="J95" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I95)</f>
@@ -20152,7 +20168,7 @@
       </c>
       <c r="I98" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H98,$F98,$D98,$E98,$G98,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ1#0001</v>
+        <v>EUR_YC3MRH_FUT3MZ1#0002</v>
       </c>
       <c r="J98" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I98)</f>
@@ -20263,7 +20279,7 @@
       </c>
       <c r="I101" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H101,$F101,$D101,$E101,$G101,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH2#0001</v>
+        <v>EUR_YC3MRH_FUT3MH2#0002</v>
       </c>
       <c r="J101" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I101)</f>
@@ -20374,7 +20390,7 @@
       </c>
       <c r="I104" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H104,$F104,$D104,$E104,$G104,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM2#0001</v>
+        <v>EUR_YC3MRH_FUT3MM2#0002</v>
       </c>
       <c r="J104" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I104)</f>
@@ -21194,7 +21210,7 @@
       </c>
       <c r="L4" s="204" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC3MRH_AB3E_ibor3M#0001</v>
+        <v>EUR_YC3MRH_AB3E_ibor3M#0002</v>
       </c>
       <c r="M4" s="203" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -21258,7 +21274,7 @@
       </c>
       <c r="L6" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E1Y#0001</v>
+        <v>EUR_YC3MRH_AB3E1Y#0002</v>
       </c>
       <c r="M6" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -21313,7 +21329,7 @@
       </c>
       <c r="L7" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E15M#0001</v>
+        <v>EUR_YC3MRH_AB3E15M#0002</v>
       </c>
       <c r="M7" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -21368,7 +21384,7 @@
       </c>
       <c r="L8" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E18M#0001</v>
+        <v>EUR_YC3MRH_AB3E18M#0002</v>
       </c>
       <c r="M8" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -21423,7 +21439,7 @@
       </c>
       <c r="L9" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E21M#0001</v>
+        <v>EUR_YC3MRH_AB3E21M#0002</v>
       </c>
       <c r="M9" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -21478,7 +21494,7 @@
       </c>
       <c r="L10" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E2Y#0001</v>
+        <v>EUR_YC3MRH_AB3E2Y#0002</v>
       </c>
       <c r="M10" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -21533,7 +21549,7 @@
       </c>
       <c r="L11" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E3Y#0001</v>
+        <v>EUR_YC3MRH_AB3E3Y#0002</v>
       </c>
       <c r="M11" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -21579,7 +21595,7 @@
       </c>
       <c r="L12" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E4Y#0001</v>
+        <v>EUR_YC3MRH_AB3E4Y#0002</v>
       </c>
       <c r="M12" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -21625,7 +21641,7 @@
       </c>
       <c r="L13" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E5Y#0001</v>
+        <v>EUR_YC3MRH_AB3E5Y#0002</v>
       </c>
       <c r="M13" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -21671,7 +21687,7 @@
       </c>
       <c r="L14" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E6Y#0001</v>
+        <v>EUR_YC3MRH_AB3E6Y#0002</v>
       </c>
       <c r="M14" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -21717,7 +21733,7 @@
       </c>
       <c r="L15" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E7Y#0001</v>
+        <v>EUR_YC3MRH_AB3E7Y#0002</v>
       </c>
       <c r="M15" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -21763,7 +21779,7 @@
       </c>
       <c r="L16" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E8Y#0001</v>
+        <v>EUR_YC3MRH_AB3E8Y#0002</v>
       </c>
       <c r="M16" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -21809,7 +21825,7 @@
       </c>
       <c r="L17" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E9Y#0001</v>
+        <v>EUR_YC3MRH_AB3E9Y#0002</v>
       </c>
       <c r="M17" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -21855,7 +21871,7 @@
       </c>
       <c r="L18" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E10Y#0001</v>
+        <v>EUR_YC3MRH_AB3E10Y#0002</v>
       </c>
       <c r="M18" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -21901,7 +21917,7 @@
       </c>
       <c r="L19" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E11Y#0001</v>
+        <v>EUR_YC3MRH_AB3E11Y#0002</v>
       </c>
       <c r="M19" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -21947,7 +21963,7 @@
       </c>
       <c r="L20" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E12Y#0001</v>
+        <v>EUR_YC3MRH_AB3E12Y#0002</v>
       </c>
       <c r="M20" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -21993,7 +22009,7 @@
       </c>
       <c r="L21" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E13Y#0001</v>
+        <v>EUR_YC3MRH_AB3E13Y#0002</v>
       </c>
       <c r="M21" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -22039,7 +22055,7 @@
       </c>
       <c r="L22" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E14Y#0001</v>
+        <v>EUR_YC3MRH_AB3E14Y#0002</v>
       </c>
       <c r="M22" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -22085,7 +22101,7 @@
       </c>
       <c r="L23" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E15Y#0001</v>
+        <v>EUR_YC3MRH_AB3E15Y#0002</v>
       </c>
       <c r="M23" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -22131,7 +22147,7 @@
       </c>
       <c r="L24" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E16Y#0001</v>
+        <v>EUR_YC3MRH_AB3E16Y#0002</v>
       </c>
       <c r="M24" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -22177,7 +22193,7 @@
       </c>
       <c r="L25" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E17Y#0001</v>
+        <v>EUR_YC3MRH_AB3E17Y#0002</v>
       </c>
       <c r="M25" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -22223,7 +22239,7 @@
       </c>
       <c r="L26" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E18Y#0001</v>
+        <v>EUR_YC3MRH_AB3E18Y#0002</v>
       </c>
       <c r="M26" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -22269,7 +22285,7 @@
       </c>
       <c r="L27" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E19Y#0001</v>
+        <v>EUR_YC3MRH_AB3E19Y#0002</v>
       </c>
       <c r="M27" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -22315,7 +22331,7 @@
       </c>
       <c r="L28" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E20Y#0001</v>
+        <v>EUR_YC3MRH_AB3E20Y#0002</v>
       </c>
       <c r="M28" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -22361,7 +22377,7 @@
       </c>
       <c r="L29" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E21Y#0001</v>
+        <v>EUR_YC3MRH_AB3E21Y#0002</v>
       </c>
       <c r="M29" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -22407,7 +22423,7 @@
       </c>
       <c r="L30" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E22Y#0001</v>
+        <v>EUR_YC3MRH_AB3E22Y#0002</v>
       </c>
       <c r="M30" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -22453,7 +22469,7 @@
       </c>
       <c r="L31" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E23Y#0001</v>
+        <v>EUR_YC3MRH_AB3E23Y#0002</v>
       </c>
       <c r="M31" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -22499,7 +22515,7 @@
       </c>
       <c r="L32" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E24Y#0001</v>
+        <v>EUR_YC3MRH_AB3E24Y#0002</v>
       </c>
       <c r="M32" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -22545,7 +22561,7 @@
       </c>
       <c r="L33" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E25Y#0001</v>
+        <v>EUR_YC3MRH_AB3E25Y#0002</v>
       </c>
       <c r="M33" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -22591,7 +22607,7 @@
       </c>
       <c r="L34" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E26Y#0001</v>
+        <v>EUR_YC3MRH_AB3E26Y#0002</v>
       </c>
       <c r="M34" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -22637,7 +22653,7 @@
       </c>
       <c r="L35" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E27Y#0001</v>
+        <v>EUR_YC3MRH_AB3E27Y#0002</v>
       </c>
       <c r="M35" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -22683,7 +22699,7 @@
       </c>
       <c r="L36" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E28Y#0001</v>
+        <v>EUR_YC3MRH_AB3E28Y#0002</v>
       </c>
       <c r="M36" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -22729,7 +22745,7 @@
       </c>
       <c r="L37" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E29Y#0001</v>
+        <v>EUR_YC3MRH_AB3E29Y#0002</v>
       </c>
       <c r="M37" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -22775,7 +22791,7 @@
       </c>
       <c r="L38" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E30Y#0001</v>
+        <v>EUR_YC3MRH_AB3E30Y#0002</v>
       </c>
       <c r="M38" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -22821,7 +22837,7 @@
       </c>
       <c r="L39" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E35Y#0001</v>
+        <v>EUR_YC3MRH_AB3E35Y#0002</v>
       </c>
       <c r="M39" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -22867,7 +22883,7 @@
       </c>
       <c r="L40" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E40Y#0001</v>
+        <v>EUR_YC3MRH_AB3E40Y#0002</v>
       </c>
       <c r="M40" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -22913,7 +22929,7 @@
       </c>
       <c r="L41" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E50Y#0001</v>
+        <v>EUR_YC3MRH_AB3E50Y#0002</v>
       </c>
       <c r="M41" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -22959,7 +22975,7 @@
       </c>
       <c r="L42" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E60Y#0001</v>
+        <v>EUR_YC3MRH_AB3E60Y#0002</v>
       </c>
       <c r="M42" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -23017,7 +23033,7 @@
       </c>
       <c r="L44" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S12#0001</v>
+        <v>EUR_YC3MRH_1S12#0002</v>
       </c>
       <c r="M44" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -23062,7 +23078,7 @@
       </c>
       <c r="L45" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2S12#0001</v>
+        <v>EUR_YC3MRH_2S12#0002</v>
       </c>
       <c r="M45" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -23107,7 +23123,7 @@
       </c>
       <c r="L46" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3S12#0001</v>
+        <v>EUR_YC3MRH_3S12#0002</v>
       </c>
       <c r="M46" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -23152,7 +23168,7 @@
       </c>
       <c r="L47" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_4S12#0001</v>
+        <v>EUR_YC3MRH_4S12#0002</v>
       </c>
       <c r="M47" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -23197,7 +23213,7 @@
       </c>
       <c r="L48" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S24#0001</v>
+        <v>EUR_YC3MRH_1S24#0002</v>
       </c>
       <c r="M48" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -23242,7 +23258,7 @@
       </c>
       <c r="L49" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2S24#0001</v>
+        <v>EUR_YC3MRH_2S24#0002</v>
       </c>
       <c r="M49" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -23287,7 +23303,7 @@
       </c>
       <c r="L50" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S36#0001</v>
+        <v>EUR_YC3MRH_1S36#0002</v>
       </c>
       <c r="M50" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -23461,7 +23477,7 @@
       </c>
       <c r="L4" s="204" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC3MRH_AB3EBASIS_ibor3M#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS_ibor3M#0002</v>
       </c>
       <c r="M4" s="203" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -23525,7 +23541,7 @@
       </c>
       <c r="L6" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS1Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS1Y#0001</v>
       </c>
       <c r="M6" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -23574,7 +23590,7 @@
       </c>
       <c r="L7" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS15M#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS15M#0001</v>
       </c>
       <c r="M7" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -23623,7 +23639,7 @@
       </c>
       <c r="L8" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS18M#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS18M#0001</v>
       </c>
       <c r="M8" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -23672,7 +23688,7 @@
       </c>
       <c r="L9" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS21M#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS21M#0001</v>
       </c>
       <c r="M9" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -23721,7 +23737,7 @@
       </c>
       <c r="L10" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS2Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS2Y#0001</v>
       </c>
       <c r="M10" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -23779,7 +23795,7 @@
       </c>
       <c r="L11" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS3Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS3Y#0001</v>
       </c>
       <c r="M11" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -23837,7 +23853,7 @@
       </c>
       <c r="L12" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS4Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS4Y#0001</v>
       </c>
       <c r="M12" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -23895,7 +23911,7 @@
       </c>
       <c r="L13" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS5Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS5Y#0001</v>
       </c>
       <c r="M13" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -23953,7 +23969,7 @@
       </c>
       <c r="L14" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS6Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS6Y#0001</v>
       </c>
       <c r="M14" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -24011,7 +24027,7 @@
       </c>
       <c r="L15" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS7Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS7Y#0001</v>
       </c>
       <c r="M15" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -24063,7 +24079,7 @@
       </c>
       <c r="L16" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS8Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS8Y#0001</v>
       </c>
       <c r="M16" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -24112,7 +24128,7 @@
       </c>
       <c r="L17" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS9Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS9Y#0001</v>
       </c>
       <c r="M17" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -24161,7 +24177,7 @@
       </c>
       <c r="L18" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS10Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS10Y#0001</v>
       </c>
       <c r="M18" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -24210,7 +24226,7 @@
       </c>
       <c r="L19" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS11Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS11Y#0001</v>
       </c>
       <c r="M19" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -24259,7 +24275,7 @@
       </c>
       <c r="L20" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS12Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS12Y#0001</v>
       </c>
       <c r="M20" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -24308,7 +24324,7 @@
       </c>
       <c r="L21" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS13Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS13Y#0001</v>
       </c>
       <c r="M21" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -24357,7 +24373,7 @@
       </c>
       <c r="L22" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS14Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS14Y#0001</v>
       </c>
       <c r="M22" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -24406,7 +24422,7 @@
       </c>
       <c r="L23" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS15Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS15Y#0001</v>
       </c>
       <c r="M23" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -24455,7 +24471,7 @@
       </c>
       <c r="L24" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS16Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS16Y#0001</v>
       </c>
       <c r="M24" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -24504,7 +24520,7 @@
       </c>
       <c r="L25" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS17Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS17Y#0001</v>
       </c>
       <c r="M25" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -24553,7 +24569,7 @@
       </c>
       <c r="L26" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS18Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS18Y#0001</v>
       </c>
       <c r="M26" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -24602,7 +24618,7 @@
       </c>
       <c r="L27" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS19Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS19Y#0001</v>
       </c>
       <c r="M27" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -24651,7 +24667,7 @@
       </c>
       <c r="L28" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS20Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS20Y#0001</v>
       </c>
       <c r="M28" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -24700,7 +24716,7 @@
       </c>
       <c r="L29" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS21Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS21Y#0001</v>
       </c>
       <c r="M29" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -24749,7 +24765,7 @@
       </c>
       <c r="L30" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS22Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS22Y#0001</v>
       </c>
       <c r="M30" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -24798,7 +24814,7 @@
       </c>
       <c r="L31" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS23Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS23Y#0001</v>
       </c>
       <c r="M31" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -24847,7 +24863,7 @@
       </c>
       <c r="L32" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS24Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS24Y#0001</v>
       </c>
       <c r="M32" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -24896,7 +24912,7 @@
       </c>
       <c r="L33" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS25Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS25Y#0001</v>
       </c>
       <c r="M33" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -24945,7 +24961,7 @@
       </c>
       <c r="L34" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS26Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS26Y#0001</v>
       </c>
       <c r="M34" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -24994,7 +25010,7 @@
       </c>
       <c r="L35" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS27Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS27Y#0001</v>
       </c>
       <c r="M35" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -25043,7 +25059,7 @@
       </c>
       <c r="L36" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS28Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS28Y#0001</v>
       </c>
       <c r="M36" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -25092,7 +25108,7 @@
       </c>
       <c r="L37" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS29Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS29Y#0001</v>
       </c>
       <c r="M37" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -25141,7 +25157,7 @@
       </c>
       <c r="L38" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS30Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS30Y#0001</v>
       </c>
       <c r="M38" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -25190,7 +25206,7 @@
       </c>
       <c r="L39" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS35Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS35Y#0001</v>
       </c>
       <c r="M39" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -25239,7 +25255,7 @@
       </c>
       <c r="L40" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS40Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS40Y#0001</v>
       </c>
       <c r="M40" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -25288,7 +25304,7 @@
       </c>
       <c r="L41" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS50Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS50Y#0001</v>
       </c>
       <c r="M41" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -25337,7 +25353,7 @@
       </c>
       <c r="L42" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS60Y#0000</v>
+        <v>EUR_YC3MRH_AB3EBASIS60Y#0001</v>
       </c>
       <c r="M42" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>

<commit_message>
EUR 3M curve bootstrap - work in progress - workaround for bug in setting futures quotes
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC3MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -309,7 +309,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="191">
   <si>
     <t>Error</t>
   </si>
@@ -882,9 +882,6 @@
   </si>
   <si>
     <t>EUR_YCRH_SwapsFromBasis</t>
-  </si>
-  <si>
-    <t>incorrectly selected in old build because of bug in setting futures quotes</t>
   </si>
 </sst>
 </file>
@@ -1568,7 +1565,7 @@
     <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -2038,13 +2035,7 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2054,6 +2045,13 @@
     <xf numFmtId="0" fontId="19" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2069,10 +2067,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2618,7 +2612,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AG95"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2643,19 +2637,19 @@
       </c>
     </row>
     <row r="2" spans="1:33" s="53" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="217" t="s">
+      <c r="B2" s="221" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="219"/>
-      <c r="K2" s="220" t="s">
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="223"/>
+      <c r="K2" s="218" t="s">
         <v>163</v>
       </c>
-      <c r="L2" s="221"/>
-      <c r="M2" s="221"/>
-      <c r="N2" s="222"/>
+      <c r="L2" s="219"/>
+      <c r="M2" s="219"/>
+      <c r="N2" s="220"/>
     </row>
     <row r="3" spans="1:33" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="53"/>
@@ -3013,7 +3007,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="86">
-        <v>41646.188391203701</v>
+        <v>41646.210173611114</v>
       </c>
       <c r="E11" s="58"/>
       <c r="F11" s="57"/>
@@ -3060,12 +3054,12 @@
       <c r="H12" s="53"/>
       <c r="I12" s="53"/>
       <c r="J12" s="53"/>
-      <c r="K12" s="220" t="s">
+      <c r="K12" s="218" t="s">
         <v>159</v>
       </c>
-      <c r="L12" s="221"/>
-      <c r="M12" s="221"/>
-      <c r="N12" s="222"/>
+      <c r="L12" s="219"/>
+      <c r="M12" s="219"/>
+      <c r="N12" s="220"/>
       <c r="O12" s="53"/>
       <c r="P12" s="53"/>
       <c r="Q12" s="53"/>
@@ -3129,7 +3123,7 @@
       </c>
       <c r="D14" s="83" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYC3M#0008</v>
+        <v>_EURYC3M#0005</v>
       </c>
       <c r="E14" s="58"/>
       <c r="F14" s="57"/>
@@ -3344,12 +3338,12 @@
       <c r="H19" s="53"/>
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
-      <c r="K19" s="220" t="s">
+      <c r="K19" s="218" t="s">
         <v>163</v>
       </c>
-      <c r="L19" s="221"/>
-      <c r="M19" s="221"/>
-      <c r="N19" s="222"/>
+      <c r="L19" s="219"/>
+      <c r="M19" s="219"/>
+      <c r="N19" s="220"/>
       <c r="O19" s="53"/>
       <c r="P19" s="53"/>
       <c r="Q19" s="53"/>
@@ -3682,9 +3676,9 @@
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
         <v>41648</v>
       </c>
-      <c r="D27" s="64" t="e">
+      <c r="D27" s="64">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="E27" s="58"/>
       <c r="F27" s="57"/>
@@ -3723,9 +3717,9 @@
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
         <v>63563</v>
       </c>
-      <c r="D28" s="62" t="e">
+      <c r="D28" s="62">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>#NUM!</v>
+        <v>0.20246286490853307</v>
       </c>
       <c r="E28" s="58"/>
       <c r="F28" s="57"/>
@@ -3764,8 +3758,8 @@
         <v>0</v>
       </c>
       <c r="D29" s="59" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v>qlPiecewiseYieldCurveData - 13th instrument (maturity: January 9th, 2017) has an invalid quote</v>
+        <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
+        <v/>
       </c>
       <c r="E29" s="58"/>
       <c r="F29" s="57"/>
@@ -3773,12 +3767,12 @@
       <c r="H29" s="53"/>
       <c r="I29" s="53"/>
       <c r="J29" s="53"/>
-      <c r="K29" s="220" t="s">
+      <c r="K29" s="218" t="s">
         <v>159</v>
       </c>
-      <c r="L29" s="221"/>
-      <c r="M29" s="221"/>
-      <c r="N29" s="222"/>
+      <c r="L29" s="219"/>
+      <c r="M29" s="219"/>
+      <c r="N29" s="220"/>
       <c r="O29" s="53"/>
       <c r="P29" s="53"/>
       <c r="Q29" s="53"/>
@@ -4032,12 +4026,12 @@
       <c r="H36" s="53"/>
       <c r="I36" s="53"/>
       <c r="J36" s="53"/>
-      <c r="K36" s="220" t="s">
+      <c r="K36" s="218" t="s">
         <v>163</v>
       </c>
-      <c r="L36" s="221"/>
-      <c r="M36" s="221"/>
-      <c r="N36" s="222"/>
+      <c r="L36" s="219"/>
+      <c r="M36" s="219"/>
+      <c r="N36" s="220"/>
       <c r="O36" s="53"/>
       <c r="P36" s="53"/>
       <c r="Q36" s="53"/>
@@ -4407,12 +4401,12 @@
       <c r="H46" s="53"/>
       <c r="I46" s="53"/>
       <c r="J46" s="53"/>
-      <c r="K46" s="220" t="s">
+      <c r="K46" s="218" t="s">
         <v>159</v>
       </c>
-      <c r="L46" s="221"/>
-      <c r="M46" s="221"/>
-      <c r="N46" s="222"/>
+      <c r="L46" s="219"/>
+      <c r="M46" s="219"/>
+      <c r="N46" s="220"/>
       <c r="O46" s="53"/>
       <c r="P46" s="53"/>
       <c r="Q46" s="53"/>
@@ -4666,12 +4660,12 @@
       <c r="H53" s="53"/>
       <c r="I53" s="53"/>
       <c r="J53" s="53"/>
-      <c r="K53" s="220" t="s">
+      <c r="K53" s="218" t="s">
         <v>163</v>
       </c>
-      <c r="L53" s="221"/>
-      <c r="M53" s="221"/>
-      <c r="N53" s="222"/>
+      <c r="L53" s="219"/>
+      <c r="M53" s="219"/>
+      <c r="N53" s="220"/>
       <c r="O53" s="53"/>
       <c r="P53" s="53"/>
       <c r="Q53" s="53"/>
@@ -5041,12 +5035,12 @@
       <c r="H63" s="53"/>
       <c r="I63" s="53"/>
       <c r="J63" s="53"/>
-      <c r="K63" s="220" t="s">
+      <c r="K63" s="218" t="s">
         <v>159</v>
       </c>
-      <c r="L63" s="221"/>
-      <c r="M63" s="221"/>
-      <c r="N63" s="222"/>
+      <c r="L63" s="219"/>
+      <c r="M63" s="219"/>
+      <c r="N63" s="220"/>
       <c r="O63" s="53"/>
       <c r="P63" s="53"/>
       <c r="Q63" s="53"/>
@@ -5308,12 +5302,12 @@
     </row>
     <row r="74" spans="1:33" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K75" s="220" t="s">
+      <c r="K75" s="218" t="s">
         <v>163</v>
       </c>
-      <c r="L75" s="221"/>
-      <c r="M75" s="221"/>
-      <c r="N75" s="222"/>
+      <c r="L75" s="219"/>
+      <c r="M75" s="219"/>
+      <c r="N75" s="220"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.2">
       <c r="K76" s="136"/>
@@ -5393,12 +5387,12 @@
       <c r="N84" s="121"/>
     </row>
     <row r="85" spans="11:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K85" s="220" t="s">
+      <c r="K85" s="218" t="s">
         <v>159</v>
       </c>
-      <c r="L85" s="221"/>
-      <c r="M85" s="221"/>
-      <c r="N85" s="222"/>
+      <c r="L85" s="219"/>
+      <c r="M85" s="219"/>
+      <c r="N85" s="220"/>
     </row>
     <row r="86" spans="11:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="K86" s="128"/>
@@ -5496,17 +5490,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K29:N29"/>
     <mergeCell ref="K85:N85"/>
     <mergeCell ref="K36:N36"/>
     <mergeCell ref="K46:N46"/>
     <mergeCell ref="K53:N53"/>
     <mergeCell ref="K63:N63"/>
     <mergeCell ref="K75:N75"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K29:N29"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 IZ25 SV25 ACR25 AMN25 AWJ25 BGF25 BQB25 BZX25 CJT25 CTP25 DDL25 DNH25 DXD25 EGZ25 EQV25 FAR25 FKN25 FUJ25 GEF25 GOB25 GXX25 HHT25 HRP25 IBL25 ILH25 IVD25 JEZ25 JOV25 JYR25 KIN25 KSJ25 LCF25 LMB25 LVX25 MFT25 MPP25 MZL25 NJH25 NTD25 OCZ25 OMV25 OWR25 PGN25 PQJ25 QAF25 QKB25 QTX25 RDT25 RNP25 RXL25 SHH25 SRD25 TAZ25 TKV25 TUR25 UEN25 UOJ25 UYF25 VIB25 VRX25 WBT25 WLP25 WVL25 D65561 IZ65561 SV65561 ACR65561 AMN65561 AWJ65561 BGF65561 BQB65561 BZX65561 CJT65561 CTP65561 DDL65561 DNH65561 DXD65561 EGZ65561 EQV65561 FAR65561 FKN65561 FUJ65561 GEF65561 GOB65561 GXX65561 HHT65561 HRP65561 IBL65561 ILH65561 IVD65561 JEZ65561 JOV65561 JYR65561 KIN65561 KSJ65561 LCF65561 LMB65561 LVX65561 MFT65561 MPP65561 MZL65561 NJH65561 NTD65561 OCZ65561 OMV65561 OWR65561 PGN65561 PQJ65561 QAF65561 QKB65561 QTX65561 RDT65561 RNP65561 RXL65561 SHH65561 SRD65561 TAZ65561 TKV65561 TUR65561 UEN65561 UOJ65561 UYF65561 VIB65561 VRX65561 WBT65561 WLP65561 WVL65561 D131097 IZ131097 SV131097 ACR131097 AMN131097 AWJ131097 BGF131097 BQB131097 BZX131097 CJT131097 CTP131097 DDL131097 DNH131097 DXD131097 EGZ131097 EQV131097 FAR131097 FKN131097 FUJ131097 GEF131097 GOB131097 GXX131097 HHT131097 HRP131097 IBL131097 ILH131097 IVD131097 JEZ131097 JOV131097 JYR131097 KIN131097 KSJ131097 LCF131097 LMB131097 LVX131097 MFT131097 MPP131097 MZL131097 NJH131097 NTD131097 OCZ131097 OMV131097 OWR131097 PGN131097 PQJ131097 QAF131097 QKB131097 QTX131097 RDT131097 RNP131097 RXL131097 SHH131097 SRD131097 TAZ131097 TKV131097 TUR131097 UEN131097 UOJ131097 UYF131097 VIB131097 VRX131097 WBT131097 WLP131097 WVL131097 D196633 IZ196633 SV196633 ACR196633 AMN196633 AWJ196633 BGF196633 BQB196633 BZX196633 CJT196633 CTP196633 DDL196633 DNH196633 DXD196633 EGZ196633 EQV196633 FAR196633 FKN196633 FUJ196633 GEF196633 GOB196633 GXX196633 HHT196633 HRP196633 IBL196633 ILH196633 IVD196633 JEZ196633 JOV196633 JYR196633 KIN196633 KSJ196633 LCF196633 LMB196633 LVX196633 MFT196633 MPP196633 MZL196633 NJH196633 NTD196633 OCZ196633 OMV196633 OWR196633 PGN196633 PQJ196633 QAF196633 QKB196633 QTX196633 RDT196633 RNP196633 RXL196633 SHH196633 SRD196633 TAZ196633 TKV196633 TUR196633 UEN196633 UOJ196633 UYF196633 VIB196633 VRX196633 WBT196633 WLP196633 WVL196633 D262169 IZ262169 SV262169 ACR262169 AMN262169 AWJ262169 BGF262169 BQB262169 BZX262169 CJT262169 CTP262169 DDL262169 DNH262169 DXD262169 EGZ262169 EQV262169 FAR262169 FKN262169 FUJ262169 GEF262169 GOB262169 GXX262169 HHT262169 HRP262169 IBL262169 ILH262169 IVD262169 JEZ262169 JOV262169 JYR262169 KIN262169 KSJ262169 LCF262169 LMB262169 LVX262169 MFT262169 MPP262169 MZL262169 NJH262169 NTD262169 OCZ262169 OMV262169 OWR262169 PGN262169 PQJ262169 QAF262169 QKB262169 QTX262169 RDT262169 RNP262169 RXL262169 SHH262169 SRD262169 TAZ262169 TKV262169 TUR262169 UEN262169 UOJ262169 UYF262169 VIB262169 VRX262169 WBT262169 WLP262169 WVL262169 D327705 IZ327705 SV327705 ACR327705 AMN327705 AWJ327705 BGF327705 BQB327705 BZX327705 CJT327705 CTP327705 DDL327705 DNH327705 DXD327705 EGZ327705 EQV327705 FAR327705 FKN327705 FUJ327705 GEF327705 GOB327705 GXX327705 HHT327705 HRP327705 IBL327705 ILH327705 IVD327705 JEZ327705 JOV327705 JYR327705 KIN327705 KSJ327705 LCF327705 LMB327705 LVX327705 MFT327705 MPP327705 MZL327705 NJH327705 NTD327705 OCZ327705 OMV327705 OWR327705 PGN327705 PQJ327705 QAF327705 QKB327705 QTX327705 RDT327705 RNP327705 RXL327705 SHH327705 SRD327705 TAZ327705 TKV327705 TUR327705 UEN327705 UOJ327705 UYF327705 VIB327705 VRX327705 WBT327705 WLP327705 WVL327705 D393241 IZ393241 SV393241 ACR393241 AMN393241 AWJ393241 BGF393241 BQB393241 BZX393241 CJT393241 CTP393241 DDL393241 DNH393241 DXD393241 EGZ393241 EQV393241 FAR393241 FKN393241 FUJ393241 GEF393241 GOB393241 GXX393241 HHT393241 HRP393241 IBL393241 ILH393241 IVD393241 JEZ393241 JOV393241 JYR393241 KIN393241 KSJ393241 LCF393241 LMB393241 LVX393241 MFT393241 MPP393241 MZL393241 NJH393241 NTD393241 OCZ393241 OMV393241 OWR393241 PGN393241 PQJ393241 QAF393241 QKB393241 QTX393241 RDT393241 RNP393241 RXL393241 SHH393241 SRD393241 TAZ393241 TKV393241 TUR393241 UEN393241 UOJ393241 UYF393241 VIB393241 VRX393241 WBT393241 WLP393241 WVL393241 D458777 IZ458777 SV458777 ACR458777 AMN458777 AWJ458777 BGF458777 BQB458777 BZX458777 CJT458777 CTP458777 DDL458777 DNH458777 DXD458777 EGZ458777 EQV458777 FAR458777 FKN458777 FUJ458777 GEF458777 GOB458777 GXX458777 HHT458777 HRP458777 IBL458777 ILH458777 IVD458777 JEZ458777 JOV458777 JYR458777 KIN458777 KSJ458777 LCF458777 LMB458777 LVX458777 MFT458777 MPP458777 MZL458777 NJH458777 NTD458777 OCZ458777 OMV458777 OWR458777 PGN458777 PQJ458777 QAF458777 QKB458777 QTX458777 RDT458777 RNP458777 RXL458777 SHH458777 SRD458777 TAZ458777 TKV458777 TUR458777 UEN458777 UOJ458777 UYF458777 VIB458777 VRX458777 WBT458777 WLP458777 WVL458777 D524313 IZ524313 SV524313 ACR524313 AMN524313 AWJ524313 BGF524313 BQB524313 BZX524313 CJT524313 CTP524313 DDL524313 DNH524313 DXD524313 EGZ524313 EQV524313 FAR524313 FKN524313 FUJ524313 GEF524313 GOB524313 GXX524313 HHT524313 HRP524313 IBL524313 ILH524313 IVD524313 JEZ524313 JOV524313 JYR524313 KIN524313 KSJ524313 LCF524313 LMB524313 LVX524313 MFT524313 MPP524313 MZL524313 NJH524313 NTD524313 OCZ524313 OMV524313 OWR524313 PGN524313 PQJ524313 QAF524313 QKB524313 QTX524313 RDT524313 RNP524313 RXL524313 SHH524313 SRD524313 TAZ524313 TKV524313 TUR524313 UEN524313 UOJ524313 UYF524313 VIB524313 VRX524313 WBT524313 WLP524313 WVL524313 D589849 IZ589849 SV589849 ACR589849 AMN589849 AWJ589849 BGF589849 BQB589849 BZX589849 CJT589849 CTP589849 DDL589849 DNH589849 DXD589849 EGZ589849 EQV589849 FAR589849 FKN589849 FUJ589849 GEF589849 GOB589849 GXX589849 HHT589849 HRP589849 IBL589849 ILH589849 IVD589849 JEZ589849 JOV589849 JYR589849 KIN589849 KSJ589849 LCF589849 LMB589849 LVX589849 MFT589849 MPP589849 MZL589849 NJH589849 NTD589849 OCZ589849 OMV589849 OWR589849 PGN589849 PQJ589849 QAF589849 QKB589849 QTX589849 RDT589849 RNP589849 RXL589849 SHH589849 SRD589849 TAZ589849 TKV589849 TUR589849 UEN589849 UOJ589849 UYF589849 VIB589849 VRX589849 WBT589849 WLP589849 WVL589849 D655385 IZ655385 SV655385 ACR655385 AMN655385 AWJ655385 BGF655385 BQB655385 BZX655385 CJT655385 CTP655385 DDL655385 DNH655385 DXD655385 EGZ655385 EQV655385 FAR655385 FKN655385 FUJ655385 GEF655385 GOB655385 GXX655385 HHT655385 HRP655385 IBL655385 ILH655385 IVD655385 JEZ655385 JOV655385 JYR655385 KIN655385 KSJ655385 LCF655385 LMB655385 LVX655385 MFT655385 MPP655385 MZL655385 NJH655385 NTD655385 OCZ655385 OMV655385 OWR655385 PGN655385 PQJ655385 QAF655385 QKB655385 QTX655385 RDT655385 RNP655385 RXL655385 SHH655385 SRD655385 TAZ655385 TKV655385 TUR655385 UEN655385 UOJ655385 UYF655385 VIB655385 VRX655385 WBT655385 WLP655385 WVL655385 D720921 IZ720921 SV720921 ACR720921 AMN720921 AWJ720921 BGF720921 BQB720921 BZX720921 CJT720921 CTP720921 DDL720921 DNH720921 DXD720921 EGZ720921 EQV720921 FAR720921 FKN720921 FUJ720921 GEF720921 GOB720921 GXX720921 HHT720921 HRP720921 IBL720921 ILH720921 IVD720921 JEZ720921 JOV720921 JYR720921 KIN720921 KSJ720921 LCF720921 LMB720921 LVX720921 MFT720921 MPP720921 MZL720921 NJH720921 NTD720921 OCZ720921 OMV720921 OWR720921 PGN720921 PQJ720921 QAF720921 QKB720921 QTX720921 RDT720921 RNP720921 RXL720921 SHH720921 SRD720921 TAZ720921 TKV720921 TUR720921 UEN720921 UOJ720921 UYF720921 VIB720921 VRX720921 WBT720921 WLP720921 WVL720921 D786457 IZ786457 SV786457 ACR786457 AMN786457 AWJ786457 BGF786457 BQB786457 BZX786457 CJT786457 CTP786457 DDL786457 DNH786457 DXD786457 EGZ786457 EQV786457 FAR786457 FKN786457 FUJ786457 GEF786457 GOB786457 GXX786457 HHT786457 HRP786457 IBL786457 ILH786457 IVD786457 JEZ786457 JOV786457 JYR786457 KIN786457 KSJ786457 LCF786457 LMB786457 LVX786457 MFT786457 MPP786457 MZL786457 NJH786457 NTD786457 OCZ786457 OMV786457 OWR786457 PGN786457 PQJ786457 QAF786457 QKB786457 QTX786457 RDT786457 RNP786457 RXL786457 SHH786457 SRD786457 TAZ786457 TKV786457 TUR786457 UEN786457 UOJ786457 UYF786457 VIB786457 VRX786457 WBT786457 WLP786457 WVL786457 D851993 IZ851993 SV851993 ACR851993 AMN851993 AWJ851993 BGF851993 BQB851993 BZX851993 CJT851993 CTP851993 DDL851993 DNH851993 DXD851993 EGZ851993 EQV851993 FAR851993 FKN851993 FUJ851993 GEF851993 GOB851993 GXX851993 HHT851993 HRP851993 IBL851993 ILH851993 IVD851993 JEZ851993 JOV851993 JYR851993 KIN851993 KSJ851993 LCF851993 LMB851993 LVX851993 MFT851993 MPP851993 MZL851993 NJH851993 NTD851993 OCZ851993 OMV851993 OWR851993 PGN851993 PQJ851993 QAF851993 QKB851993 QTX851993 RDT851993 RNP851993 RXL851993 SHH851993 SRD851993 TAZ851993 TKV851993 TUR851993 UEN851993 UOJ851993 UYF851993 VIB851993 VRX851993 WBT851993 WLP851993 WVL851993 D917529 IZ917529 SV917529 ACR917529 AMN917529 AWJ917529 BGF917529 BQB917529 BZX917529 CJT917529 CTP917529 DDL917529 DNH917529 DXD917529 EGZ917529 EQV917529 FAR917529 FKN917529 FUJ917529 GEF917529 GOB917529 GXX917529 HHT917529 HRP917529 IBL917529 ILH917529 IVD917529 JEZ917529 JOV917529 JYR917529 KIN917529 KSJ917529 LCF917529 LMB917529 LVX917529 MFT917529 MPP917529 MZL917529 NJH917529 NTD917529 OCZ917529 OMV917529 OWR917529 PGN917529 PQJ917529 QAF917529 QKB917529 QTX917529 RDT917529 RNP917529 RXL917529 SHH917529 SRD917529 TAZ917529 TKV917529 TUR917529 UEN917529 UOJ917529 UYF917529 VIB917529 VRX917529 WBT917529 WLP917529 WVL917529 D983065 IZ983065 SV983065 ACR983065 AMN983065 AWJ983065 BGF983065 BQB983065 BZX983065 CJT983065 CTP983065 DDL983065 DNH983065 DXD983065 EGZ983065 EQV983065 FAR983065 FKN983065 FUJ983065 GEF983065 GOB983065 GXX983065 HHT983065 HRP983065 IBL983065 ILH983065 IVD983065 JEZ983065 JOV983065 JYR983065 KIN983065 KSJ983065 LCF983065 LMB983065 LVX983065 MFT983065 MPP983065 MZL983065 NJH983065 NTD983065 OCZ983065 OMV983065 OWR983065 PGN983065 PQJ983065 QAF983065 QKB983065 QTX983065 RDT983065 RNP983065 RXL983065 SHH983065 SRD983065 TAZ983065 TKV983065 TUR983065 UEN983065 UOJ983065 UYF983065 VIB983065 VRX983065 WBT983065 WLP983065 WVL983065">
@@ -5574,11 +5568,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="224" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="224"/>
-      <c r="D1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="226"/>
       <c r="E1" s="51" t="s">
         <v>83</v>
       </c>
@@ -6757,7 +6751,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B33" s="36">
         <v>16</v>
       </c>
@@ -6795,7 +6789,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B34" s="36">
         <v>17</v>
       </c>
@@ -6833,7 +6827,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B35" s="29">
         <v>18</v>
       </c>
@@ -6871,7 +6865,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="43" t="b">
         <v>0</v>
       </c>
@@ -6914,7 +6908,7 @@
         <v>41744</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="b">
         <v>0</v>
       </c>
@@ -6956,7 +6950,7 @@
         <v>41778</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="35" t="b">
         <v>0</v>
       </c>
@@ -6998,7 +6992,7 @@
         <v>41809</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="35" t="b">
         <v>0</v>
       </c>
@@ -7022,8 +7016,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E39,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H39" s="228" t="b">
-        <v>0</v>
+      <c r="H39" s="32" t="b">
+        <v>1</v>
       </c>
       <c r="I39" s="32">
         <v>60</v>
@@ -7039,11 +7033,8 @@
         <f>_xll.qlRateHelperLatestDate($E39,Trigger)</f>
         <v>41836</v>
       </c>
-      <c r="N39" s="229" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="b">
         <v>0</v>
       </c>
@@ -7061,7 +7052,7 @@
       </c>
       <c r="F40" s="48">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
-        <v>99.677500000000009</v>
+        <v>99.677499999999995</v>
       </c>
       <c r="G40" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E40,Trigger)</f>
@@ -7085,7 +7076,7 @@
         <v>41872</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="b">
         <v>0</v>
       </c>
@@ -7101,16 +7092,16 @@
         <f t="shared" si="2"/>
         <v>EUR_YC3MRH_FUT3MM4</v>
       </c>
-      <c r="F41" s="48" t="e">
+      <c r="F41" s="48">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G41" s="33" t="e">
+        <v>99.547499999999999</v>
+      </c>
+      <c r="G41" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E41,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H41" s="228" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="H41" s="32" t="b">
+        <v>1</v>
       </c>
       <c r="I41" s="32">
         <v>60</v>
@@ -7127,7 +7118,7 @@
         <v>41900</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="35" t="b">
         <v>0</v>
       </c>
@@ -7151,8 +7142,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E42,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H42" s="228" t="b">
-        <v>0</v>
+      <c r="H42" s="32" t="b">
+        <v>1</v>
       </c>
       <c r="I42" s="32">
         <v>60</v>
@@ -7169,7 +7160,7 @@
         <v>41928</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="35" t="b">
         <v>0</v>
       </c>
@@ -7211,7 +7202,7 @@
         <v>41963</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="b">
         <v>0</v>
       </c>
@@ -7227,16 +7218,16 @@
         <f t="shared" si="2"/>
         <v>EUR_YC3MRH_FUT3MU4</v>
       </c>
-      <c r="F44" s="48" t="e">
+      <c r="F44" s="48">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G44" s="33" t="e">
+        <v>99.487499999999997</v>
+      </c>
+      <c r="G44" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E44,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H44" s="228" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="H44" s="32" t="b">
+        <v>1</v>
       </c>
       <c r="I44" s="32">
         <v>60</v>
@@ -7253,7 +7244,7 @@
         <v>41990</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="b">
         <v>0</v>
       </c>
@@ -7277,8 +7268,8 @@
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E45,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H45" s="228" t="b">
-        <v>0</v>
+      <c r="H45" s="32" t="b">
+        <v>1</v>
       </c>
       <c r="I45" s="32">
         <v>60</v>
@@ -7295,7 +7286,7 @@
         <v>42019</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="b">
         <v>0</v>
       </c>
@@ -7337,7 +7328,7 @@
         <v>42054</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="b">
         <v>0</v>
       </c>
@@ -7353,16 +7344,16 @@
         <f t="shared" si="2"/>
         <v>EUR_YC3MRH_FUT3MZ4</v>
       </c>
-      <c r="F47" s="48" t="e">
+      <c r="F47" s="48">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G47" s="33" t="e">
+        <v>99.417500000000004</v>
+      </c>
+      <c r="G47" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E47,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H47" s="228" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="H47" s="32" t="b">
+        <v>1</v>
       </c>
       <c r="I47" s="32">
         <v>60</v>
@@ -7379,7 +7370,7 @@
         <v>42080</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="b">
         <v>1</v>
       </c>
@@ -7607,7 +7598,7 @@
       </c>
       <c r="F53" s="48">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
-        <v>99.074999999999989</v>
+        <v>99.075000000000003</v>
       </c>
       <c r="G53" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E53,Trigger)</f>
@@ -7649,7 +7640,7 @@
       </c>
       <c r="F54" s="48">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
-        <v>98.949999999999989</v>
+        <v>98.95</v>
       </c>
       <c r="G54" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E54,Trigger)</f>
@@ -7691,7 +7682,7 @@
       </c>
       <c r="F55" s="48">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
-        <v>98.802500000000009</v>
+        <v>98.802499999999995</v>
       </c>
       <c r="G55" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E55,Trigger)</f>
@@ -7817,7 +7808,7 @@
       </c>
       <c r="F58" s="48">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
-        <v>98.38</v>
+        <v>98.385000000000005</v>
       </c>
       <c r="G58" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E58,Trigger)</f>
@@ -7859,7 +7850,7 @@
       </c>
       <c r="F59" s="48">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
-        <v>98.245000000000005</v>
+        <v>98.25</v>
       </c>
       <c r="G59" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E59,Trigger)</f>
@@ -7901,7 +7892,7 @@
       </c>
       <c r="F60" s="48">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
-        <v>98.122500000000002</v>
+        <v>98.125</v>
       </c>
       <c r="G60" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E60,Trigger)</f>
@@ -7943,7 +7934,7 @@
       </c>
       <c r="F61" s="48">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
-        <v>98.004999999999995</v>
+        <v>98.01</v>
       </c>
       <c r="G61" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E61,Trigger)</f>
@@ -7985,7 +7976,7 @@
       </c>
       <c r="F62" s="48">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
-        <v>97.91749999999999</v>
+        <v>97.922499999999999</v>
       </c>
       <c r="G62" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E62,Trigger)</f>
@@ -8027,7 +8018,7 @@
       </c>
       <c r="F63" s="48">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
-        <v>97.83250000000001</v>
+        <v>97.834999999999994</v>
       </c>
       <c r="G63" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E63,Trigger)</f>
@@ -8069,7 +8060,7 @@
       </c>
       <c r="F64" s="48">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
-        <v>97.757499999999993</v>
+        <v>97.76</v>
       </c>
       <c r="G64" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E64,Trigger)</f>
@@ -8111,7 +8102,7 @@
       </c>
       <c r="F65" s="48">
         <f>_xll.qlRateHelperQuoteValue($E65,Trigger)</f>
-        <v>97.67</v>
+        <v>97.672499999999999</v>
       </c>
       <c r="G65" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E65,Trigger)</f>
@@ -9342,9 +9333,9 @@
         <f t="shared" si="4"/>
         <v>EUR_YC3MRH_AB3E1Y</v>
       </c>
-      <c r="F96" s="33" t="e">
+      <c r="F96" s="33">
         <f>_xll.qlRateHelperQuoteValue($E96,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.2699999999999995E-3</v>
       </c>
       <c r="G96" s="33">
         <f>_xll.qlSwapRateHelperSpread($E96,Trigger)</f>
@@ -9367,9 +9358,9 @@
         <f>_xll.qlRateHelperLatestDate($E96,Trigger)</f>
         <v>42013</v>
       </c>
-      <c r="N96" s="37" t="e">
+      <c r="N96" s="37">
         <f t="shared" ref="N96:N132" si="7">IF(G96=G133,F96-F133,"--")</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.2">
@@ -9388,9 +9379,9 @@
         <f t="shared" si="4"/>
         <v>EUR_YC3MRH_AB3E15M</v>
       </c>
-      <c r="F97" s="33" t="e">
+      <c r="F97" s="33">
         <f>_xll.qlRateHelperQuoteValue($E97,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.5899999999999999E-3</v>
       </c>
       <c r="G97" s="33">
         <f>_xll.qlSwapRateHelperSpread($E97,Trigger)</f>
@@ -9413,9 +9404,9 @@
         <f>_xll.qlRateHelperLatestDate($E97,Trigger)</f>
         <v>42103</v>
       </c>
-      <c r="N97" s="37" t="e">
+      <c r="N97" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>1.4100000000000007E-4</v>
       </c>
     </row>
     <row r="98" spans="2:14" x14ac:dyDescent="0.2">
@@ -9434,9 +9425,9 @@
         <f t="shared" ref="E98:E129" si="8">RateHelperPrefix&amp;"_"&amp;$B98&amp;$C98&amp;$D98</f>
         <v>EUR_YC3MRH_AB3E18M</v>
       </c>
-      <c r="F98" s="33" t="e">
+      <c r="F98" s="33">
         <f>_xll.qlRateHelperQuoteValue($E98,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.9199999999999999E-3</v>
       </c>
       <c r="G98" s="33">
         <f>_xll.qlSwapRateHelperSpread($E98,Trigger)</f>
@@ -9459,9 +9450,9 @@
         <f>_xll.qlRateHelperLatestDate($E98,Trigger)</f>
         <v>42194</v>
       </c>
-      <c r="N98" s="37" t="e">
+      <c r="N98" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>9.9999999999995925E-6</v>
       </c>
     </row>
     <row r="99" spans="2:14" x14ac:dyDescent="0.2">
@@ -9480,9 +9471,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E21M</v>
       </c>
-      <c r="F99" s="33" t="e">
+      <c r="F99" s="33">
         <f>_xll.qlRateHelperQuoteValue($E99,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.2300000000000003E-3</v>
       </c>
       <c r="G99" s="33">
         <f>_xll.qlSwapRateHelperSpread($E99,Trigger)</f>
@@ -9505,9 +9496,9 @@
         <f>_xll.qlRateHelperLatestDate($E99,Trigger)</f>
         <v>42286</v>
       </c>
-      <c r="N99" s="37" t="e">
+      <c r="N99" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>1.0999999999999985E-4</v>
       </c>
     </row>
     <row r="100" spans="2:14" x14ac:dyDescent="0.2">
@@ -9526,9 +9517,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E2Y</v>
       </c>
-      <c r="F100" s="33" t="e">
+      <c r="F100" s="33">
         <f>_xll.qlRateHelperQuoteValue($E100,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.5699999999999994E-3</v>
       </c>
       <c r="G100" s="33">
         <f>_xll.qlSwapRateHelperSpread($E100,Trigger)</f>
@@ -9551,9 +9542,9 @@
         <f>_xll.qlRateHelperLatestDate($E100,Trigger)</f>
         <v>42380</v>
       </c>
-      <c r="N100" s="37" t="e">
+      <c r="N100" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>4.9999999999989289E-6</v>
       </c>
     </row>
     <row r="101" spans="2:14" x14ac:dyDescent="0.2">
@@ -9572,9 +9563,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E3Y</v>
       </c>
-      <c r="F101" s="33" t="e">
+      <c r="F101" s="33">
         <f>_xll.qlRateHelperQuoteValue($E101,Trigger)</f>
-        <v>#NUM!</v>
+        <v>6.2100000000000002E-3</v>
       </c>
       <c r="G101" s="33">
         <f>_xll.qlSwapRateHelperSpread($E101,Trigger)</f>
@@ -9597,9 +9588,9 @@
         <f>_xll.qlRateHelperLatestDate($E101,Trigger)</f>
         <v>42744</v>
       </c>
-      <c r="N101" s="37" t="e">
+      <c r="N101" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="2:14" x14ac:dyDescent="0.2">
@@ -9618,9 +9609,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E4Y</v>
       </c>
-      <c r="F102" s="33" t="e">
+      <c r="F102" s="33">
         <f>_xll.qlRateHelperQuoteValue($E102,Trigger)</f>
-        <v>#NUM!</v>
+        <v>8.3800000000000003E-3</v>
       </c>
       <c r="G102" s="33">
         <f>_xll.qlSwapRateHelperSpread($E102,Trigger)</f>
@@ -9643,9 +9634,9 @@
         <f>_xll.qlRateHelperLatestDate($E102,Trigger)</f>
         <v>43109</v>
       </c>
-      <c r="N102" s="37" t="e">
+      <c r="N102" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>4.9999999999997963E-6</v>
       </c>
     </row>
     <row r="103" spans="2:14" x14ac:dyDescent="0.2">
@@ -9664,9 +9655,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E5Y</v>
       </c>
-      <c r="F103" s="33" t="e">
+      <c r="F103" s="33">
         <f>_xll.qlRateHelperQuoteValue($E103,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.065E-2</v>
       </c>
       <c r="G103" s="33">
         <f>_xll.qlSwapRateHelperSpread($E103,Trigger)</f>
@@ -9689,9 +9680,9 @@
         <f>_xll.qlRateHelperLatestDate($E103,Trigger)</f>
         <v>43474</v>
       </c>
-      <c r="N103" s="37" t="e">
+      <c r="N103" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-1.7347234759768071E-18</v>
       </c>
     </row>
     <row r="104" spans="2:14" x14ac:dyDescent="0.2">
@@ -9710,9 +9701,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E6Y</v>
       </c>
-      <c r="F104" s="33" t="e">
+      <c r="F104" s="33">
         <f>_xll.qlRateHelperQuoteValue($E104,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.2629999999999999E-2</v>
       </c>
       <c r="G104" s="33">
         <f>_xll.qlSwapRateHelperSpread($E104,Trigger)</f>
@@ -9735,9 +9726,9 @@
         <f>_xll.qlRateHelperLatestDate($E104,Trigger)</f>
         <v>43839</v>
       </c>
-      <c r="N104" s="37" t="e">
+      <c r="N104" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>4.9999999999997963E-6</v>
       </c>
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.2">
@@ -9756,9 +9747,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E7Y</v>
       </c>
-      <c r="F105" s="33" t="e">
+      <c r="F105" s="33">
         <f>_xll.qlRateHelperQuoteValue($E105,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.439E-2</v>
       </c>
       <c r="G105" s="33">
         <f>_xll.qlSwapRateHelperSpread($E105,Trigger)</f>
@@ -9781,9 +9772,9 @@
         <f>_xll.qlRateHelperLatestDate($E105,Trigger)</f>
         <v>44207</v>
       </c>
-      <c r="N105" s="37" t="e">
+      <c r="N105" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>1.7347234759768071E-18</v>
       </c>
     </row>
     <row r="106" spans="2:14" x14ac:dyDescent="0.2">
@@ -9802,9 +9793,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E8Y</v>
       </c>
-      <c r="F106" s="33" t="e">
+      <c r="F106" s="33">
         <f>_xll.qlRateHelperQuoteValue($E106,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.5950000000000002E-2</v>
       </c>
       <c r="G106" s="33">
         <f>_xll.qlSwapRateHelperSpread($E106,Trigger)</f>
@@ -9827,9 +9818,9 @@
         <f>_xll.qlRateHelperLatestDate($E106,Trigger)</f>
         <v>44571</v>
       </c>
-      <c r="N106" s="37" t="e">
+      <c r="N106" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>3.4694469519536142E-18</v>
       </c>
     </row>
     <row r="107" spans="2:14" x14ac:dyDescent="0.2">
@@ -9848,9 +9839,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E9Y</v>
       </c>
-      <c r="F107" s="33" t="e">
+      <c r="F107" s="33">
         <f>_xll.qlRateHelperQuoteValue($E107,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="G107" s="33">
         <f>_xll.qlSwapRateHelperSpread($E107,Trigger)</f>
@@ -9873,9 +9864,9 @@
         <f>_xll.qlRateHelperLatestDate($E107,Trigger)</f>
         <v>44935</v>
       </c>
-      <c r="N107" s="37" t="e">
+      <c r="N107" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>4.9999999999980616E-6</v>
       </c>
     </row>
     <row r="108" spans="2:14" x14ac:dyDescent="0.2">
@@ -9894,9 +9885,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E10Y</v>
       </c>
-      <c r="F108" s="33" t="e">
+      <c r="F108" s="33">
         <f>_xll.qlRateHelperQuoteValue($E108,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.8710000000000001E-2</v>
       </c>
       <c r="G108" s="33">
         <f>_xll.qlSwapRateHelperSpread($E108,Trigger)</f>
@@ -9919,9 +9910,9 @@
         <f>_xll.qlRateHelperLatestDate($E108,Trigger)</f>
         <v>45300</v>
       </c>
-      <c r="N108" s="37" t="e">
+      <c r="N108" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-9.9999999999995925E-6</v>
       </c>
     </row>
     <row r="109" spans="2:14" x14ac:dyDescent="0.2">
@@ -9940,9 +9931,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E11Y</v>
       </c>
-      <c r="F109" s="33" t="e">
+      <c r="F109" s="33">
         <f>_xll.qlRateHelperQuoteValue($E109,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.9860000000000003E-2</v>
       </c>
       <c r="G109" s="33">
         <f>_xll.qlSwapRateHelperSpread($E109,Trigger)</f>
@@ -9965,9 +9956,9 @@
         <f>_xll.qlRateHelperLatestDate($E109,Trigger)</f>
         <v>45666</v>
       </c>
-      <c r="N109" s="37" t="e">
+      <c r="N109" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-4.9999999999980616E-6</v>
       </c>
     </row>
     <row r="110" spans="2:14" x14ac:dyDescent="0.2">
@@ -9986,9 +9977,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E12Y</v>
       </c>
-      <c r="F110" s="33" t="e">
+      <c r="F110" s="33">
         <f>_xll.qlRateHelperQuoteValue($E110,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.0840000000000001E-2</v>
       </c>
       <c r="G110" s="33">
         <f>_xll.qlSwapRateHelperSpread($E110,Trigger)</f>
@@ -10011,9 +10002,9 @@
         <f>_xll.qlRateHelperLatestDate($E110,Trigger)</f>
         <v>46031</v>
       </c>
-      <c r="N110" s="37" t="e">
+      <c r="N110" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-4.9999999999980616E-6</v>
       </c>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.2">
@@ -10124,9 +10115,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E15Y</v>
       </c>
-      <c r="F113" s="33" t="e">
+      <c r="F113" s="33">
         <f>_xll.qlRateHelperQuoteValue($E113,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.2889999999999997E-2</v>
       </c>
       <c r="G113" s="33">
         <f>_xll.qlSwapRateHelperSpread($E113,Trigger)</f>
@@ -10149,9 +10140,9 @@
         <f>_xll.qlRateHelperLatestDate($E113,Trigger)</f>
         <v>47127</v>
       </c>
-      <c r="N113" s="37" t="e">
+      <c r="N113" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-1.0000000000003062E-5</v>
       </c>
     </row>
     <row r="114" spans="2:14" x14ac:dyDescent="0.2">
@@ -10354,9 +10345,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E20Y</v>
       </c>
-      <c r="F118" s="33" t="e">
+      <c r="F118" s="33">
         <f>_xll.qlRateHelperQuoteValue($E118,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.4119999999999999E-2</v>
       </c>
       <c r="G118" s="33">
         <f>_xll.qlSwapRateHelperSpread($E118,Trigger)</f>
@@ -10379,9 +10370,9 @@
         <f>_xll.qlRateHelperLatestDate($E118,Trigger)</f>
         <v>48953</v>
       </c>
-      <c r="N118" s="37" t="e">
+      <c r="N118" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-9.9999999999995925E-6</v>
       </c>
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.2">
@@ -10584,9 +10575,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E25Y</v>
       </c>
-      <c r="F123" s="33" t="e">
+      <c r="F123" s="33">
         <f>_xll.qlRateHelperQuoteValue($E123,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.4340000000000001E-2</v>
       </c>
       <c r="G123" s="33">
         <f>_xll.qlSwapRateHelperSpread($E123,Trigger)</f>
@@ -10609,9 +10600,9 @@
         <f>_xll.qlRateHelperLatestDate($E123,Trigger)</f>
         <v>50780</v>
       </c>
-      <c r="N123" s="37" t="e">
+      <c r="N123" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-4.9999999999980616E-6</v>
       </c>
     </row>
     <row r="124" spans="2:14" x14ac:dyDescent="0.2">
@@ -10814,9 +10805,9 @@
         <f t="shared" si="8"/>
         <v>EUR_YC3MRH_AB3E30Y</v>
       </c>
-      <c r="F128" s="33" t="e">
+      <c r="F128" s="33">
         <f>_xll.qlRateHelperQuoteValue($E128,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.4310000000000002E-2</v>
       </c>
       <c r="G128" s="33">
         <f>_xll.qlSwapRateHelperSpread($E128,Trigger)</f>
@@ -10839,9 +10830,9 @@
         <f>_xll.qlRateHelperLatestDate($E128,Trigger)</f>
         <v>52607</v>
       </c>
-      <c r="N128" s="37" t="e">
+      <c r="N128" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-9.9999999999961231E-6</v>
       </c>
     </row>
     <row r="129" spans="2:14" x14ac:dyDescent="0.2">
@@ -10906,9 +10897,9 @@
         <f t="shared" ref="E130:E161" si="10">RateHelperPrefix&amp;"_"&amp;$B130&amp;$C130&amp;$D130</f>
         <v>EUR_YC3MRH_AB3E40Y</v>
       </c>
-      <c r="F130" s="33" t="e">
+      <c r="F130" s="33">
         <f>_xll.qlRateHelperQuoteValue($E130,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.4809999999999999E-2</v>
       </c>
       <c r="G130" s="33">
         <f>_xll.qlSwapRateHelperSpread($E130,Trigger)</f>
@@ -10931,9 +10922,9 @@
         <f>_xll.qlRateHelperLatestDate($E130,Trigger)</f>
         <v>56258</v>
       </c>
-      <c r="N130" s="37" t="e">
+      <c r="N130" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-1.0000000000003062E-5</v>
       </c>
     </row>
     <row r="131" spans="2:14" x14ac:dyDescent="0.2">
@@ -10952,9 +10943,9 @@
         <f t="shared" si="10"/>
         <v>EUR_YC3MRH_AB3E50Y</v>
       </c>
-      <c r="F131" s="33" t="e">
+      <c r="F131" s="33">
         <f>_xll.qlRateHelperQuoteValue($E131,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.5300000000000003E-2</v>
       </c>
       <c r="G131" s="33">
         <f>_xll.qlSwapRateHelperSpread($E131,Trigger)</f>
@@ -10977,9 +10968,9 @@
         <f>_xll.qlRateHelperLatestDate($E131,Trigger)</f>
         <v>59910</v>
       </c>
-      <c r="N131" s="37" t="e">
+      <c r="N131" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>-4.9999999999980616E-6</v>
       </c>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.2">
@@ -10998,9 +10989,9 @@
         <f t="shared" si="10"/>
         <v>EUR_YC3MRH_AB3E60Y</v>
       </c>
-      <c r="F132" s="26" t="e">
+      <c r="F132" s="26">
         <f>_xll.qlRateHelperQuoteValue($E132,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.564E-2</v>
       </c>
       <c r="G132" s="26">
         <f>_xll.qlSwapRateHelperSpread($E132,Trigger)</f>
@@ -11023,9 +11014,9 @@
         <f>_xll.qlRateHelperLatestDate($E132,Trigger)</f>
         <v>63563</v>
       </c>
-      <c r="N132" s="37" t="e">
+      <c r="N132" s="37">
         <f t="shared" si="7"/>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.2">
@@ -12598,7 +12589,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -12618,10 +12609,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="227" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="227"/>
+      <c r="B1" s="228"/>
       <c r="D1" s="22" t="s">
         <v>9</v>
       </c>
@@ -12635,9 +12626,9 @@
       <c r="H1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="e">
+      <c r="I1" s="3">
         <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -12667,8 +12658,8 @@
         <f>_xll.qlRateHelperLatestDate($D2)</f>
         <v>41662</v>
       </c>
-      <c r="I2" s="3" t="e">
-        <v>#NUM!</v>
+      <c r="I2" s="3">
+        <v>0.99992312257724181</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>116</v>
@@ -12703,8 +12694,8 @@
         <f>_xll.qlRateHelperLatestDate($D3)</f>
         <v>41669</v>
       </c>
-      <c r="I3" s="3" t="e">
-        <v>#NUM!</v>
+      <c r="I3" s="3">
+        <v>0.99988381350087097</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>117</v>
@@ -12739,8 +12730,8 @@
         <f>_xll.qlRateHelperLatestDate($D4)</f>
         <v>41680</v>
       </c>
-      <c r="I4" s="3" t="e">
-        <v>#NUM!</v>
+      <c r="I4" s="3">
+        <v>0.99982109867807345</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>118</v>
@@ -12775,8 +12766,8 @@
         <f>_xll.qlRateHelperLatestDate($D5)</f>
         <v>41708</v>
       </c>
-      <c r="I5" s="3" t="e">
-        <v>#NUM!</v>
+      <c r="I5" s="3">
+        <v>0.99964545907718061</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>119</v>
@@ -12812,8 +12803,8 @@
         <f>_xll.qlRateHelperLatestDate($D6)</f>
         <v>41739</v>
       </c>
-      <c r="I6" s="3" t="e">
-        <v>#NUM!</v>
+      <c r="I6" s="3">
+        <v>0.99943236937651492</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>120</v>
@@ -12825,7 +12816,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="str">
         <f>_xll.ohGroup(,_xll.ohPack(D2:D126),Permanent,,ObjectOverwrite)</f>
-        <v>obj_0065a#0008</v>
+        <v>obj_0065a#0005</v>
       </c>
       <c r="B7" s="12" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -12850,8 +12841,8 @@
         <f>_xll.qlRateHelperLatestDate($D7)</f>
         <v>41809</v>
       </c>
-      <c r="I7" s="3" t="e">
-        <v>#NUM!</v>
+      <c r="I7" s="3">
+        <v>0.99885756504830558</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>121</v>
@@ -12862,11 +12853,11 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MH5</v>
+        <v>EUR_YC3MRH_FUT3MM4</v>
       </c>
       <c r="E8" s="10">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>5.1250000000000462E-3</v>
+        <v>4.5250000000000012E-3</v>
       </c>
       <c r="F8" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -12874,16 +12865,16 @@
       </c>
       <c r="G8" s="9">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>42081</v>
+        <v>41808</v>
       </c>
       <c r="H8" s="8">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>42173</v>
-      </c>
-      <c r="I8" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K8" s="229" t="s">
+        <v>41900</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.99771397583391219</v>
+      </c>
+      <c r="K8" s="217" t="s">
         <v>122</v>
       </c>
       <c r="L8" s="46">
@@ -12892,11 +12883,11 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MM5</v>
+        <v>EUR_YC3MRH_FUT3MU4</v>
       </c>
       <c r="E9" s="10">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>5.8249999999999691E-3</v>
+        <v>5.1250000000000462E-3</v>
       </c>
       <c r="F9" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -12904,16 +12895,16 @@
       </c>
       <c r="G9" s="9">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>42172</v>
+        <v>41899</v>
       </c>
       <c r="H9" s="8">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>42264</v>
-      </c>
-      <c r="I9" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K9" s="229" t="s">
+        <v>41990</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.99643674809953053</v>
+      </c>
+      <c r="K9" s="217" t="s">
         <v>123</v>
       </c>
       <c r="L9" s="46">
@@ -12922,11 +12913,11 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D10" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MU5</v>
+        <v>EUR_YC3MRH_FUT3MZ4</v>
       </c>
       <c r="E10" s="10">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>6.525000000000003E-3</v>
+        <v>5.8249999999999691E-3</v>
       </c>
       <c r="F10" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -12934,16 +12925,16 @@
       </c>
       <c r="G10" s="9">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42263</v>
+        <v>41990</v>
       </c>
       <c r="H10" s="8">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42354</v>
-      </c>
-      <c r="I10" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="K10" s="229" t="s">
+        <v>42080</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.99498779711997465</v>
+      </c>
+      <c r="K10" s="217" t="s">
         <v>124</v>
       </c>
       <c r="L10" s="46">
@@ -12952,11 +12943,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MZ5</v>
+        <v>EUR_YC3MRH_FUT3MH5</v>
       </c>
       <c r="E11" s="10">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>7.3250000000000259E-3</v>
+        <v>5.1250000000000462E-3</v>
       </c>
       <c r="F11" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -12964,14 +12955,14 @@
       </c>
       <c r="G11" s="9">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42354</v>
+        <v>42081</v>
       </c>
       <c r="H11" s="8">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42445</v>
-      </c>
-      <c r="I11" s="3" t="e">
-        <v>#NUM!</v>
+        <v>42173</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.99367121095164468</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>125</v>
@@ -12982,11 +12973,11 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MH6</v>
+        <v>EUR_YC3MRH_FUT3MM5</v>
       </c>
       <c r="E12" s="10">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>8.1749999999999323E-3</v>
+        <v>5.8249999999999691E-3</v>
       </c>
       <c r="F12" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -12994,14 +12985,14 @@
       </c>
       <c r="G12" s="9">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42445</v>
+        <v>42172</v>
       </c>
       <c r="H12" s="8">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42537</v>
-      </c>
-      <c r="I12" s="3" t="e">
-        <v>#NUM!</v>
+        <v>42264</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.99220879012734486</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>126</v>
@@ -13012,11 +13003,11 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D13" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MM6</v>
+        <v>EUR_YC3MRH_FUT3MU5</v>
       </c>
       <c r="E13" s="10">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>9.2500000000000915E-3</v>
+        <v>6.525000000000003E-3</v>
       </c>
       <c r="F13" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -13024,14 +13015,14 @@
       </c>
       <c r="G13" s="9">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42536</v>
+        <v>42263</v>
       </c>
       <c r="H13" s="8">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42628</v>
-      </c>
-      <c r="I13" s="3" t="e">
-        <v>#NUM!</v>
+        <v>42354</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.99059202119743606</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>127</v>
@@ -13042,11 +13033,11 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D14" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E3Y</v>
-      </c>
-      <c r="E14" s="10" t="e">
+        <v>EUR_YC3MRH_FUT3MZ5</v>
+      </c>
+      <c r="E14" s="10">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>#NUM!</v>
+        <v>7.3250000000000259E-3</v>
       </c>
       <c r="F14" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -13054,14 +13045,14 @@
       </c>
       <c r="G14" s="9">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41648</v>
+        <v>42354</v>
       </c>
       <c r="H14" s="8">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42744</v>
-      </c>
-      <c r="I14" s="3" t="e">
-        <v>#NUM!</v>
+        <v>42445</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.98876123364378021</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>128</v>
@@ -13072,11 +13063,11 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E4Y</v>
-      </c>
-      <c r="E15" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E3Y</v>
+      </c>
+      <c r="E15" s="10">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>#NUM!</v>
+        <v>6.2100000000000002E-3</v>
       </c>
       <c r="F15" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -13088,10 +13079,10 @@
       </c>
       <c r="H15" s="8">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>43109</v>
-      </c>
-      <c r="I15" s="3" t="e">
-        <v>#NUM!</v>
+        <v>42744</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.98157013253261871</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>129</v>
@@ -13102,11 +13093,11 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E5Y</v>
-      </c>
-      <c r="E16" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E4Y</v>
+      </c>
+      <c r="E16" s="10">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>#NUM!</v>
+        <v>8.3800000000000003E-3</v>
       </c>
       <c r="F16" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -13118,10 +13109,10 @@
       </c>
       <c r="H16" s="8">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>43474</v>
-      </c>
-      <c r="I16" s="3" t="e">
-        <v>#NUM!</v>
+        <v>43109</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.96702638501648219</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>130</v>
@@ -13132,11 +13123,11 @@
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D17" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E6Y</v>
-      </c>
-      <c r="E17" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E5Y</v>
+      </c>
+      <c r="E17" s="10">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>#NUM!</v>
+        <v>1.065E-2</v>
       </c>
       <c r="F17" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -13148,10 +13139,10 @@
       </c>
       <c r="H17" s="8">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>43839</v>
-      </c>
-      <c r="I17" s="3" t="e">
-        <v>#NUM!</v>
+        <v>43474</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.94799821051689015</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>131</v>
@@ -13162,11 +13153,11 @@
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D18" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E7Y</v>
-      </c>
-      <c r="E18" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E6Y</v>
+      </c>
+      <c r="E18" s="10">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>#NUM!</v>
+        <v>1.2629999999999999E-2</v>
       </c>
       <c r="F18" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -13178,10 +13169,10 @@
       </c>
       <c r="H18" s="8">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>44207</v>
-      </c>
-      <c r="I18" s="3" t="e">
-        <v>#NUM!</v>
+        <v>43839</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.92662697351495837</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>132</v>
@@ -13192,11 +13183,11 @@
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D19" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E8Y</v>
-      </c>
-      <c r="E19" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E7Y</v>
+      </c>
+      <c r="E19" s="10">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>#NUM!</v>
+        <v>1.439E-2</v>
       </c>
       <c r="F19" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -13208,10 +13199,10 @@
       </c>
       <c r="H19" s="8">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>44571</v>
-      </c>
-      <c r="I19" s="3" t="e">
-        <v>#NUM!</v>
+        <v>44207</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.90333123430935147</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>133</v>
@@ -13222,11 +13213,11 @@
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D20" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E9Y</v>
-      </c>
-      <c r="E20" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E8Y</v>
+      </c>
+      <c r="E20" s="10">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>#NUM!</v>
+        <v>1.5950000000000002E-2</v>
       </c>
       <c r="F20" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -13238,10 +13229,10 @@
       </c>
       <c r="H20" s="8">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>44935</v>
-      </c>
-      <c r="I20" s="3" t="e">
-        <v>#NUM!</v>
+        <v>44571</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.87887243076614874</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>134</v>
@@ -13252,11 +13243,11 @@
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D21" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E10Y</v>
-      </c>
-      <c r="E21" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E9Y</v>
+      </c>
+      <c r="E21" s="10">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>#NUM!</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="F21" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -13268,10 +13259,10 @@
       </c>
       <c r="H21" s="8">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>45300</v>
-      </c>
-      <c r="I21" s="3" t="e">
-        <v>#NUM!</v>
+        <v>44935</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.85305884090859074</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>135</v>
@@ -13282,11 +13273,11 @@
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D22" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E12Y</v>
-      </c>
-      <c r="E22" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E10Y</v>
+      </c>
+      <c r="E22" s="10">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>#NUM!</v>
+        <v>1.8710000000000001E-2</v>
       </c>
       <c r="F22" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -13298,10 +13289,10 @@
       </c>
       <c r="H22" s="8">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>46031</v>
-      </c>
-      <c r="I22" s="3" t="e">
-        <v>#NUM!</v>
+        <v>45300</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.8265316228423667</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>136</v>
@@ -13312,11 +13303,11 @@
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D23" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E15Y</v>
-      </c>
-      <c r="E23" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E12Y</v>
+      </c>
+      <c r="E23" s="10">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>#NUM!</v>
+        <v>2.0840000000000001E-2</v>
       </c>
       <c r="F23" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -13328,10 +13319,10 @@
       </c>
       <c r="H23" s="8">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>47127</v>
-      </c>
-      <c r="I23" s="3" t="e">
-        <v>#NUM!</v>
+        <v>46031</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.77398207320333701</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>137</v>
@@ -13342,11 +13333,11 @@
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D24" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E20Y</v>
-      </c>
-      <c r="E24" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E15Y</v>
+      </c>
+      <c r="E24" s="10">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>#NUM!</v>
+        <v>2.2889999999999997E-2</v>
       </c>
       <c r="F24" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -13358,10 +13349,10 @@
       </c>
       <c r="H24" s="8">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>48953</v>
-      </c>
-      <c r="I24" s="3" t="e">
-        <v>#NUM!</v>
+        <v>47127</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.70195267593278343</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>138</v>
@@ -13372,11 +13363,11 @@
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D25" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E25Y</v>
-      </c>
-      <c r="E25" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E20Y</v>
+      </c>
+      <c r="E25" s="10">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>#NUM!</v>
+        <v>2.4119999999999999E-2</v>
       </c>
       <c r="F25" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -13388,10 +13379,10 @@
       </c>
       <c r="H25" s="8">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>50780</v>
-      </c>
-      <c r="I25" s="3" t="e">
-        <v>#NUM!</v>
+        <v>48953</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.60833147378291885</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>139</v>
@@ -13402,11 +13393,11 @@
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D26" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E30Y</v>
-      </c>
-      <c r="E26" s="10" t="e">
+        <v>EUR_YC3MRH_AB3E25Y</v>
+      </c>
+      <c r="E26" s="10">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>#NUM!</v>
+        <v>2.4340000000000001E-2</v>
       </c>
       <c r="F26" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -13418,10 +13409,10 @@
       </c>
       <c r="H26" s="8">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>52607</v>
-      </c>
-      <c r="I26" s="3" t="e">
-        <v>#NUM!</v>
+        <v>50780</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.53612052213363737</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>140</v>
@@ -13432,11 +13423,11 @@
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D27" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS35Y</v>
+        <v>EUR_YC3MRH_AB3E30Y</v>
       </c>
       <c r="E27" s="10">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>2.4505000000000002E-2</v>
+        <v>2.4310000000000002E-2</v>
       </c>
       <c r="F27" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -13448,10 +13439,10 @@
       </c>
       <c r="H27" s="8">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>54434</v>
-      </c>
-      <c r="I27" s="3" t="e">
-        <v>#NUM!</v>
+        <v>52607</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0.47593975963723573</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>141</v>
@@ -13462,11 +13453,11 @@
     </row>
     <row r="28" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D28" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS40Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS35Y</v>
       </c>
       <c r="E28" s="10">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.4820000000000002E-2</v>
+        <v>2.4505000000000002E-2</v>
       </c>
       <c r="F28" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -13478,10 +13469,10 @@
       </c>
       <c r="H28" s="8">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>56258</v>
-      </c>
-      <c r="I28" s="3" t="e">
-        <v>#NUM!</v>
+        <v>54434</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0.41771217357978524</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>142</v>
@@ -13492,11 +13483,11 @@
     </row>
     <row r="29" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D29" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS50Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS40Y</v>
       </c>
       <c r="E29" s="10">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.5305000000000001E-2</v>
+        <v>2.4820000000000002E-2</v>
       </c>
       <c r="F29" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -13508,10 +13499,10 @@
       </c>
       <c r="H29" s="8">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>59910</v>
-      </c>
-      <c r="I29" s="3" t="e">
-        <v>#NUM!</v>
+        <v>56258</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.3625977530257124</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>143</v>
@@ -13522,11 +13513,11 @@
     </row>
     <row r="30" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D30" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS60Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS50Y</v>
       </c>
       <c r="E30" s="10">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.564E-2</v>
+        <v>2.5305000000000001E-2</v>
       </c>
       <c r="F30" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -13538,10 +13529,10 @@
       </c>
       <c r="H30" s="8">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>63563</v>
-      </c>
-      <c r="I30" s="3" t="e">
-        <v>#NUM!</v>
+        <v>59910</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.27157930902452659</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>144</v>
@@ -13551,27 +13542,27 @@
       </c>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D31" s="11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E31" s="10" t="e">
+      <c r="D31" s="11" t="str">
+        <v>EUR_YC3MRH_AB3EBASIS60Y</v>
+      </c>
+      <c r="E31" s="10">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F31" s="10" t="str">
+        <v>2.564E-2</v>
+      </c>
+      <c r="F31" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
-        <v>--</v>
-      </c>
-      <c r="G31" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="G31" s="9">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H31" s="8" t="e">
+        <v>41648</v>
+      </c>
+      <c r="H31" s="8">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="3" t="e">
-        <v>#NUM!</v>
+        <v>63563</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.20246286490853307</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>145</v>
@@ -13601,7 +13592,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I32" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.2">
@@ -13625,7 +13616,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I33" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.2">
@@ -13649,7 +13640,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I34" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.2">
@@ -13673,7 +13664,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I35" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.2">
@@ -13697,7 +13688,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I36" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.2">
@@ -13721,7 +13712,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I37" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.2">
@@ -13745,7 +13736,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I38" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.2">
@@ -13769,7 +13760,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I39" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.2">
@@ -13793,7 +13784,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I40" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.2">
@@ -13817,7 +13808,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I41" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.2">
@@ -13841,7 +13832,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I42" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.2">
@@ -13865,7 +13856,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I43" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.2">
@@ -13889,7 +13880,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I44" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.2">
@@ -13913,7 +13904,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I45" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.2">
@@ -13937,7 +13928,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I46" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.2">
@@ -13961,7 +13952,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I47" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.2">
@@ -13985,7 +13976,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I48" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.2">
@@ -14009,7 +14000,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I49" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.2">
@@ -14033,7 +14024,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I50" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="4:9" x14ac:dyDescent="0.2">
@@ -14057,7 +14048,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I51" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.2">
@@ -14081,7 +14072,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I52" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.2">
@@ -14105,7 +14096,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I53" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.2">
@@ -14129,7 +14120,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I54" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="55" spans="4:9" x14ac:dyDescent="0.2">
@@ -14153,7 +14144,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I55" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="56" spans="4:9" x14ac:dyDescent="0.2">
@@ -14177,7 +14168,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I56" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="4:9" x14ac:dyDescent="0.2">
@@ -14201,7 +14192,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I57" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.2">
@@ -14225,7 +14216,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I58" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="59" spans="4:9" x14ac:dyDescent="0.2">
@@ -14249,7 +14240,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I59" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="4:9" x14ac:dyDescent="0.2">
@@ -14273,7 +14264,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I60" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="61" spans="4:9" x14ac:dyDescent="0.2">
@@ -14297,7 +14288,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I61" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="4:9" x14ac:dyDescent="0.2">
@@ -14321,7 +14312,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I62" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.2">
@@ -14345,7 +14336,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I63" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.2">
@@ -14369,7 +14360,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I64" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.2">
@@ -14393,7 +14384,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I65" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.2">
@@ -14417,7 +14408,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I66" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.2">
@@ -14441,7 +14432,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I67" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.2">
@@ -14465,7 +14456,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I68" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.2">
@@ -14489,7 +14480,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I69" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.2">
@@ -14513,7 +14504,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I70" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.2">
@@ -14537,7 +14528,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I71" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.2">
@@ -14561,7 +14552,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I72" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.2">
@@ -14585,7 +14576,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I73" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.2">
@@ -14609,7 +14600,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I74" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.2">
@@ -14633,7 +14624,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I75" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.2">
@@ -14657,7 +14648,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I76" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.2">
@@ -14681,7 +14672,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I77" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.2">
@@ -14705,7 +14696,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I78" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.2">
@@ -14729,7 +14720,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I79" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.2">
@@ -14753,7 +14744,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I80" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="81" spans="4:9" x14ac:dyDescent="0.2">
@@ -14777,7 +14768,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I81" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="82" spans="4:9" x14ac:dyDescent="0.2">
@@ -14801,7 +14792,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I82" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="83" spans="4:9" x14ac:dyDescent="0.2">
@@ -14825,7 +14816,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I83" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="84" spans="4:9" x14ac:dyDescent="0.2">
@@ -14849,7 +14840,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I84" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="85" spans="4:9" x14ac:dyDescent="0.2">
@@ -14873,7 +14864,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I85" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="4:9" x14ac:dyDescent="0.2">
@@ -14897,7 +14888,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I86" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="4:9" x14ac:dyDescent="0.2">
@@ -14921,7 +14912,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I87" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="4:9" x14ac:dyDescent="0.2">
@@ -14945,7 +14936,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I88" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="89" spans="4:9" x14ac:dyDescent="0.2">
@@ -14969,7 +14960,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I89" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="90" spans="4:9" x14ac:dyDescent="0.2">
@@ -14993,7 +14984,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I90" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="4:9" x14ac:dyDescent="0.2">
@@ -15017,7 +15008,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I91" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="4:9" x14ac:dyDescent="0.2">
@@ -15041,7 +15032,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I92" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="4:9" x14ac:dyDescent="0.2">
@@ -15065,7 +15056,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I93" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="4:9" x14ac:dyDescent="0.2">
@@ -15089,7 +15080,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I94" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="95" spans="4:9" x14ac:dyDescent="0.2">
@@ -15113,7 +15104,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I95" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="96" spans="4:9" x14ac:dyDescent="0.2">
@@ -15137,7 +15128,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I96" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
@@ -15161,7 +15152,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I97" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
@@ -15185,7 +15176,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I98" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
@@ -15209,7 +15200,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I99" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
@@ -15233,7 +15224,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I100" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
@@ -15257,7 +15248,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I101" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
@@ -15281,7 +15272,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I102" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="103" spans="4:9" x14ac:dyDescent="0.2">
@@ -15305,7 +15296,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I103" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
@@ -15329,7 +15320,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I104" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
@@ -15353,7 +15344,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I105" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="106" spans="4:9" x14ac:dyDescent="0.2">
@@ -15377,7 +15368,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I106" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="107" spans="4:9" x14ac:dyDescent="0.2">
@@ -15401,7 +15392,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I107" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
@@ -15425,7 +15416,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I108" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
@@ -15449,7 +15440,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I109" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
@@ -15473,7 +15464,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I110" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
@@ -15497,7 +15488,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I111" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
@@ -15521,7 +15512,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I112" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="113" spans="4:9" x14ac:dyDescent="0.2">
@@ -15545,7 +15536,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I113" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="114" spans="4:9" x14ac:dyDescent="0.2">
@@ -15569,7 +15560,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I114" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="4:9" x14ac:dyDescent="0.2">
@@ -15593,7 +15584,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I115" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="116" spans="4:9" x14ac:dyDescent="0.2">
@@ -15617,7 +15608,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I116" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="4:9" x14ac:dyDescent="0.2">
@@ -15641,7 +15632,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I117" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="118" spans="4:9" x14ac:dyDescent="0.2">
@@ -15665,7 +15656,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I118" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="119" spans="4:9" x14ac:dyDescent="0.2">
@@ -15689,7 +15680,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I119" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="120" spans="4:9" x14ac:dyDescent="0.2">
@@ -15713,7 +15704,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I120" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="121" spans="4:9" x14ac:dyDescent="0.2">
@@ -15737,7 +15728,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I121" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="122" spans="4:9" x14ac:dyDescent="0.2">
@@ -15761,7 +15752,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I122" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="123" spans="4:9" x14ac:dyDescent="0.2">
@@ -15785,7 +15776,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I123" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="124" spans="4:9" x14ac:dyDescent="0.2">
@@ -15809,7 +15800,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I124" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="4:9" x14ac:dyDescent="0.2">
@@ -15833,7 +15824,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I125" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="126" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -15857,7 +15848,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I126" s="3" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -15952,7 +15943,7 @@
       </c>
       <c r="F3" s="109" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_SND#0002</v>
+        <v>EUR_YC3MRH_SND#0005</v>
       </c>
       <c r="G3" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -15979,7 +15970,7 @@
       </c>
       <c r="F4" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_SWD#0002</v>
+        <v>EUR_YC3MRH_SWD#0005</v>
       </c>
       <c r="G4" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -16006,7 +15997,7 @@
       </c>
       <c r="F5" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2WD#0002</v>
+        <v>EUR_YC3MRH_2WD#0005</v>
       </c>
       <c r="G5" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -16033,7 +16024,7 @@
       </c>
       <c r="F6" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3WD#0002</v>
+        <v>EUR_YC3MRH_3WD#0005</v>
       </c>
       <c r="G6" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -16060,7 +16051,7 @@
       </c>
       <c r="F7" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1MD#0002</v>
+        <v>EUR_YC3MRH_1MD#0005</v>
       </c>
       <c r="G7" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -16087,7 +16078,7 @@
       </c>
       <c r="F8" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2MD#0002</v>
+        <v>EUR_YC3MRH_2MD#0005</v>
       </c>
       <c r="G8" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -16114,7 +16105,7 @@
       </c>
       <c r="F9" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3MD#0002</v>
+        <v>EUR_YC3MRH_3MD#0005</v>
       </c>
       <c r="G9" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -16233,7 +16224,7 @@
       </c>
       <c r="H3" s="152" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_T3F1#0002</v>
+        <v>EUR_YC3MRH_T3F1#0005</v>
       </c>
       <c r="I3" s="151" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -16267,7 +16258,7 @@
       </c>
       <c r="H4" s="144" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_TOM3F1#0002</v>
+        <v>EUR_YC3MRH_TOM3F1#0005</v>
       </c>
       <c r="I4" s="150" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -16302,7 +16293,7 @@
       </c>
       <c r="H5" s="147" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1x4F#0002</v>
+        <v>EUR_YC3MRH_1x4F#0005</v>
       </c>
       <c r="I5" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -16337,7 +16328,7 @@
       </c>
       <c r="H6" s="147" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2x5F#0002</v>
+        <v>EUR_YC3MRH_2x5F#0005</v>
       </c>
       <c r="I6" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -16372,7 +16363,7 @@
       </c>
       <c r="H7" s="147" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3x6F#0002</v>
+        <v>EUR_YC3MRH_3x6F#0005</v>
       </c>
       <c r="I7" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -16407,7 +16398,7 @@
       </c>
       <c r="H8" s="147" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_4x7F#0002</v>
+        <v>EUR_YC3MRH_4x7F#0005</v>
       </c>
       <c r="I8" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -16442,7 +16433,7 @@
       </c>
       <c r="H9" s="147" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_5x8F#0002</v>
+        <v>EUR_YC3MRH_5x8F#0005</v>
       </c>
       <c r="I9" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -16477,7 +16468,7 @@
       </c>
       <c r="H10" s="144" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_6x9F#0002</v>
+        <v>EUR_YC3MRH_6x9F#0005</v>
       </c>
       <c r="I10" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -16616,7 +16607,7 @@
       </c>
       <c r="I3" s="174" t="str">
         <f>_xll.qlFuturesRateHelper(H3,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MF4#0002</v>
+        <v>EUR_YC3MRH_FUT3MF4#0005</v>
       </c>
       <c r="J3" s="173" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -16654,7 +16645,7 @@
       </c>
       <c r="I4" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H4,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MG4#0002</v>
+        <v>EUR_YC3MRH_FUT3MG4#0005</v>
       </c>
       <c r="J4" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -16692,7 +16683,7 @@
       </c>
       <c r="I5" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H5,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH4#0002</v>
+        <v>EUR_YC3MRH_FUT3MH4#0005</v>
       </c>
       <c r="J5" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -16730,7 +16721,7 @@
       </c>
       <c r="I6" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H6,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MJ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MJ4#0005</v>
       </c>
       <c r="J6" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -16768,7 +16759,7 @@
       </c>
       <c r="I7" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H7,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MK4#0002</v>
+        <v>EUR_YC3MRH_FUT3MK4#0005</v>
       </c>
       <c r="J7" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -16806,7 +16797,7 @@
       </c>
       <c r="I8" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H8,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM4#0002</v>
+        <v>EUR_YC3MRH_FUT3MM4#0005</v>
       </c>
       <c r="J8" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -16844,7 +16835,7 @@
       </c>
       <c r="I9" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H9,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MN4#0002</v>
+        <v>EUR_YC3MRH_FUT3MN4#0005</v>
       </c>
       <c r="J9" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -16882,7 +16873,7 @@
       </c>
       <c r="I10" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H10,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MQ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MQ4#0005</v>
       </c>
       <c r="J10" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -16920,7 +16911,7 @@
       </c>
       <c r="I11" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H11,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU4#0002</v>
+        <v>EUR_YC3MRH_FUT3MU4#0005</v>
       </c>
       <c r="J11" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -16958,7 +16949,7 @@
       </c>
       <c r="I12" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H12,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MV4#0002</v>
+        <v>EUR_YC3MRH_FUT3MV4#0005</v>
       </c>
       <c r="J12" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -16996,7 +16987,7 @@
       </c>
       <c r="I13" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H13,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MX4#0002</v>
+        <v>EUR_YC3MRH_FUT3MX4#0005</v>
       </c>
       <c r="J13" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -17034,7 +17025,7 @@
       </c>
       <c r="I14" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H14,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ4#0005</v>
       </c>
       <c r="J14" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -17148,7 +17139,7 @@
       </c>
       <c r="I17" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H17,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH5#0002</v>
+        <v>EUR_YC3MRH_FUT3MH5#0005</v>
       </c>
       <c r="J17" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -17262,7 +17253,7 @@
       </c>
       <c r="I20" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H20,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM5#0002</v>
+        <v>EUR_YC3MRH_FUT3MM5#0005</v>
       </c>
       <c r="J20" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -17376,7 +17367,7 @@
       </c>
       <c r="I23" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H23,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU5#0002</v>
+        <v>EUR_YC3MRH_FUT3MU5#0005</v>
       </c>
       <c r="J23" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
@@ -17490,7 +17481,7 @@
       </c>
       <c r="I26" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H26,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ5#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ5#0005</v>
       </c>
       <c r="J26" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
@@ -17604,7 +17595,7 @@
       </c>
       <c r="I29" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H29,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH6#0002</v>
+        <v>EUR_YC3MRH_FUT3MH6#0005</v>
       </c>
       <c r="J29" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
@@ -17718,7 +17709,7 @@
       </c>
       <c r="I32" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H32,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM6#0002</v>
+        <v>EUR_YC3MRH_FUT3MM6#0005</v>
       </c>
       <c r="J32" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
@@ -17832,7 +17823,7 @@
       </c>
       <c r="I35" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H35,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU6#0002</v>
+        <v>EUR_YC3MRH_FUT3MU6#0005</v>
       </c>
       <c r="J35" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
@@ -17946,7 +17937,7 @@
       </c>
       <c r="I38" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H38,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ6#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ6#0005</v>
       </c>
       <c r="J38" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
@@ -18059,7 +18050,7 @@
       </c>
       <c r="I41" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H41,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH7#0002</v>
+        <v>EUR_YC3MRH_FUT3MH7#0005</v>
       </c>
       <c r="J41" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
@@ -18170,7 +18161,7 @@
       </c>
       <c r="I44" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H44,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM7#0002</v>
+        <v>EUR_YC3MRH_FUT3MM7#0005</v>
       </c>
       <c r="J44" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I44)</f>
@@ -18281,7 +18272,7 @@
       </c>
       <c r="I47" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H47,$F47,$D47,$E47,$G47,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU7#0002</v>
+        <v>EUR_YC3MRH_FUT3MU7#0005</v>
       </c>
       <c r="J47" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I47)</f>
@@ -18392,7 +18383,7 @@
       </c>
       <c r="I50" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H50,$F50,$D50,$E50,$G50,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ7#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ7#0005</v>
       </c>
       <c r="J50" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I50)</f>
@@ -18503,7 +18494,7 @@
       </c>
       <c r="I53" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H53,$F53,$D53,$E53,$G53,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH8#0002</v>
+        <v>EUR_YC3MRH_FUT3MH8#0005</v>
       </c>
       <c r="J53" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I53)</f>
@@ -18614,7 +18605,7 @@
       </c>
       <c r="I56" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H56,$F56,$D56,$E56,$G56,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM8#0002</v>
+        <v>EUR_YC3MRH_FUT3MM8#0005</v>
       </c>
       <c r="J56" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I56)</f>
@@ -18725,7 +18716,7 @@
       </c>
       <c r="I59" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H59,$F59,$D59,$E59,$G59,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU8#0002</v>
+        <v>EUR_YC3MRH_FUT3MU8#0005</v>
       </c>
       <c r="J59" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I59)</f>
@@ -18836,7 +18827,7 @@
       </c>
       <c r="I62" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H62,$F62,$D62,$E62,$G62,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ8#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ8#0005</v>
       </c>
       <c r="J62" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I62)</f>
@@ -18947,7 +18938,7 @@
       </c>
       <c r="I65" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H65,$F65,$D65,$E65,$G65,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH9#0002</v>
+        <v>EUR_YC3MRH_FUT3MH9#0005</v>
       </c>
       <c r="J65" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I65)</f>
@@ -19058,7 +19049,7 @@
       </c>
       <c r="I68" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H68,$F68,$D68,$E68,$G68,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM9#0002</v>
+        <v>EUR_YC3MRH_FUT3MM9#0005</v>
       </c>
       <c r="J68" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I68)</f>
@@ -19169,7 +19160,7 @@
       </c>
       <c r="I71" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H71,$F71,$D71,$E71,$G71,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU9#0002</v>
+        <v>EUR_YC3MRH_FUT3MU9#0005</v>
       </c>
       <c r="J71" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I71)</f>
@@ -19280,7 +19271,7 @@
       </c>
       <c r="I74" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H74,$F74,$D74,$E74,$G74,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ9#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ9#0005</v>
       </c>
       <c r="J74" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I74)</f>
@@ -19391,7 +19382,7 @@
       </c>
       <c r="I77" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H77,$F77,$D77,$E77,$G77,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH0#0002</v>
+        <v>EUR_YC3MRH_FUT3MH0#0005</v>
       </c>
       <c r="J77" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I77)</f>
@@ -19502,7 +19493,7 @@
       </c>
       <c r="I80" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H80,$F80,$D80,$E80,$G80,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM0#0002</v>
+        <v>EUR_YC3MRH_FUT3MM0#0005</v>
       </c>
       <c r="J80" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I80)</f>
@@ -19613,7 +19604,7 @@
       </c>
       <c r="I83" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H83,$F83,$D83,$E83,$G83,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU0#0002</v>
+        <v>EUR_YC3MRH_FUT3MU0#0005</v>
       </c>
       <c r="J83" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I83)</f>
@@ -19724,7 +19715,7 @@
       </c>
       <c r="I86" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H86,$F86,$D86,$E86,$G86,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ0#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ0#0005</v>
       </c>
       <c r="J86" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I86)</f>
@@ -19835,7 +19826,7 @@
       </c>
       <c r="I89" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H89,$F89,$D89,$E89,$G89,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH1#0002</v>
+        <v>EUR_YC3MRH_FUT3MH1#0005</v>
       </c>
       <c r="J89" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I89)</f>
@@ -19946,7 +19937,7 @@
       </c>
       <c r="I92" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H92,$F92,$D92,$E92,$G92,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM1#0002</v>
+        <v>EUR_YC3MRH_FUT3MM1#0005</v>
       </c>
       <c r="J92" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I92)</f>
@@ -20057,7 +20048,7 @@
       </c>
       <c r="I95" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H95,$F95,$D95,$E95,$G95,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU1#0002</v>
+        <v>EUR_YC3MRH_FUT3MU1#0005</v>
       </c>
       <c r="J95" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I95)</f>
@@ -20168,7 +20159,7 @@
       </c>
       <c r="I98" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H98,$F98,$D98,$E98,$G98,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ1#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ1#0005</v>
       </c>
       <c r="J98" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I98)</f>
@@ -20279,7 +20270,7 @@
       </c>
       <c r="I101" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H101,$F101,$D101,$E101,$G101,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH2#0002</v>
+        <v>EUR_YC3MRH_FUT3MH2#0005</v>
       </c>
       <c r="J101" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I101)</f>
@@ -20390,7 +20381,7 @@
       </c>
       <c r="I104" s="167" t="str">
         <f>_xll.qlFuturesRateHelper(H104,$F104,$D104,$E104,$G104,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM2#0002</v>
+        <v>EUR_YC3MRH_FUT3MM2#0005</v>
       </c>
       <c r="J104" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(I104)</f>
@@ -21210,7 +21201,7 @@
       </c>
       <c r="L4" s="204" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC3MRH_AB3E_ibor3M#0002</v>
+        <v>EUR_YC3MRH_AB3E_ibor3M#0005</v>
       </c>
       <c r="M4" s="203" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -21274,7 +21265,7 @@
       </c>
       <c r="L6" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E1Y#0002</v>
+        <v>EUR_YC3MRH_AB3E1Y#0005</v>
       </c>
       <c r="M6" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -21329,7 +21320,7 @@
       </c>
       <c r="L7" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E15M#0002</v>
+        <v>EUR_YC3MRH_AB3E15M#0005</v>
       </c>
       <c r="M7" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -21384,7 +21375,7 @@
       </c>
       <c r="L8" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E18M#0002</v>
+        <v>EUR_YC3MRH_AB3E18M#0005</v>
       </c>
       <c r="M8" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -21439,7 +21430,7 @@
       </c>
       <c r="L9" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E21M#0002</v>
+        <v>EUR_YC3MRH_AB3E21M#0005</v>
       </c>
       <c r="M9" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -21494,7 +21485,7 @@
       </c>
       <c r="L10" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E2Y#0002</v>
+        <v>EUR_YC3MRH_AB3E2Y#0005</v>
       </c>
       <c r="M10" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -21549,7 +21540,7 @@
       </c>
       <c r="L11" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E3Y#0002</v>
+        <v>EUR_YC3MRH_AB3E3Y#0005</v>
       </c>
       <c r="M11" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -21595,7 +21586,7 @@
       </c>
       <c r="L12" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E4Y#0002</v>
+        <v>EUR_YC3MRH_AB3E4Y#0005</v>
       </c>
       <c r="M12" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -21641,7 +21632,7 @@
       </c>
       <c r="L13" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E5Y#0002</v>
+        <v>EUR_YC3MRH_AB3E5Y#0005</v>
       </c>
       <c r="M13" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -21687,7 +21678,7 @@
       </c>
       <c r="L14" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E6Y#0002</v>
+        <v>EUR_YC3MRH_AB3E6Y#0005</v>
       </c>
       <c r="M14" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -21733,7 +21724,7 @@
       </c>
       <c r="L15" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E7Y#0002</v>
+        <v>EUR_YC3MRH_AB3E7Y#0005</v>
       </c>
       <c r="M15" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -21779,7 +21770,7 @@
       </c>
       <c r="L16" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E8Y#0002</v>
+        <v>EUR_YC3MRH_AB3E8Y#0005</v>
       </c>
       <c r="M16" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -21825,7 +21816,7 @@
       </c>
       <c r="L17" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E9Y#0002</v>
+        <v>EUR_YC3MRH_AB3E9Y#0005</v>
       </c>
       <c r="M17" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -21871,7 +21862,7 @@
       </c>
       <c r="L18" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E10Y#0002</v>
+        <v>EUR_YC3MRH_AB3E10Y#0005</v>
       </c>
       <c r="M18" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -21917,7 +21908,7 @@
       </c>
       <c r="L19" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E11Y#0002</v>
+        <v>EUR_YC3MRH_AB3E11Y#0005</v>
       </c>
       <c r="M19" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -21963,7 +21954,7 @@
       </c>
       <c r="L20" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E12Y#0002</v>
+        <v>EUR_YC3MRH_AB3E12Y#0005</v>
       </c>
       <c r="M20" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -22009,7 +22000,7 @@
       </c>
       <c r="L21" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E13Y#0002</v>
+        <v>EUR_YC3MRH_AB3E13Y#0005</v>
       </c>
       <c r="M21" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -22055,7 +22046,7 @@
       </c>
       <c r="L22" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E14Y#0002</v>
+        <v>EUR_YC3MRH_AB3E14Y#0005</v>
       </c>
       <c r="M22" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -22101,7 +22092,7 @@
       </c>
       <c r="L23" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E15Y#0002</v>
+        <v>EUR_YC3MRH_AB3E15Y#0005</v>
       </c>
       <c r="M23" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -22147,7 +22138,7 @@
       </c>
       <c r="L24" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E16Y#0002</v>
+        <v>EUR_YC3MRH_AB3E16Y#0005</v>
       </c>
       <c r="M24" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -22193,7 +22184,7 @@
       </c>
       <c r="L25" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E17Y#0002</v>
+        <v>EUR_YC3MRH_AB3E17Y#0005</v>
       </c>
       <c r="M25" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -22239,7 +22230,7 @@
       </c>
       <c r="L26" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E18Y#0002</v>
+        <v>EUR_YC3MRH_AB3E18Y#0005</v>
       </c>
       <c r="M26" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -22285,7 +22276,7 @@
       </c>
       <c r="L27" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E19Y#0002</v>
+        <v>EUR_YC3MRH_AB3E19Y#0005</v>
       </c>
       <c r="M27" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -22331,7 +22322,7 @@
       </c>
       <c r="L28" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E20Y#0002</v>
+        <v>EUR_YC3MRH_AB3E20Y#0005</v>
       </c>
       <c r="M28" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -22377,7 +22368,7 @@
       </c>
       <c r="L29" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E21Y#0002</v>
+        <v>EUR_YC3MRH_AB3E21Y#0005</v>
       </c>
       <c r="M29" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -22423,7 +22414,7 @@
       </c>
       <c r="L30" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E22Y#0002</v>
+        <v>EUR_YC3MRH_AB3E22Y#0005</v>
       </c>
       <c r="M30" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -22469,7 +22460,7 @@
       </c>
       <c r="L31" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E23Y#0002</v>
+        <v>EUR_YC3MRH_AB3E23Y#0005</v>
       </c>
       <c r="M31" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -22515,7 +22506,7 @@
       </c>
       <c r="L32" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E24Y#0002</v>
+        <v>EUR_YC3MRH_AB3E24Y#0005</v>
       </c>
       <c r="M32" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -22561,7 +22552,7 @@
       </c>
       <c r="L33" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E25Y#0002</v>
+        <v>EUR_YC3MRH_AB3E25Y#0005</v>
       </c>
       <c r="M33" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -22607,7 +22598,7 @@
       </c>
       <c r="L34" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E26Y#0002</v>
+        <v>EUR_YC3MRH_AB3E26Y#0005</v>
       </c>
       <c r="M34" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -22653,7 +22644,7 @@
       </c>
       <c r="L35" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E27Y#0002</v>
+        <v>EUR_YC3MRH_AB3E27Y#0005</v>
       </c>
       <c r="M35" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -22699,7 +22690,7 @@
       </c>
       <c r="L36" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E28Y#0002</v>
+        <v>EUR_YC3MRH_AB3E28Y#0005</v>
       </c>
       <c r="M36" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -22745,7 +22736,7 @@
       </c>
       <c r="L37" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E29Y#0002</v>
+        <v>EUR_YC3MRH_AB3E29Y#0005</v>
       </c>
       <c r="M37" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -22791,7 +22782,7 @@
       </c>
       <c r="L38" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E30Y#0002</v>
+        <v>EUR_YC3MRH_AB3E30Y#0005</v>
       </c>
       <c r="M38" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -22837,7 +22828,7 @@
       </c>
       <c r="L39" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E35Y#0002</v>
+        <v>EUR_YC3MRH_AB3E35Y#0005</v>
       </c>
       <c r="M39" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -22883,7 +22874,7 @@
       </c>
       <c r="L40" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E40Y#0002</v>
+        <v>EUR_YC3MRH_AB3E40Y#0005</v>
       </c>
       <c r="M40" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -22929,7 +22920,7 @@
       </c>
       <c r="L41" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E50Y#0002</v>
+        <v>EUR_YC3MRH_AB3E50Y#0005</v>
       </c>
       <c r="M41" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -22975,7 +22966,7 @@
       </c>
       <c r="L42" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E60Y#0002</v>
+        <v>EUR_YC3MRH_AB3E60Y#0005</v>
       </c>
       <c r="M42" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -23033,7 +23024,7 @@
       </c>
       <c r="L44" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S12#0002</v>
+        <v>EUR_YC3MRH_1S12#0005</v>
       </c>
       <c r="M44" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -23078,7 +23069,7 @@
       </c>
       <c r="L45" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2S12#0002</v>
+        <v>EUR_YC3MRH_2S12#0005</v>
       </c>
       <c r="M45" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -23123,7 +23114,7 @@
       </c>
       <c r="L46" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3S12#0002</v>
+        <v>EUR_YC3MRH_3S12#0005</v>
       </c>
       <c r="M46" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -23168,7 +23159,7 @@
       </c>
       <c r="L47" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_4S12#0002</v>
+        <v>EUR_YC3MRH_4S12#0005</v>
       </c>
       <c r="M47" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -23213,7 +23204,7 @@
       </c>
       <c r="L48" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S24#0002</v>
+        <v>EUR_YC3MRH_1S24#0005</v>
       </c>
       <c r="M48" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -23258,7 +23249,7 @@
       </c>
       <c r="L49" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2S24#0002</v>
+        <v>EUR_YC3MRH_2S24#0005</v>
       </c>
       <c r="M49" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -23303,7 +23294,7 @@
       </c>
       <c r="L50" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S36#0002</v>
+        <v>EUR_YC3MRH_1S36#0005</v>
       </c>
       <c r="M50" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -23477,7 +23468,7 @@
       </c>
       <c r="L4" s="204" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC3MRH_AB3EBASIS_ibor3M#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS_ibor3M#0005</v>
       </c>
       <c r="M4" s="203" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -23541,7 +23532,7 @@
       </c>
       <c r="L6" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS1Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS1Y#0004</v>
       </c>
       <c r="M6" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -23590,7 +23581,7 @@
       </c>
       <c r="L7" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS15M#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS15M#0004</v>
       </c>
       <c r="M7" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -23639,7 +23630,7 @@
       </c>
       <c r="L8" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS18M#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS18M#0004</v>
       </c>
       <c r="M8" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -23688,7 +23679,7 @@
       </c>
       <c r="L9" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS21M#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS21M#0004</v>
       </c>
       <c r="M9" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -23737,7 +23728,7 @@
       </c>
       <c r="L10" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS2Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS2Y#0004</v>
       </c>
       <c r="M10" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -23795,7 +23786,7 @@
       </c>
       <c r="L11" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS3Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS3Y#0004</v>
       </c>
       <c r="M11" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -23853,7 +23844,7 @@
       </c>
       <c r="L12" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS4Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS4Y#0004</v>
       </c>
       <c r="M12" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -23911,7 +23902,7 @@
       </c>
       <c r="L13" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS5Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS5Y#0004</v>
       </c>
       <c r="M13" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -23969,7 +23960,7 @@
       </c>
       <c r="L14" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS6Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS6Y#0004</v>
       </c>
       <c r="M14" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -24027,7 +24018,7 @@
       </c>
       <c r="L15" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS7Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS7Y#0004</v>
       </c>
       <c r="M15" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -24079,7 +24070,7 @@
       </c>
       <c r="L16" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS8Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS8Y#0004</v>
       </c>
       <c r="M16" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -24128,7 +24119,7 @@
       </c>
       <c r="L17" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS9Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS9Y#0004</v>
       </c>
       <c r="M17" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -24177,7 +24168,7 @@
       </c>
       <c r="L18" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS10Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS10Y#0004</v>
       </c>
       <c r="M18" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -24226,7 +24217,7 @@
       </c>
       <c r="L19" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS11Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS11Y#0004</v>
       </c>
       <c r="M19" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -24275,7 +24266,7 @@
       </c>
       <c r="L20" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS12Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS12Y#0004</v>
       </c>
       <c r="M20" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -24324,7 +24315,7 @@
       </c>
       <c r="L21" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS13Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS13Y#0004</v>
       </c>
       <c r="M21" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -24373,7 +24364,7 @@
       </c>
       <c r="L22" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS14Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS14Y#0004</v>
       </c>
       <c r="M22" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -24422,7 +24413,7 @@
       </c>
       <c r="L23" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS15Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS15Y#0004</v>
       </c>
       <c r="M23" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -24471,7 +24462,7 @@
       </c>
       <c r="L24" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS16Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS16Y#0004</v>
       </c>
       <c r="M24" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -24520,7 +24511,7 @@
       </c>
       <c r="L25" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS17Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS17Y#0004</v>
       </c>
       <c r="M25" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -24569,7 +24560,7 @@
       </c>
       <c r="L26" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS18Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS18Y#0004</v>
       </c>
       <c r="M26" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -24618,7 +24609,7 @@
       </c>
       <c r="L27" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS19Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS19Y#0004</v>
       </c>
       <c r="M27" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -24667,7 +24658,7 @@
       </c>
       <c r="L28" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS20Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS20Y#0004</v>
       </c>
       <c r="M28" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -24716,7 +24707,7 @@
       </c>
       <c r="L29" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS21Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS21Y#0004</v>
       </c>
       <c r="M29" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -24765,7 +24756,7 @@
       </c>
       <c r="L30" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS22Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS22Y#0004</v>
       </c>
       <c r="M30" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -24814,7 +24805,7 @@
       </c>
       <c r="L31" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS23Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS23Y#0004</v>
       </c>
       <c r="M31" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -24863,7 +24854,7 @@
       </c>
       <c r="L32" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS24Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS24Y#0004</v>
       </c>
       <c r="M32" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -24912,7 +24903,7 @@
       </c>
       <c r="L33" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS25Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS25Y#0004</v>
       </c>
       <c r="M33" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -24961,7 +24952,7 @@
       </c>
       <c r="L34" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS26Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS26Y#0004</v>
       </c>
       <c r="M34" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -25010,7 +25001,7 @@
       </c>
       <c r="L35" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS27Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS27Y#0004</v>
       </c>
       <c r="M35" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -25059,7 +25050,7 @@
       </c>
       <c r="L36" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS28Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS28Y#0004</v>
       </c>
       <c r="M36" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -25108,7 +25099,7 @@
       </c>
       <c r="L37" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS29Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS29Y#0004</v>
       </c>
       <c r="M37" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -25157,7 +25148,7 @@
       </c>
       <c r="L38" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS30Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS30Y#0004</v>
       </c>
       <c r="M38" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -25206,7 +25197,7 @@
       </c>
       <c r="L39" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS35Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS35Y#0004</v>
       </c>
       <c r="M39" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -25255,7 +25246,7 @@
       </c>
       <c r="L40" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS40Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS40Y#0004</v>
       </c>
       <c r="M40" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -25304,7 +25295,7 @@
       </c>
       <c r="L41" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS50Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS50Y#0004</v>
       </c>
       <c r="M41" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -25353,7 +25344,7 @@
       </c>
       <c r="L42" s="187" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS60Y#0001</v>
+        <v>EUR_YC3MRH_AB3EBASIS60Y#0004</v>
       </c>
       <c r="M42" s="186" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>

<commit_message>
EURYC3M - reconcile with R010202 prod
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YC3MBootstrapping.xlsx
@@ -787,7 +787,7 @@
     <t>EUR_YCRH_SwapsFromBasis</t>
   </si>
   <si>
-    <t>EUR_YC3MRH_FUT3MZ3</t>
+    <t>EUR_YC3MRH_FUT3MZ5</t>
   </si>
 </sst>
 </file>
@@ -2484,7 +2484,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="84">
-        <v>41663.489872685182</v>
+        <v>41663.495694444442</v>
       </c>
       <c r="E11" s="56"/>
       <c r="F11" s="55"/>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="D14" s="81" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYC3M#0002</v>
+        <v>_EURYC3M#0008</v>
       </c>
       <c r="E14" s="56"/>
       <c r="F14" s="55"/>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="D28" s="60">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.2024386808921399</v>
+        <v>0.19313772797651729</v>
       </c>
       <c r="E28" s="56"/>
       <c r="F28" s="55"/>
@@ -2804,7 +2804,7 @@
   <dimension ref="A1:N169"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="E4" s="34" t="str">
         <f>Deposits_3M!F3</f>
-        <v>EUR_YC3MRH_SND#0002</v>
+        <v>EUR_YC3MRH_SND#0007</v>
       </c>
       <c r="F4" s="33">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="E5" s="34" t="str">
         <f>Deposits_3M!F4</f>
-        <v>EUR_YC3MRH_SWD#0002</v>
+        <v>EUR_YC3MRH_SWD#0007</v>
       </c>
       <c r="F5" s="33">
         <f>_xll.qlRateHelperQuoteValue($E5,Trigger)</f>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="E6" s="34" t="str">
         <f>Deposits_3M!F5</f>
-        <v>EUR_YC3MRH_2WD#0002</v>
+        <v>EUR_YC3MRH_2WD#0007</v>
       </c>
       <c r="F6" s="33">
         <f>_xll.qlRateHelperQuoteValue($E6,Trigger)</f>
@@ -3061,7 +3061,7 @@
       </c>
       <c r="E7" s="34" t="str">
         <f>Deposits_3M!F6</f>
-        <v>EUR_YC3MRH_3WD#0002</v>
+        <v>EUR_YC3MRH_3WD#0007</v>
       </c>
       <c r="F7" s="33">
         <f>_xll.qlRateHelperQuoteValue($E7,Trigger)</f>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="E8" s="34" t="str">
         <f>Deposits_3M!F7</f>
-        <v>EUR_YC3MRH_1MD#0002</v>
+        <v>EUR_YC3MRH_1MD#0007</v>
       </c>
       <c r="F8" s="33">
         <f>_xll.qlRateHelperQuoteValue($E8,Trigger)</f>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="E9" s="34" t="str">
         <f>Deposits_3M!F8</f>
-        <v>EUR_YC3MRH_2MD#0002</v>
+        <v>EUR_YC3MRH_2MD#0007</v>
       </c>
       <c r="F9" s="33">
         <f>_xll.qlRateHelperQuoteValue($E9,Trigger)</f>
@@ -3172,7 +3172,7 @@
       </c>
       <c r="E10" s="34" t="str">
         <f>Deposits_3M!F9</f>
-        <v>EUR_YC3MRH_3MD#0002</v>
+        <v>EUR_YC3MRH_3MD#0007</v>
       </c>
       <c r="F10" s="33">
         <f>_xll.qlRateHelperQuoteValue($E10,Trigger)</f>
@@ -3378,11 +3378,11 @@
       </c>
       <c r="E16" s="42" t="str">
         <f>FRAs_3M!H3</f>
-        <v>EUR_YC3MRH_T3F1#0002</v>
-      </c>
-      <c r="F16" s="41">
+        <v>EUR_YC3MRH_T3F1#0007</v>
+      </c>
+      <c r="F16" s="41" t="e">
         <f>_xll.qlRateHelperQuoteValue($E16,Trigger)</f>
-        <v>2.2500000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="40" t="b">
@@ -3416,15 +3416,15 @@
       </c>
       <c r="E17" s="27" t="str">
         <f>FRAs_3M!H4</f>
-        <v>EUR_YC3MRH_TOM3F1#0002</v>
-      </c>
-      <c r="F17" s="26">
+        <v>EUR_YC3MRH_TOM3F1#0007</v>
+      </c>
+      <c r="F17" s="26" t="e">
         <f>_xll.qlRateHelperQuoteValue($E17,Trigger)</f>
-        <v>2.2500000000000003E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="25">
         <v>20</v>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="F18" s="33">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>2.4499999999999999E-3</v>
+        <v>3.0599999999999998E-3</v>
       </c>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="b">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="F19" s="33">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>2.6800000000000001E-3</v>
+        <v>2.97E-3</v>
       </c>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="b">
@@ -3534,7 +3534,7 @@
       </c>
       <c r="F20" s="33">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>2.9400000000000003E-3</v>
+        <v>2.9399999999999999E-3</v>
       </c>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="b">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="F21" s="33">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
-        <v>3.1099999999999999E-3</v>
+        <v>2.9199999999999999E-3</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="b">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="F22" s="33">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>3.3199999999999996E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="b">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="F23" s="33">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
-        <v>3.5199999999999997E-3</v>
+        <v>2.9199999999999999E-3</v>
       </c>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="b">
@@ -4140,11 +4140,11 @@
       </c>
       <c r="E36" s="34" t="str">
         <f>Futures_3M!I3</f>
-        <v>EUR_YC3MRH_FUT3MG4#0002</v>
+        <v>EUR_YC3MRH_FUT3MG4#0007</v>
       </c>
       <c r="F36" s="48">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
-        <v>99.767499999999998</v>
+        <v>99.694999999999993</v>
       </c>
       <c r="G36" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E36,Trigger)</f>
@@ -4182,11 +4182,11 @@
       </c>
       <c r="E37" s="34" t="str">
         <f>Futures_3M!I4</f>
-        <v>EUR_YC3MRH_FUT3MH4#0002</v>
+        <v>EUR_YC3MRH_FUT3MH4#0007</v>
       </c>
       <c r="F37" s="48">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
-        <v>99.737499999999997</v>
+        <v>99.702500000000001</v>
       </c>
       <c r="G37" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E37,Trigger)</f>
@@ -4224,11 +4224,11 @@
       </c>
       <c r="E38" s="34" t="str">
         <f>Futures_3M!I5</f>
-        <v>EUR_YC3MRH_FUT3MJ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MJ4#0007</v>
       </c>
       <c r="F38" s="48">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
-        <v>99.715000000000003</v>
+        <v>99.704999999999998</v>
       </c>
       <c r="G38" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E38,Trigger)</f>
@@ -4266,7 +4266,7 @@
       </c>
       <c r="E39" s="34" t="str">
         <f>Futures_3M!I6</f>
-        <v>EUR_YC3MRH_FUT3MK4#0002</v>
+        <v>EUR_YC3MRH_FUT3MK4#0007</v>
       </c>
       <c r="F39" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
@@ -4308,11 +4308,11 @@
       </c>
       <c r="E40" s="34" t="str">
         <f>Futures_3M!I7</f>
-        <v>EUR_YC3MRH_FUT3MM4#0002</v>
+        <v>EUR_YC3MRH_FUT3MM4#0007</v>
       </c>
       <c r="F40" s="48">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
-        <v>99.677499999999995</v>
+        <v>99.707499999999996</v>
       </c>
       <c r="G40" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E40,Trigger)</f>
@@ -4350,15 +4350,15 @@
       </c>
       <c r="E41" s="34" t="str">
         <f>Futures_3M!I8</f>
-        <v>EUR_YC3MRH_FUT3MN4#0002</v>
-      </c>
-      <c r="F41" s="48">
+        <v>EUR_YC3MRH_FUT3MN4#0007</v>
+      </c>
+      <c r="F41" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
-        <v>99.547499999999999</v>
-      </c>
-      <c r="G41" s="33">
+        <v>#NUM!</v>
+      </c>
+      <c r="G41" s="33" t="e">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E41,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="H41" s="32" t="b">
         <v>1</v>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="E42" s="34" t="str">
         <f>Futures_3M!I9</f>
-        <v>EUR_YC3MRH_FUT3MQ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MQ4#0007</v>
       </c>
       <c r="F42" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -4434,11 +4434,11 @@
       </c>
       <c r="E43" s="34" t="str">
         <f>Futures_3M!I10</f>
-        <v>EUR_YC3MRH_FUT3MU4#0002</v>
+        <v>EUR_YC3MRH_FUT3MU4#0007</v>
       </c>
       <c r="F43" s="48">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
-        <v>99.607500000000002</v>
+        <v>99.702500000000001</v>
       </c>
       <c r="G43" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E43,Trigger)</f>
@@ -4476,15 +4476,15 @@
       </c>
       <c r="E44" s="34" t="str">
         <f>Futures_3M!I11</f>
-        <v>EUR_YC3MRH_FUT3MV4#0002</v>
-      </c>
-      <c r="F44" s="48">
+        <v>EUR_YC3MRH_FUT3MV4#0007</v>
+      </c>
+      <c r="F44" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
-        <v>99.487499999999997</v>
-      </c>
-      <c r="G44" s="33">
+        <v>#NUM!</v>
+      </c>
+      <c r="G44" s="33" t="e">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E44,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="H44" s="32" t="b">
         <v>1</v>
@@ -4518,7 +4518,7 @@
       </c>
       <c r="E45" s="34" t="str">
         <f>Futures_3M!I12</f>
-        <v>EUR_YC3MRH_FUT3MX4#0002</v>
+        <v>EUR_YC3MRH_FUT3MX4#0007</v>
       </c>
       <c r="F45" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -4560,11 +4560,11 @@
       </c>
       <c r="E46" s="34" t="str">
         <f>Futures_3M!I13</f>
-        <v>EUR_YC3MRH_FUT3MZ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ4#0007</v>
       </c>
       <c r="F46" s="48">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
-        <v>99.547499999999999</v>
+        <v>99.682500000000005</v>
       </c>
       <c r="G46" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E46,Trigger)</f>
@@ -4602,15 +4602,15 @@
       </c>
       <c r="E47" s="34" t="str">
         <f>Futures_3M!I14</f>
-        <v>EUR_YC3MRH_FUT3MF5#0002</v>
-      </c>
-      <c r="F47" s="48">
+        <v>EUR_YC3MRH_FUT3MF5#0007</v>
+      </c>
+      <c r="F47" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
-        <v>99.417500000000004</v>
-      </c>
-      <c r="G47" s="33">
+        <v>#NUM!</v>
+      </c>
+      <c r="G47" s="33" t="e">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E47,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="H47" s="32" t="b">
         <v>1</v>
@@ -4644,11 +4644,11 @@
       </c>
       <c r="E48" s="34" t="str">
         <f>Futures_3M!I15</f>
-        <v>EUR_YC3MRH_FUT3MH5#0002</v>
+        <v>EUR_YC3MRH_FUT3MH5#0007</v>
       </c>
       <c r="F48" s="48">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
-        <v>99.487499999999997</v>
+        <v>99.642499999999998</v>
       </c>
       <c r="G48" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E48,Trigger)</f>
@@ -4686,11 +4686,11 @@
       </c>
       <c r="E49" s="34" t="str">
         <f>Futures_3M!I16</f>
-        <v>EUR_YC3MRH_FUT3MM5#0002</v>
+        <v>EUR_YC3MRH_FUT3MM5#0007</v>
       </c>
       <c r="F49" s="48">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
-        <v>99.417500000000004</v>
+        <v>99.587500000000006</v>
       </c>
       <c r="G49" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E49,Trigger)</f>
@@ -4728,11 +4728,11 @@
       </c>
       <c r="E50" s="34" t="str">
         <f>Futures_3M!I17</f>
-        <v>EUR_YC3MRH_FUT3MU5#0002</v>
+        <v>EUR_YC3MRH_FUT3MU5#0007</v>
       </c>
       <c r="F50" s="48">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
-        <v>99.347499999999997</v>
+        <v>99.507499999999993</v>
       </c>
       <c r="G50" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E50,Trigger)</f>
@@ -4770,11 +4770,11 @@
       </c>
       <c r="E51" s="34" t="str">
         <f>Futures_3M!I18</f>
-        <v>EUR_YC3MRH_FUT3MZ5#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ5#0007</v>
       </c>
       <c r="F51" s="48">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
-        <v>99.267499999999998</v>
+        <v>99.412499999999994</v>
       </c>
       <c r="G51" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E51,Trigger)</f>
@@ -4812,11 +4812,11 @@
       </c>
       <c r="E52" s="34" t="str">
         <f>Futures_3M!I19</f>
-        <v>EUR_YC3MRH_FUT3MH6#0002</v>
+        <v>EUR_YC3MRH_FUT3MH6#0007</v>
       </c>
       <c r="F52" s="48">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
-        <v>99.182500000000005</v>
+        <v>99.292500000000004</v>
       </c>
       <c r="G52" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E52,Trigger)</f>
@@ -4854,11 +4854,11 @@
       </c>
       <c r="E53" s="34" t="str">
         <f>Futures_3M!I20</f>
-        <v>EUR_YC3MRH_FUT3MM6#0002</v>
+        <v>EUR_YC3MRH_FUT3MM6#0007</v>
       </c>
       <c r="F53" s="48">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
-        <v>99.075000000000003</v>
+        <v>99.16</v>
       </c>
       <c r="G53" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E53,Trigger)</f>
@@ -4896,11 +4896,11 @@
       </c>
       <c r="E54" s="34" t="str">
         <f>Futures_3M!I21</f>
-        <v>EUR_YC3MRH_FUT3MU6#0002</v>
+        <v>EUR_YC3MRH_FUT3MU6#0007</v>
       </c>
       <c r="F54" s="48">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
-        <v>98.95</v>
+        <v>99.007499999999993</v>
       </c>
       <c r="G54" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E54,Trigger)</f>
@@ -4938,11 +4938,11 @@
       </c>
       <c r="E55" s="34" t="str">
         <f>Futures_3M!I22</f>
-        <v>EUR_YC3MRH_FUT3MZ6#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ6#0007</v>
       </c>
       <c r="F55" s="48">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
-        <v>98.802499999999995</v>
+        <v>98.844999999999999</v>
       </c>
       <c r="G55" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E55,Trigger)</f>
@@ -4980,11 +4980,11 @@
       </c>
       <c r="E56" s="34" t="str">
         <f>Futures_3M!I23</f>
-        <v>EUR_YC3MRH_FUT3MH7#0002</v>
+        <v>EUR_YC3MRH_FUT3MH7#0007</v>
       </c>
       <c r="F56" s="48">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
-        <v>98.655000000000001</v>
+        <v>98.694999999999993</v>
       </c>
       <c r="G56" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E56,Trigger)</f>
@@ -5022,11 +5022,11 @@
       </c>
       <c r="E57" s="34" t="str">
         <f>Futures_3M!I24</f>
-        <v>EUR_YC3MRH_FUT3MM7#0002</v>
+        <v>EUR_YC3MRH_FUT3MM7#0007</v>
       </c>
       <c r="F57" s="48">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
-        <v>98.515000000000001</v>
+        <v>98.54</v>
       </c>
       <c r="G57" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E57,Trigger)</f>
@@ -5064,11 +5064,11 @@
       </c>
       <c r="E58" s="34" t="str">
         <f>Futures_3M!I25</f>
-        <v>EUR_YC3MRH_FUT3MU7#0002</v>
+        <v>EUR_YC3MRH_FUT3MU7#0007</v>
       </c>
       <c r="F58" s="48">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
-        <v>98.385000000000005</v>
+        <v>98.394999999999996</v>
       </c>
       <c r="G58" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E58,Trigger)</f>
@@ -5106,11 +5106,11 @@
       </c>
       <c r="E59" s="34" t="str">
         <f>Futures_3M!I26</f>
-        <v>EUR_YC3MRH_FUT3MZ7#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ7#0007</v>
       </c>
       <c r="F59" s="48">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
-        <v>98.25</v>
+        <v>98.257499999999993</v>
       </c>
       <c r="G59" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E59,Trigger)</f>
@@ -5148,11 +5148,11 @@
       </c>
       <c r="E60" s="34" t="str">
         <f>Futures_3M!I27</f>
-        <v>EUR_YC3MRH_FUT3MH8#0002</v>
+        <v>EUR_YC3MRH_FUT3MH8#0007</v>
       </c>
       <c r="F60" s="48">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
-        <v>98.125</v>
+        <v>98.142499999999998</v>
       </c>
       <c r="G60" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E60,Trigger)</f>
@@ -5190,11 +5190,11 @@
       </c>
       <c r="E61" s="34" t="str">
         <f>Futures_3M!I28</f>
-        <v>EUR_YC3MRH_FUT3MM8#0002</v>
+        <v>EUR_YC3MRH_FUT3MM8#0007</v>
       </c>
       <c r="F61" s="48">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
-        <v>98.01</v>
+        <v>98.025000000000006</v>
       </c>
       <c r="G61" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E61,Trigger)</f>
@@ -5232,11 +5232,11 @@
       </c>
       <c r="E62" s="34" t="str">
         <f>Futures_3M!I29</f>
-        <v>EUR_YC3MRH_FUT3MU8#0002</v>
+        <v>EUR_YC3MRH_FUT3MU8#0007</v>
       </c>
       <c r="F62" s="48">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
-        <v>97.922499999999999</v>
+        <v>97.915000000000006</v>
       </c>
       <c r="G62" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E62,Trigger)</f>
@@ -5274,11 +5274,11 @@
       </c>
       <c r="E63" s="34" t="str">
         <f>Futures_3M!I30</f>
-        <v>EUR_YC3MRH_FUT3MZ8#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ8#0007</v>
       </c>
       <c r="F63" s="48">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
-        <v>97.834999999999994</v>
+        <v>97.787499999999994</v>
       </c>
       <c r="G63" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E63,Trigger)</f>
@@ -5316,11 +5316,11 @@
       </c>
       <c r="E64" s="34" t="str">
         <f>Futures_3M!I31</f>
-        <v>EUR_YC3MRH_FUT3MH9#0002</v>
+        <v>EUR_YC3MRH_FUT3MH9#0007</v>
       </c>
       <c r="F64" s="48">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
-        <v>97.76</v>
+        <v>97.685000000000002</v>
       </c>
       <c r="G64" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E64,Trigger)</f>
@@ -5358,11 +5358,11 @@
       </c>
       <c r="E65" s="34" t="str">
         <f>Futures_3M!I32</f>
-        <v>EUR_YC3MRH_FUT3MM9#0002</v>
+        <v>EUR_YC3MRH_FUT3MM9#0007</v>
       </c>
       <c r="F65" s="48">
         <f>_xll.qlRateHelperQuoteValue($E65,Trigger)</f>
-        <v>97.672499999999999</v>
+        <v>97.58</v>
       </c>
       <c r="G65" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E65,Trigger)</f>
@@ -5400,15 +5400,15 @@
       </c>
       <c r="E66" s="34" t="str">
         <f>Futures_3M!I33</f>
-        <v>EUR_YC3MRH_FUT3MU9#0002</v>
-      </c>
-      <c r="F66" s="48" t="e">
+        <v>EUR_YC3MRH_FUT3MU9#0007</v>
+      </c>
+      <c r="F66" s="48">
         <f>_xll.qlRateHelperQuoteValue($E66,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G66" s="33" t="e">
+        <v>97.472499999999997</v>
+      </c>
+      <c r="G66" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E66,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="H66" s="32" t="b">
         <v>1</v>
@@ -5442,15 +5442,15 @@
       </c>
       <c r="E67" s="34" t="str">
         <f>Futures_3M!I34</f>
-        <v>EUR_YC3MRH_FUT3MZ9#0002</v>
-      </c>
-      <c r="F67" s="48" t="e">
+        <v>EUR_YC3MRH_FUT3MZ9#0007</v>
+      </c>
+      <c r="F67" s="48">
         <f>_xll.qlRateHelperQuoteValue($E67,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G67" s="33" t="e">
+        <v>97.39</v>
+      </c>
+      <c r="G67" s="33">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E67,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="H67" s="32" t="b">
         <v>1</v>
@@ -5484,7 +5484,7 @@
       </c>
       <c r="E68" s="34" t="str">
         <f>Futures_3M!I35</f>
-        <v>EUR_YC3MRH_FUT3MH0#0002</v>
+        <v>EUR_YC3MRH_FUT3MH0#0007</v>
       </c>
       <c r="F68" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E68,Trigger)</f>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="E69" s="34" t="str">
         <f>Futures_3M!I36</f>
-        <v>EUR_YC3MRH_FUT3MM0#0002</v>
+        <v>EUR_YC3MRH_FUT3MM0#0007</v>
       </c>
       <c r="F69" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E69,Trigger)</f>
@@ -5568,7 +5568,7 @@
       </c>
       <c r="E70" s="34" t="str">
         <f>Futures_3M!I37</f>
-        <v>EUR_YC3MRH_FUT3MU0#0002</v>
+        <v>EUR_YC3MRH_FUT3MU0#0007</v>
       </c>
       <c r="F70" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E70,Trigger)</f>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="E71" s="34" t="str">
         <f>Futures_3M!I38</f>
-        <v>EUR_YC3MRH_FUT3MZ0#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ0#0007</v>
       </c>
       <c r="F71" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="E72" s="34" t="str">
         <f>Futures_3M!I39</f>
-        <v>EUR_YC3MRH_FUT3MH1#0002</v>
+        <v>EUR_YC3MRH_FUT3MH1#0007</v>
       </c>
       <c r="F72" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E72,Trigger)</f>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="E73" s="34" t="str">
         <f>Futures_3M!I40</f>
-        <v>EUR_YC3MRH_FUT3MM1#0002</v>
+        <v>EUR_YC3MRH_FUT3MM1#0007</v>
       </c>
       <c r="F73" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E73,Trigger)</f>
@@ -5736,7 +5736,7 @@
       </c>
       <c r="E74" s="34" t="str">
         <f>Futures_3M!I41</f>
-        <v>EUR_YC3MRH_FUT3MU1#0002</v>
+        <v>EUR_YC3MRH_FUT3MU1#0007</v>
       </c>
       <c r="F74" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E74,Trigger)</f>
@@ -5778,7 +5778,7 @@
       </c>
       <c r="E75" s="34" t="str">
         <f>Futures_3M!I42</f>
-        <v>EUR_YC3MRH_FUT3MZ1#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ1#0007</v>
       </c>
       <c r="F75" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E75,Trigger)</f>
@@ -5820,7 +5820,7 @@
       </c>
       <c r="E76" s="34" t="str">
         <f>Futures_3M!I43</f>
-        <v>EUR_YC3MRH_FUT3MH2#0002</v>
+        <v>EUR_YC3MRH_FUT3MH2#0007</v>
       </c>
       <c r="F76" s="48" t="e">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="E77" s="27" t="str">
         <f>Futures_3M!I44</f>
-        <v>EUR_YC3MRH_FUT3MM2#0002</v>
+        <v>EUR_YC3MRH_FUT3MM2#0007</v>
       </c>
       <c r="F77" s="47" t="e">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
@@ -6591,11 +6591,11 @@
       </c>
       <c r="E96" s="34" t="str">
         <f>Swaps_3M!L6</f>
-        <v>EUR_YC3MRH_AB3E1Y#0002</v>
+        <v>EUR_YC3MRH_AB3E1Y#0007</v>
       </c>
       <c r="F96" s="33">
         <f>_xll.qlRateHelperQuoteValue($E96,Trigger)</f>
-        <v>3.2699999999999995E-3</v>
+        <v>3.0399999999999997E-3</v>
       </c>
       <c r="G96" s="33">
         <f>_xll.qlSwapRateHelperSpread($E96,Trigger)</f>
@@ -6620,7 +6620,7 @@
       </c>
       <c r="N96" s="37">
         <f t="shared" ref="N96:N132" si="7">IF(G96=G133,F96-F133,"--")</f>
-        <v>0</v>
+        <v>4.9999999999993626E-6</v>
       </c>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.2">
@@ -6637,11 +6637,11 @@
       </c>
       <c r="E97" s="34" t="str">
         <f>Swaps_3M!L7</f>
-        <v>EUR_YC3MRH_AB3E15M#0002</v>
+        <v>EUR_YC3MRH_AB3E15M#0007</v>
       </c>
       <c r="F97" s="33">
         <f>_xll.qlRateHelperQuoteValue($E97,Trigger)</f>
-        <v>3.5899999999999999E-3</v>
+        <v>3.0899999999999999E-3</v>
       </c>
       <c r="G97" s="33">
         <f>_xll.qlSwapRateHelperSpread($E97,Trigger)</f>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="N97" s="37">
         <f t="shared" si="7"/>
-        <v>1.4100000000000007E-4</v>
+        <v>2.3399999999999897E-4</v>
       </c>
     </row>
     <row r="98" spans="2:14" x14ac:dyDescent="0.2">
@@ -6683,11 +6683,11 @@
       </c>
       <c r="E98" s="34" t="str">
         <f>Swaps_3M!L8</f>
-        <v>EUR_YC3MRH_AB3E18M#0002</v>
+        <v>EUR_YC3MRH_AB3E18M#0007</v>
       </c>
       <c r="F98" s="33">
         <f>_xll.qlRateHelperQuoteValue($E98,Trigger)</f>
-        <v>3.9199999999999999E-3</v>
+        <v>3.2100000000000002E-3</v>
       </c>
       <c r="G98" s="33">
         <f>_xll.qlSwapRateHelperSpread($E98,Trigger)</f>
@@ -6712,7 +6712,7 @@
       </c>
       <c r="N98" s="37">
         <f t="shared" si="7"/>
-        <v>9.9999999999995925E-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:14" x14ac:dyDescent="0.2">
@@ -6729,11 +6729,11 @@
       </c>
       <c r="E99" s="34" t="str">
         <f>Swaps_3M!L9</f>
-        <v>EUR_YC3MRH_AB3E21M#0002</v>
+        <v>EUR_YC3MRH_AB3E21M#0007</v>
       </c>
       <c r="F99" s="33">
         <f>_xll.qlRateHelperQuoteValue($E99,Trigger)</f>
-        <v>4.2300000000000003E-3</v>
+        <v>3.4000000000000002E-3</v>
       </c>
       <c r="G99" s="33">
         <f>_xll.qlSwapRateHelperSpread($E99,Trigger)</f>
@@ -6758,7 +6758,7 @@
       </c>
       <c r="N99" s="37">
         <f t="shared" si="7"/>
-        <v>1.0999999999999985E-4</v>
+        <v>1.7300000000000041E-4</v>
       </c>
     </row>
     <row r="100" spans="2:14" x14ac:dyDescent="0.2">
@@ -6775,11 +6775,11 @@
       </c>
       <c r="E100" s="34" t="str">
         <f>Swaps_3M!L10</f>
-        <v>EUR_YC3MRH_AB3E2Y#0002</v>
+        <v>EUR_YC3MRH_AB3E2Y#0007</v>
       </c>
       <c r="F100" s="33">
         <f>_xll.qlRateHelperQuoteValue($E100,Trigger)</f>
-        <v>4.5699999999999994E-3</v>
+        <v>3.65E-3</v>
       </c>
       <c r="G100" s="33">
         <f>_xll.qlSwapRateHelperSpread($E100,Trigger)</f>
@@ -6804,7 +6804,7 @@
       </c>
       <c r="N100" s="37">
         <f t="shared" si="7"/>
-        <v>4.9999999999989289E-6</v>
+        <v>4.3368086899420177E-19</v>
       </c>
     </row>
     <row r="101" spans="2:14" x14ac:dyDescent="0.2">
@@ -6821,11 +6821,11 @@
       </c>
       <c r="E101" s="34" t="str">
         <f>Swaps_3M!L11</f>
-        <v>EUR_YC3MRH_AB3E3Y#0002</v>
+        <v>EUR_YC3MRH_AB3E3Y#0007</v>
       </c>
       <c r="F101" s="33">
         <f>_xll.qlRateHelperQuoteValue($E101,Trigger)</f>
-        <v>6.2100000000000002E-3</v>
+        <v>5.2700000000000004E-3</v>
       </c>
       <c r="G101" s="33">
         <f>_xll.qlSwapRateHelperSpread($E101,Trigger)</f>
@@ -6850,7 +6850,7 @@
       </c>
       <c r="N101" s="37">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.0000000000006636E-6</v>
       </c>
     </row>
     <row r="102" spans="2:14" x14ac:dyDescent="0.2">
@@ -6867,11 +6867,11 @@
       </c>
       <c r="E102" s="34" t="str">
         <f>Swaps_3M!L12</f>
-        <v>EUR_YC3MRH_AB3E4Y#0002</v>
+        <v>EUR_YC3MRH_AB3E4Y#0007</v>
       </c>
       <c r="F102" s="33">
         <f>_xll.qlRateHelperQuoteValue($E102,Trigger)</f>
-        <v>8.3800000000000003E-3</v>
+        <v>7.4900000000000001E-3</v>
       </c>
       <c r="G102" s="33">
         <f>_xll.qlSwapRateHelperSpread($E102,Trigger)</f>
@@ -6896,7 +6896,7 @@
       </c>
       <c r="N102" s="37">
         <f t="shared" si="7"/>
-        <v>4.9999999999997963E-6</v>
+        <v>8.6736173798840355E-19</v>
       </c>
     </row>
     <row r="103" spans="2:14" x14ac:dyDescent="0.2">
@@ -6913,11 +6913,11 @@
       </c>
       <c r="E103" s="34" t="str">
         <f>Swaps_3M!L13</f>
-        <v>EUR_YC3MRH_AB3E5Y#0002</v>
+        <v>EUR_YC3MRH_AB3E5Y#0007</v>
       </c>
       <c r="F103" s="33">
         <f>_xll.qlRateHelperQuoteValue($E103,Trigger)</f>
-        <v>1.065E-2</v>
+        <v>9.8099999999999993E-3</v>
       </c>
       <c r="G103" s="33">
         <f>_xll.qlSwapRateHelperSpread($E103,Trigger)</f>
@@ -6959,11 +6959,11 @@
       </c>
       <c r="E104" s="34" t="str">
         <f>Swaps_3M!L14</f>
-        <v>EUR_YC3MRH_AB3E6Y#0002</v>
+        <v>EUR_YC3MRH_AB3E6Y#0007</v>
       </c>
       <c r="F104" s="33">
         <f>_xll.qlRateHelperQuoteValue($E104,Trigger)</f>
-        <v>1.2629999999999999E-2</v>
+        <v>1.201E-2</v>
       </c>
       <c r="G104" s="33">
         <f>_xll.qlSwapRateHelperSpread($E104,Trigger)</f>
@@ -6988,7 +6988,7 @@
       </c>
       <c r="N104" s="37">
         <f t="shared" si="7"/>
-        <v>4.9999999999997963E-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.2">
@@ -7005,11 +7005,11 @@
       </c>
       <c r="E105" s="34" t="str">
         <f>Swaps_3M!L15</f>
-        <v>EUR_YC3MRH_AB3E7Y#0002</v>
+        <v>EUR_YC3MRH_AB3E7Y#0007</v>
       </c>
       <c r="F105" s="33">
         <f>_xll.qlRateHelperQuoteValue($E105,Trigger)</f>
-        <v>1.439E-2</v>
+        <v>1.405E-2</v>
       </c>
       <c r="G105" s="33">
         <f>_xll.qlSwapRateHelperSpread($E105,Trigger)</f>
@@ -7034,7 +7034,7 @@
       </c>
       <c r="N105" s="37">
         <f t="shared" si="7"/>
-        <v>1.7347234759768071E-18</v>
+        <v>5.000000000001531E-6</v>
       </c>
     </row>
     <row r="106" spans="2:14" x14ac:dyDescent="0.2">
@@ -7051,11 +7051,11 @@
       </c>
       <c r="E106" s="34" t="str">
         <f>Swaps_3M!L16</f>
-        <v>EUR_YC3MRH_AB3E8Y#0002</v>
+        <v>EUR_YC3MRH_AB3E8Y#0007</v>
       </c>
       <c r="F106" s="33">
         <f>_xll.qlRateHelperQuoteValue($E106,Trigger)</f>
-        <v>1.5950000000000002E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="G106" s="33">
         <f>_xll.qlSwapRateHelperSpread($E106,Trigger)</f>
@@ -7080,7 +7080,7 @@
       </c>
       <c r="N106" s="37">
         <f t="shared" si="7"/>
-        <v>3.4694469519536142E-18</v>
+        <v>5.000000000001531E-6</v>
       </c>
     </row>
     <row r="107" spans="2:14" x14ac:dyDescent="0.2">
@@ -7097,11 +7097,11 @@
       </c>
       <c r="E107" s="34" t="str">
         <f>Swaps_3M!L17</f>
-        <v>EUR_YC3MRH_AB3E9Y#0002</v>
+        <v>EUR_YC3MRH_AB3E9Y#0007</v>
       </c>
       <c r="F107" s="33">
         <f>_xll.qlRateHelperQuoteValue($E107,Trigger)</f>
-        <v>1.7399999999999999E-2</v>
+        <v>1.755E-2</v>
       </c>
       <c r="G107" s="33">
         <f>_xll.qlSwapRateHelperSpread($E107,Trigger)</f>
@@ -7126,7 +7126,7 @@
       </c>
       <c r="N107" s="37">
         <f t="shared" si="7"/>
-        <v>4.9999999999980616E-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="2:14" x14ac:dyDescent="0.2">
@@ -7143,11 +7143,11 @@
       </c>
       <c r="E108" s="34" t="str">
         <f>Swaps_3M!L18</f>
-        <v>EUR_YC3MRH_AB3E10Y#0002</v>
+        <v>EUR_YC3MRH_AB3E10Y#0007</v>
       </c>
       <c r="F108" s="33">
         <f>_xll.qlRateHelperQuoteValue($E108,Trigger)</f>
-        <v>1.8710000000000001E-2</v>
+        <v>1.9019999999999999E-2</v>
       </c>
       <c r="G108" s="33">
         <f>_xll.qlSwapRateHelperSpread($E108,Trigger)</f>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="N108" s="37">
         <f t="shared" si="7"/>
-        <v>-9.9999999999995925E-6</v>
+        <v>4.9999999999980616E-6</v>
       </c>
     </row>
     <row r="109" spans="2:14" x14ac:dyDescent="0.2">
@@ -7189,11 +7189,11 @@
       </c>
       <c r="E109" s="34" t="str">
         <f>Swaps_3M!L19</f>
-        <v>EUR_YC3MRH_AB3E11Y#0002</v>
+        <v>EUR_YC3MRH_AB3E11Y#0007</v>
       </c>
       <c r="F109" s="33">
         <f>_xll.qlRateHelperQuoteValue($E109,Trigger)</f>
-        <v>1.9860000000000003E-2</v>
+        <v>2.0289999999999999E-2</v>
       </c>
       <c r="G109" s="33">
         <f>_xll.qlSwapRateHelperSpread($E109,Trigger)</f>
@@ -7218,7 +7218,7 @@
       </c>
       <c r="N109" s="37">
         <f t="shared" si="7"/>
-        <v>-4.9999999999980616E-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:14" x14ac:dyDescent="0.2">
@@ -7235,11 +7235,11 @@
       </c>
       <c r="E110" s="34" t="str">
         <f>Swaps_3M!L20</f>
-        <v>EUR_YC3MRH_AB3E12Y#0002</v>
+        <v>EUR_YC3MRH_AB3E12Y#0007</v>
       </c>
       <c r="F110" s="33">
         <f>_xll.qlRateHelperQuoteValue($E110,Trigger)</f>
-        <v>2.0840000000000001E-2</v>
+        <v>2.1400000000000002E-2</v>
       </c>
       <c r="G110" s="33">
         <f>_xll.qlSwapRateHelperSpread($E110,Trigger)</f>
@@ -7264,7 +7264,7 @@
       </c>
       <c r="N110" s="37">
         <f t="shared" si="7"/>
-        <v>-4.9999999999980616E-6</v>
+        <v>5.000000000001531E-6</v>
       </c>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.2">
@@ -7281,7 +7281,7 @@
       </c>
       <c r="E111" s="34" t="str">
         <f>Swaps_3M!L21</f>
-        <v>EUR_YC3MRH_AB3E13Y#0002</v>
+        <v>EUR_YC3MRH_AB3E13Y#0007</v>
       </c>
       <c r="F111" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E111,Trigger)</f>
@@ -7327,7 +7327,7 @@
       </c>
       <c r="E112" s="34" t="str">
         <f>Swaps_3M!L22</f>
-        <v>EUR_YC3MRH_AB3E14Y#0002</v>
+        <v>EUR_YC3MRH_AB3E14Y#0007</v>
       </c>
       <c r="F112" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E112,Trigger)</f>
@@ -7373,11 +7373,11 @@
       </c>
       <c r="E113" s="34" t="str">
         <f>Swaps_3M!L23</f>
-        <v>EUR_YC3MRH_AB3E15Y#0002</v>
+        <v>EUR_YC3MRH_AB3E15Y#0007</v>
       </c>
       <c r="F113" s="33">
         <f>_xll.qlRateHelperQuoteValue($E113,Trigger)</f>
-        <v>2.2889999999999997E-2</v>
+        <v>2.3780000000000003E-2</v>
       </c>
       <c r="G113" s="33">
         <f>_xll.qlSwapRateHelperSpread($E113,Trigger)</f>
@@ -7402,7 +7402,7 @@
       </c>
       <c r="N113" s="37">
         <f t="shared" si="7"/>
-        <v>-1.0000000000003062E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="2:14" x14ac:dyDescent="0.2">
@@ -7419,7 +7419,7 @@
       </c>
       <c r="E114" s="34" t="str">
         <f>Swaps_3M!L24</f>
-        <v>EUR_YC3MRH_AB3E16Y#0002</v>
+        <v>EUR_YC3MRH_AB3E16Y#0007</v>
       </c>
       <c r="F114" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E114,Trigger)</f>
@@ -7465,7 +7465,7 @@
       </c>
       <c r="E115" s="34" t="str">
         <f>Swaps_3M!L25</f>
-        <v>EUR_YC3MRH_AB3E17Y#0002</v>
+        <v>EUR_YC3MRH_AB3E17Y#0007</v>
       </c>
       <c r="F115" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E115,Trigger)</f>
@@ -7511,7 +7511,7 @@
       </c>
       <c r="E116" s="34" t="str">
         <f>Swaps_3M!L26</f>
-        <v>EUR_YC3MRH_AB3E18Y#0002</v>
+        <v>EUR_YC3MRH_AB3E18Y#0007</v>
       </c>
       <c r="F116" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E116,Trigger)</f>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="E117" s="34" t="str">
         <f>Swaps_3M!L27</f>
-        <v>EUR_YC3MRH_AB3E19Y#0002</v>
+        <v>EUR_YC3MRH_AB3E19Y#0007</v>
       </c>
       <c r="F117" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E117,Trigger)</f>
@@ -7603,11 +7603,11 @@
       </c>
       <c r="E118" s="34" t="str">
         <f>Swaps_3M!L28</f>
-        <v>EUR_YC3MRH_AB3E20Y#0002</v>
+        <v>EUR_YC3MRH_AB3E20Y#0007</v>
       </c>
       <c r="F118" s="33">
         <f>_xll.qlRateHelperQuoteValue($E118,Trigger)</f>
-        <v>2.4119999999999999E-2</v>
+        <v>2.545E-2</v>
       </c>
       <c r="G118" s="33">
         <f>_xll.qlSwapRateHelperSpread($E118,Trigger)</f>
@@ -7632,7 +7632,7 @@
       </c>
       <c r="N118" s="37">
         <f t="shared" si="7"/>
-        <v>-9.9999999999995925E-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.2">
@@ -7649,7 +7649,7 @@
       </c>
       <c r="E119" s="34" t="str">
         <f>Swaps_3M!L29</f>
-        <v>EUR_YC3MRH_AB3E21Y#0002</v>
+        <v>EUR_YC3MRH_AB3E21Y#0007</v>
       </c>
       <c r="F119" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E119,Trigger)</f>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="E120" s="34" t="str">
         <f>Swaps_3M!L30</f>
-        <v>EUR_YC3MRH_AB3E22Y#0002</v>
+        <v>EUR_YC3MRH_AB3E22Y#0007</v>
       </c>
       <c r="F120" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E120,Trigger)</f>
@@ -7741,7 +7741,7 @@
       </c>
       <c r="E121" s="34" t="str">
         <f>Swaps_3M!L31</f>
-        <v>EUR_YC3MRH_AB3E23Y#0002</v>
+        <v>EUR_YC3MRH_AB3E23Y#0007</v>
       </c>
       <c r="F121" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E121,Trigger)</f>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="E122" s="34" t="str">
         <f>Swaps_3M!L32</f>
-        <v>EUR_YC3MRH_AB3E24Y#0002</v>
+        <v>EUR_YC3MRH_AB3E24Y#0007</v>
       </c>
       <c r="F122" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E122,Trigger)</f>
@@ -7833,11 +7833,11 @@
       </c>
       <c r="E123" s="34" t="str">
         <f>Swaps_3M!L33</f>
-        <v>EUR_YC3MRH_AB3E25Y#0002</v>
+        <v>EUR_YC3MRH_AB3E25Y#0007</v>
       </c>
       <c r="F123" s="33">
         <f>_xll.qlRateHelperQuoteValue($E123,Trigger)</f>
-        <v>2.4340000000000001E-2</v>
+        <v>2.5939999999999998E-2</v>
       </c>
       <c r="G123" s="33">
         <f>_xll.qlSwapRateHelperSpread($E123,Trigger)</f>
@@ -7862,7 +7862,7 @@
       </c>
       <c r="N123" s="37">
         <f t="shared" si="7"/>
-        <v>-4.9999999999980616E-6</v>
+        <v>4.9999999999945921E-6</v>
       </c>
     </row>
     <row r="124" spans="2:14" x14ac:dyDescent="0.2">
@@ -7879,7 +7879,7 @@
       </c>
       <c r="E124" s="34" t="str">
         <f>Swaps_3M!L34</f>
-        <v>EUR_YC3MRH_AB3E26Y#0002</v>
+        <v>EUR_YC3MRH_AB3E26Y#0007</v>
       </c>
       <c r="F124" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E124,Trigger)</f>
@@ -7925,7 +7925,7 @@
       </c>
       <c r="E125" s="34" t="str">
         <f>Swaps_3M!L35</f>
-        <v>EUR_YC3MRH_AB3E27Y#0002</v>
+        <v>EUR_YC3MRH_AB3E27Y#0007</v>
       </c>
       <c r="F125" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E125,Trigger)</f>
@@ -7971,7 +7971,7 @@
       </c>
       <c r="E126" s="34" t="str">
         <f>Swaps_3M!L36</f>
-        <v>EUR_YC3MRH_AB3E28Y#0002</v>
+        <v>EUR_YC3MRH_AB3E28Y#0007</v>
       </c>
       <c r="F126" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E126,Trigger)</f>
@@ -8017,7 +8017,7 @@
       </c>
       <c r="E127" s="34" t="str">
         <f>Swaps_3M!L37</f>
-        <v>EUR_YC3MRH_AB3E29Y#0002</v>
+        <v>EUR_YC3MRH_AB3E29Y#0007</v>
       </c>
       <c r="F127" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E127,Trigger)</f>
@@ -8063,11 +8063,11 @@
       </c>
       <c r="E128" s="34" t="str">
         <f>Swaps_3M!L38</f>
-        <v>EUR_YC3MRH_AB3E30Y#0002</v>
+        <v>EUR_YC3MRH_AB3E30Y#0007</v>
       </c>
       <c r="F128" s="33">
         <f>_xll.qlRateHelperQuoteValue($E128,Trigger)</f>
-        <v>2.4310000000000002E-2</v>
+        <v>2.6000000000000002E-2</v>
       </c>
       <c r="G128" s="33">
         <f>_xll.qlSwapRateHelperSpread($E128,Trigger)</f>
@@ -8092,7 +8092,7 @@
       </c>
       <c r="N128" s="37">
         <f t="shared" si="7"/>
-        <v>-9.9999999999961231E-6</v>
+        <v>5.000000000001531E-6</v>
       </c>
     </row>
     <row r="129" spans="2:14" x14ac:dyDescent="0.2">
@@ -8109,7 +8109,7 @@
       </c>
       <c r="E129" s="34" t="str">
         <f>Swaps_3M!L39</f>
-        <v>EUR_YC3MRH_AB3E35Y#0002</v>
+        <v>EUR_YC3MRH_AB3E35Y#0007</v>
       </c>
       <c r="F129" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E129,Trigger)</f>
@@ -8155,11 +8155,11 @@
       </c>
       <c r="E130" s="34" t="str">
         <f>Swaps_3M!L40</f>
-        <v>EUR_YC3MRH_AB3E40Y#0002</v>
+        <v>EUR_YC3MRH_AB3E40Y#0007</v>
       </c>
       <c r="F130" s="33">
         <f>_xll.qlRateHelperQuoteValue($E130,Trigger)</f>
-        <v>2.4809999999999999E-2</v>
+        <v>2.632E-2</v>
       </c>
       <c r="G130" s="33">
         <f>_xll.qlSwapRateHelperSpread($E130,Trigger)</f>
@@ -8184,7 +8184,7 @@
       </c>
       <c r="N130" s="37">
         <f t="shared" si="7"/>
-        <v>-1.0000000000003062E-5</v>
+        <v>4.9999999999980616E-6</v>
       </c>
     </row>
     <row r="131" spans="2:14" x14ac:dyDescent="0.2">
@@ -8201,11 +8201,11 @@
       </c>
       <c r="E131" s="34" t="str">
         <f>Swaps_3M!L41</f>
-        <v>EUR_YC3MRH_AB3E50Y#0002</v>
+        <v>EUR_YC3MRH_AB3E50Y#0007</v>
       </c>
       <c r="F131" s="33">
         <f>_xll.qlRateHelperQuoteValue($E131,Trigger)</f>
-        <v>2.5300000000000003E-2</v>
+        <v>2.656E-2</v>
       </c>
       <c r="G131" s="33">
         <f>_xll.qlSwapRateHelperSpread($E131,Trigger)</f>
@@ -8230,7 +8230,7 @@
       </c>
       <c r="N131" s="37">
         <f t="shared" si="7"/>
-        <v>-4.9999999999980616E-6</v>
+        <v>5.000000000001531E-6</v>
       </c>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.2">
@@ -8247,11 +8247,11 @@
       </c>
       <c r="E132" s="27" t="str">
         <f>Swaps_3M!L42</f>
-        <v>EUR_YC3MRH_AB3E60Y#0002</v>
+        <v>EUR_YC3MRH_AB3E60Y#0007</v>
       </c>
       <c r="F132" s="26">
         <f>_xll.qlRateHelperQuoteValue($E132,Trigger)</f>
-        <v>2.564E-2</v>
+        <v>2.6720000000000001E-2</v>
       </c>
       <c r="G132" s="26">
         <f>_xll.qlSwapRateHelperSpread($E132,Trigger)</f>
@@ -8276,7 +8276,7 @@
       </c>
       <c r="N132" s="37">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.9999999999970615E-6</v>
       </c>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.2">
@@ -8293,11 +8293,11 @@
       </c>
       <c r="E133" s="34" t="str">
         <f>SwapsFromBasis_3M!L6</f>
-        <v>EUR_YC3MRH_AB3EBASIS1Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS1Y#0007</v>
       </c>
       <c r="F133" s="33">
         <f>_xll.qlRateHelperQuoteValue($E133,Trigger)</f>
-        <v>3.2699999999999995E-3</v>
+        <v>3.0350000000000004E-3</v>
       </c>
       <c r="G133" s="33">
         <f>_xll.qlSwapRateHelperSpread($E133,Trigger)</f>
@@ -8335,11 +8335,11 @@
       </c>
       <c r="E134" s="34" t="str">
         <f>SwapsFromBasis_3M!L7</f>
-        <v>EUR_YC3MRH_AB3EBASIS15M#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS15M#0007</v>
       </c>
       <c r="F134" s="33">
         <f>_xll.qlRateHelperQuoteValue($E134,Trigger)</f>
-        <v>3.4489999999999998E-3</v>
+        <v>2.8560000000000009E-3</v>
       </c>
       <c r="G134" s="33">
         <f>_xll.qlSwapRateHelperSpread($E134,Trigger)</f>
@@ -8377,11 +8377,11 @@
       </c>
       <c r="E135" s="34" t="str">
         <f>SwapsFromBasis_3M!L8</f>
-        <v>EUR_YC3MRH_AB3EBASIS18M#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS18M#0007</v>
       </c>
       <c r="F135" s="33">
         <f>_xll.qlRateHelperQuoteValue($E135,Trigger)</f>
-        <v>3.9100000000000003E-3</v>
+        <v>3.2100000000000002E-3</v>
       </c>
       <c r="G135" s="33">
         <f>_xll.qlSwapRateHelperSpread($E135,Trigger)</f>
@@ -8419,11 +8419,11 @@
       </c>
       <c r="E136" s="34" t="str">
         <f>SwapsFromBasis_3M!L9</f>
-        <v>EUR_YC3MRH_AB3EBASIS21M#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS21M#0007</v>
       </c>
       <c r="F136" s="33">
         <f>_xll.qlRateHelperQuoteValue($E136,Trigger)</f>
-        <v>4.1200000000000004E-3</v>
+        <v>3.2269999999999998E-3</v>
       </c>
       <c r="G136" s="33">
         <f>_xll.qlSwapRateHelperSpread($E136,Trigger)</f>
@@ -8461,11 +8461,11 @@
       </c>
       <c r="E137" s="34" t="str">
         <f>SwapsFromBasis_3M!L10</f>
-        <v>EUR_YC3MRH_AB3EBASIS2Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS2Y#0007</v>
       </c>
       <c r="F137" s="33">
         <f>_xll.qlRateHelperQuoteValue($E137,Trigger)</f>
-        <v>4.5650000000000005E-3</v>
+        <v>3.6499999999999996E-3</v>
       </c>
       <c r="G137" s="33">
         <f>_xll.qlSwapRateHelperSpread($E137,Trigger)</f>
@@ -8503,11 +8503,11 @@
       </c>
       <c r="E138" s="34" t="str">
         <f>SwapsFromBasis_3M!L11</f>
-        <v>EUR_YC3MRH_AB3EBASIS3Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS3Y#0007</v>
       </c>
       <c r="F138" s="33">
         <f>_xll.qlRateHelperQuoteValue($E138,Trigger)</f>
-        <v>6.2100000000000002E-3</v>
+        <v>5.2649999999999997E-3</v>
       </c>
       <c r="G138" s="33">
         <f>_xll.qlSwapRateHelperSpread($E138,Trigger)</f>
@@ -8545,11 +8545,11 @@
       </c>
       <c r="E139" s="34" t="str">
         <f>SwapsFromBasis_3M!L12</f>
-        <v>EUR_YC3MRH_AB3EBASIS4Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS4Y#0007</v>
       </c>
       <c r="F139" s="33">
         <f>_xll.qlRateHelperQuoteValue($E139,Trigger)</f>
-        <v>8.3750000000000005E-3</v>
+        <v>7.4899999999999993E-3</v>
       </c>
       <c r="G139" s="33">
         <f>_xll.qlSwapRateHelperSpread($E139,Trigger)</f>
@@ -8587,11 +8587,11 @@
       </c>
       <c r="E140" s="34" t="str">
         <f>SwapsFromBasis_3M!L13</f>
-        <v>EUR_YC3MRH_AB3EBASIS5Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS5Y#0007</v>
       </c>
       <c r="F140" s="33">
         <f>_xll.qlRateHelperQuoteValue($E140,Trigger)</f>
-        <v>1.0650000000000001E-2</v>
+        <v>9.810000000000001E-3</v>
       </c>
       <c r="G140" s="33">
         <f>_xll.qlSwapRateHelperSpread($E140,Trigger)</f>
@@ -8629,11 +8629,11 @@
       </c>
       <c r="E141" s="34" t="str">
         <f>SwapsFromBasis_3M!L14</f>
-        <v>EUR_YC3MRH_AB3EBASIS6Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS6Y#0007</v>
       </c>
       <c r="F141" s="33">
         <f>_xll.qlRateHelperQuoteValue($E141,Trigger)</f>
-        <v>1.2624999999999999E-2</v>
+        <v>1.201E-2</v>
       </c>
       <c r="G141" s="33">
         <f>_xll.qlSwapRateHelperSpread($E141,Trigger)</f>
@@ -8671,11 +8671,11 @@
       </c>
       <c r="E142" s="34" t="str">
         <f>SwapsFromBasis_3M!L15</f>
-        <v>EUR_YC3MRH_AB3EBASIS7Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS7Y#0007</v>
       </c>
       <c r="F142" s="33">
         <f>_xll.qlRateHelperQuoteValue($E142,Trigger)</f>
-        <v>1.4389999999999998E-2</v>
+        <v>1.4044999999999998E-2</v>
       </c>
       <c r="G142" s="33">
         <f>_xll.qlSwapRateHelperSpread($E142,Trigger)</f>
@@ -8713,11 +8713,11 @@
       </c>
       <c r="E143" s="34" t="str">
         <f>SwapsFromBasis_3M!L16</f>
-        <v>EUR_YC3MRH_AB3EBASIS8Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS8Y#0007</v>
       </c>
       <c r="F143" s="33">
         <f>_xll.qlRateHelperQuoteValue($E143,Trigger)</f>
-        <v>1.5949999999999999E-2</v>
+        <v>1.5894999999999999E-2</v>
       </c>
       <c r="G143" s="33">
         <f>_xll.qlSwapRateHelperSpread($E143,Trigger)</f>
@@ -8755,11 +8755,11 @@
       </c>
       <c r="E144" s="34" t="str">
         <f>SwapsFromBasis_3M!L17</f>
-        <v>EUR_YC3MRH_AB3EBASIS9Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS9Y#0007</v>
       </c>
       <c r="F144" s="33">
         <f>_xll.qlRateHelperQuoteValue($E144,Trigger)</f>
-        <v>1.7395000000000001E-2</v>
+        <v>1.755E-2</v>
       </c>
       <c r="G144" s="33">
         <f>_xll.qlSwapRateHelperSpread($E144,Trigger)</f>
@@ -8797,11 +8797,11 @@
       </c>
       <c r="E145" s="34" t="str">
         <f>SwapsFromBasis_3M!L18</f>
-        <v>EUR_YC3MRH_AB3EBASIS10Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS10Y#0007</v>
       </c>
       <c r="F145" s="33">
         <f>_xll.qlRateHelperQuoteValue($E145,Trigger)</f>
-        <v>1.8720000000000001E-2</v>
+        <v>1.9015000000000001E-2</v>
       </c>
       <c r="G145" s="33">
         <f>_xll.qlSwapRateHelperSpread($E145,Trigger)</f>
@@ -8839,11 +8839,11 @@
       </c>
       <c r="E146" s="34" t="str">
         <f>SwapsFromBasis_3M!L19</f>
-        <v>EUR_YC3MRH_AB3EBASIS11Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS11Y#0007</v>
       </c>
       <c r="F146" s="33">
         <f>_xll.qlRateHelperQuoteValue($E146,Trigger)</f>
-        <v>1.9865000000000001E-2</v>
+        <v>2.0289999999999999E-2</v>
       </c>
       <c r="G146" s="33">
         <f>_xll.qlSwapRateHelperSpread($E146,Trigger)</f>
@@ -8881,11 +8881,11 @@
       </c>
       <c r="E147" s="34" t="str">
         <f>SwapsFromBasis_3M!L20</f>
-        <v>EUR_YC3MRH_AB3EBASIS12Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS12Y#0007</v>
       </c>
       <c r="F147" s="33">
         <f>_xll.qlRateHelperQuoteValue($E147,Trigger)</f>
-        <v>2.0844999999999999E-2</v>
+        <v>2.1395000000000001E-2</v>
       </c>
       <c r="G147" s="33">
         <f>_xll.qlSwapRateHelperSpread($E147,Trigger)</f>
@@ -8923,11 +8923,11 @@
       </c>
       <c r="E148" s="34" t="str">
         <f>SwapsFromBasis_3M!L21</f>
-        <v>EUR_YC3MRH_AB3EBASIS13Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS13Y#0007</v>
       </c>
       <c r="F148" s="33">
         <f>_xll.qlRateHelperQuoteValue($E148,Trigger)</f>
-        <v>2.1675999999999997E-2</v>
+        <v>2.2339999999999999E-2</v>
       </c>
       <c r="G148" s="33">
         <f>_xll.qlSwapRateHelperSpread($E148,Trigger)</f>
@@ -8965,11 +8965,11 @@
       </c>
       <c r="E149" s="34" t="str">
         <f>SwapsFromBasis_3M!L22</f>
-        <v>EUR_YC3MRH_AB3EBASIS14Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS14Y#0007</v>
       </c>
       <c r="F149" s="33">
         <f>_xll.qlRateHelperQuoteValue($E149,Trigger)</f>
-        <v>2.2359000000000004E-2</v>
+        <v>2.3132E-2</v>
       </c>
       <c r="G149" s="33">
         <f>_xll.qlSwapRateHelperSpread($E149,Trigger)</f>
@@ -9007,11 +9007,11 @@
       </c>
       <c r="E150" s="34" t="str">
         <f>SwapsFromBasis_3M!L23</f>
-        <v>EUR_YC3MRH_AB3EBASIS15Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS15Y#0007</v>
       </c>
       <c r="F150" s="33">
         <f>_xll.qlRateHelperQuoteValue($E150,Trigger)</f>
-        <v>2.29E-2</v>
+        <v>2.3780000000000003E-2</v>
       </c>
       <c r="G150" s="33">
         <f>_xll.qlSwapRateHelperSpread($E150,Trigger)</f>
@@ -9049,11 +9049,11 @@
       </c>
       <c r="E151" s="34" t="str">
         <f>SwapsFromBasis_3M!L24</f>
-        <v>EUR_YC3MRH_AB3EBASIS16Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS16Y#0007</v>
       </c>
       <c r="F151" s="33">
         <f>_xll.qlRateHelperQuoteValue($E151,Trigger)</f>
-        <v>2.3319000000000003E-2</v>
+        <v>2.4301999999999997E-2</v>
       </c>
       <c r="G151" s="33">
         <f>_xll.qlSwapRateHelperSpread($E151,Trigger)</f>
@@ -9091,11 +9091,11 @@
       </c>
       <c r="E152" s="34" t="str">
         <f>SwapsFromBasis_3M!L25</f>
-        <v>EUR_YC3MRH_AB3EBASIS17Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS17Y#0007</v>
       </c>
       <c r="F152" s="33">
         <f>_xll.qlRateHelperQuoteValue($E152,Trigger)</f>
-        <v>2.3635E-2</v>
+        <v>2.4707000000000003E-2</v>
       </c>
       <c r="G152" s="33">
         <f>_xll.qlSwapRateHelperSpread($E152,Trigger)</f>
@@ -9133,11 +9133,11 @@
       </c>
       <c r="E153" s="34" t="str">
         <f>SwapsFromBasis_3M!L26</f>
-        <v>EUR_YC3MRH_AB3EBASIS18Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS18Y#0007</v>
       </c>
       <c r="F153" s="33">
         <f>_xll.qlRateHelperQuoteValue($E153,Trigger)</f>
-        <v>2.3858999999999998E-2</v>
+        <v>2.5018000000000002E-2</v>
       </c>
       <c r="G153" s="33">
         <f>_xll.qlSwapRateHelperSpread($E153,Trigger)</f>
@@ -9175,11 +9175,11 @@
       </c>
       <c r="E154" s="34" t="str">
         <f>SwapsFromBasis_3M!L27</f>
-        <v>EUR_YC3MRH_AB3EBASIS19Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS19Y#0007</v>
       </c>
       <c r="F154" s="33">
         <f>_xll.qlRateHelperQuoteValue($E154,Trigger)</f>
-        <v>2.4020000000000003E-2</v>
+        <v>2.5266E-2</v>
       </c>
       <c r="G154" s="33">
         <f>_xll.qlSwapRateHelperSpread($E154,Trigger)</f>
@@ -9217,11 +9217,11 @@
       </c>
       <c r="E155" s="34" t="str">
         <f>SwapsFromBasis_3M!L28</f>
-        <v>EUR_YC3MRH_AB3EBASIS20Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS20Y#0007</v>
       </c>
       <c r="F155" s="33">
         <f>_xll.qlRateHelperQuoteValue($E155,Trigger)</f>
-        <v>2.4129999999999999E-2</v>
+        <v>2.545E-2</v>
       </c>
       <c r="G155" s="33">
         <f>_xll.qlSwapRateHelperSpread($E155,Trigger)</f>
@@ -9259,11 +9259,11 @@
       </c>
       <c r="E156" s="34" t="str">
         <f>SwapsFromBasis_3M!L29</f>
-        <v>EUR_YC3MRH_AB3EBASIS21Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS21Y#0007</v>
       </c>
       <c r="F156" s="33">
         <f>_xll.qlRateHelperQuoteValue($E156,Trigger)</f>
-        <v>2.4207999999999997E-2</v>
+        <v>2.5611999999999999E-2</v>
       </c>
       <c r="G156" s="33">
         <f>_xll.qlSwapRateHelperSpread($E156,Trigger)</f>
@@ -9301,11 +9301,11 @@
       </c>
       <c r="E157" s="34" t="str">
         <f>SwapsFromBasis_3M!L30</f>
-        <v>EUR_YC3MRH_AB3EBASIS22Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS22Y#0007</v>
       </c>
       <c r="F157" s="33">
         <f>_xll.qlRateHelperQuoteValue($E157,Trigger)</f>
-        <v>2.4274000000000004E-2</v>
+        <v>2.5723000000000003E-2</v>
       </c>
       <c r="G157" s="33">
         <f>_xll.qlSwapRateHelperSpread($E157,Trigger)</f>
@@ -9343,11 +9343,11 @@
       </c>
       <c r="E158" s="34" t="str">
         <f>SwapsFromBasis_3M!L31</f>
-        <v>EUR_YC3MRH_AB3EBASIS23Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS23Y#0007</v>
       </c>
       <c r="F158" s="33">
         <f>_xll.qlRateHelperQuoteValue($E158,Trigger)</f>
-        <v>2.4318999999999997E-2</v>
+        <v>2.5822000000000001E-2</v>
       </c>
       <c r="G158" s="33">
         <f>_xll.qlSwapRateHelperSpread($E158,Trigger)</f>
@@ -9385,11 +9385,11 @@
       </c>
       <c r="E159" s="34" t="str">
         <f>SwapsFromBasis_3M!L32</f>
-        <v>EUR_YC3MRH_AB3EBASIS24Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS24Y#0007</v>
       </c>
       <c r="F159" s="33">
         <f>_xll.qlRateHelperQuoteValue($E159,Trigger)</f>
-        <v>2.4331999999999996E-2</v>
+        <v>2.5888999999999999E-2</v>
       </c>
       <c r="G159" s="33">
         <f>_xll.qlSwapRateHelperSpread($E159,Trigger)</f>
@@ -9427,11 +9427,11 @@
       </c>
       <c r="E160" s="34" t="str">
         <f>SwapsFromBasis_3M!L33</f>
-        <v>EUR_YC3MRH_AB3EBASIS25Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS25Y#0007</v>
       </c>
       <c r="F160" s="33">
         <f>_xll.qlRateHelperQuoteValue($E160,Trigger)</f>
-        <v>2.4344999999999999E-2</v>
+        <v>2.5935000000000003E-2</v>
       </c>
       <c r="G160" s="33">
         <f>_xll.qlSwapRateHelperSpread($E160,Trigger)</f>
@@ -9469,11 +9469,11 @@
       </c>
       <c r="E161" s="34" t="str">
         <f>SwapsFromBasis_3M!L34</f>
-        <v>EUR_YC3MRH_AB3EBASIS26Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS26Y#0007</v>
       </c>
       <c r="F161" s="33">
         <f>_xll.qlRateHelperQuoteValue($E161,Trigger)</f>
-        <v>2.4347000000000001E-2</v>
+        <v>2.5959000000000003E-2</v>
       </c>
       <c r="G161" s="33">
         <f>_xll.qlSwapRateHelperSpread($E161,Trigger)</f>
@@ -9511,11 +9511,11 @@
       </c>
       <c r="E162" s="34" t="str">
         <f>SwapsFromBasis_3M!L35</f>
-        <v>EUR_YC3MRH_AB3EBASIS27Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS27Y#0007</v>
       </c>
       <c r="F162" s="33">
         <f>_xll.qlRateHelperQuoteValue($E162,Trigger)</f>
-        <v>2.4339000000000003E-2</v>
+        <v>2.5981999999999998E-2</v>
       </c>
       <c r="G162" s="33">
         <f>_xll.qlSwapRateHelperSpread($E162,Trigger)</f>
@@ -9553,11 +9553,11 @@
       </c>
       <c r="E163" s="34" t="str">
         <f>SwapsFromBasis_3M!L36</f>
-        <v>EUR_YC3MRH_AB3EBASIS28Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS28Y#0007</v>
       </c>
       <c r="F163" s="33">
         <f>_xll.qlRateHelperQuoteValue($E163,Trigger)</f>
-        <v>2.4319E-2</v>
+        <v>2.5984E-2</v>
       </c>
       <c r="G163" s="33">
         <f>_xll.qlSwapRateHelperSpread($E163,Trigger)</f>
@@ -9595,11 +9595,11 @@
       </c>
       <c r="E164" s="34" t="str">
         <f>SwapsFromBasis_3M!L37</f>
-        <v>EUR_YC3MRH_AB3EBASIS29Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS29Y#0007</v>
       </c>
       <c r="F164" s="33">
         <f>_xll.qlRateHelperQuoteValue($E164,Trigger)</f>
-        <v>2.4319999999999998E-2</v>
+        <v>2.5985000000000001E-2</v>
       </c>
       <c r="G164" s="33">
         <f>_xll.qlSwapRateHelperSpread($E164,Trigger)</f>
@@ -9637,11 +9637,11 @@
       </c>
       <c r="E165" s="34" t="str">
         <f>SwapsFromBasis_3M!L38</f>
-        <v>EUR_YC3MRH_AB3EBASIS30Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS30Y#0007</v>
       </c>
       <c r="F165" s="33">
         <f>_xll.qlRateHelperQuoteValue($E165,Trigger)</f>
-        <v>2.4319999999999998E-2</v>
+        <v>2.5995000000000001E-2</v>
       </c>
       <c r="G165" s="33">
         <f>_xll.qlSwapRateHelperSpread($E165,Trigger)</f>
@@ -9679,11 +9679,11 @@
       </c>
       <c r="E166" s="34" t="str">
         <f>SwapsFromBasis_3M!L39</f>
-        <v>EUR_YC3MRH_AB3EBASIS35Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS35Y#0007</v>
       </c>
       <c r="F166" s="33">
         <f>_xll.qlRateHelperQuoteValue($E166,Trigger)</f>
-        <v>2.4505000000000002E-2</v>
+        <v>2.6120000000000001E-2</v>
       </c>
       <c r="G166" s="33">
         <f>_xll.qlSwapRateHelperSpread($E166,Trigger)</f>
@@ -9721,11 +9721,11 @@
       </c>
       <c r="E167" s="34" t="str">
         <f>SwapsFromBasis_3M!L40</f>
-        <v>EUR_YC3MRH_AB3EBASIS40Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS40Y#0007</v>
       </c>
       <c r="F167" s="33">
         <f>_xll.qlRateHelperQuoteValue($E167,Trigger)</f>
-        <v>2.4820000000000002E-2</v>
+        <v>2.6315000000000002E-2</v>
       </c>
       <c r="G167" s="33">
         <f>_xll.qlSwapRateHelperSpread($E167,Trigger)</f>
@@ -9763,11 +9763,11 @@
       </c>
       <c r="E168" s="34" t="str">
         <f>SwapsFromBasis_3M!L41</f>
-        <v>EUR_YC3MRH_AB3EBASIS50Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS50Y#0007</v>
       </c>
       <c r="F168" s="33">
         <f>_xll.qlRateHelperQuoteValue($E168,Trigger)</f>
-        <v>2.5305000000000001E-2</v>
+        <v>2.6554999999999999E-2</v>
       </c>
       <c r="G168" s="33">
         <f>_xll.qlSwapRateHelperSpread($E168,Trigger)</f>
@@ -9805,11 +9805,11 @@
       </c>
       <c r="E169" s="27" t="str">
         <f>SwapsFromBasis_3M!L42</f>
-        <v>EUR_YC3MRH_AB3EBASIS60Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS60Y#0007</v>
       </c>
       <c r="F169" s="26">
         <f>_xll.qlRateHelperQuoteValue($E169,Trigger)</f>
-        <v>2.564E-2</v>
+        <v>2.6716000000000004E-2</v>
       </c>
       <c r="G169" s="26">
         <f>_xll.qlSwapRateHelperSpread($E169,Trigger)</f>
@@ -9850,7 +9850,7 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -9925,7 +9925,7 @@
         <v>115</v>
       </c>
       <c r="L2" s="37">
-        <v>2.1610000000000002E-3</v>
+        <v>3.0699999999999998E-3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -9961,7 +9961,7 @@
         <v>116</v>
       </c>
       <c r="L3" s="37">
-        <v>2.1159999999999998E-3</v>
+        <v>3.0240000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -9997,7 +9997,7 @@
         <v>117</v>
       </c>
       <c r="L4" s="37">
-        <v>2.1389999999999998E-3</v>
+        <v>2.967E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -10033,7 +10033,7 @@
         <v>118</v>
       </c>
       <c r="L5" s="37">
-        <v>2.2430000000000002E-3</v>
+        <v>2.993E-3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -10045,49 +10045,49 @@
         <v/>
       </c>
       <c r="D6" s="11" t="str">
-        <v>EUR_YC3MRH_TOM3F1</v>
+        <v>EUR_YC3MRH_FUT3MH4</v>
       </c>
       <c r="E6" s="10">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>2.2500000000000003E-3</v>
-      </c>
-      <c r="F6" s="10" t="str">
+        <v>2.9749999999999499E-3</v>
+      </c>
+      <c r="F6" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="G6" s="9">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41661</v>
+        <v>41717</v>
       </c>
       <c r="H6" s="8">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41751</v>
+        <v>41809</v>
       </c>
       <c r="I6" s="3">
-        <v>0.99942920371582944</v>
+        <v>0.9987674438824794</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="L6" s="37">
-        <v>2.1749999999999999E-3</v>
+        <v>2.9750000000000002E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="str">
         <f>_xll.ohGroup(,_xll.ohPack(D2:D126),Permanent,,ObjectOverwrite)</f>
-        <v>obj_00652#0002</v>
+        <v>obj_00652#0008</v>
       </c>
       <c r="B7" s="12" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
         <v/>
       </c>
       <c r="D7" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MH4</v>
+        <v>EUR_YC3MRH_FUT3MM4</v>
       </c>
       <c r="E7" s="10">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>2.6249999999999885E-3</v>
+        <v>2.9250000000000664E-3</v>
       </c>
       <c r="F7" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -10095,29 +10095,29 @@
       </c>
       <c r="G7" s="9">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41717</v>
+        <v>41808</v>
       </c>
       <c r="H7" s="8">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41809</v>
+        <v>41900</v>
       </c>
       <c r="I7" s="3">
-        <v>0.99885105854675016</v>
+        <v>0.99802952065646833</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L7" s="37">
-        <v>2.2750000000000001E-3</v>
+        <v>2.9250000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MM4</v>
+        <v>EUR_YC3MRH_FUT3MU4</v>
       </c>
       <c r="E8" s="10">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>3.2250000000000334E-3</v>
+        <v>2.9749999999999499E-3</v>
       </c>
       <c r="F8" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -10125,29 +10125,29 @@
       </c>
       <c r="G8" s="9">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41808</v>
+        <v>41899</v>
       </c>
       <c r="H8" s="8">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41900</v>
+        <v>41990</v>
       </c>
       <c r="I8" s="3">
-        <v>0.99803990807081455</v>
+        <v>0.99728767716154787</v>
       </c>
       <c r="K8" s="218" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L8" s="37">
-        <v>2.575E-3</v>
+        <v>2.9750000000000002E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MU4</v>
+        <v>EUR_YC3MRH_FUT3MZ4</v>
       </c>
       <c r="E9" s="10">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>3.9249999999999563E-3</v>
+        <v>3.1749999999999279E-3</v>
       </c>
       <c r="F9" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -10155,29 +10155,29 @@
       </c>
       <c r="G9" s="9">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41899</v>
+        <v>41990</v>
       </c>
       <c r="H9" s="8">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41990</v>
+        <v>42080</v>
       </c>
       <c r="I9" s="3">
-        <v>0.9970596694493179</v>
+        <v>0.99649670789965239</v>
       </c>
       <c r="K9" s="218" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L9" s="37">
-        <v>2.8249999999999998E-3</v>
+        <v>3.1749999999999999E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D10" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MZ4</v>
+        <v>EUR_YC3MRH_FUT3MH5</v>
       </c>
       <c r="E10" s="10">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>4.5250000000000012E-3</v>
+        <v>3.5749999999999948E-3</v>
       </c>
       <c r="F10" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -10185,29 +10185,29 @@
       </c>
       <c r="G10" s="9">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41990</v>
+        <v>42081</v>
       </c>
       <c r="H10" s="8">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>42080</v>
+        <v>42173</v>
       </c>
       <c r="I10" s="3">
-        <v>0.99593302022019381</v>
+        <v>0.99557787792129249</v>
       </c>
       <c r="K10" s="218" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L10" s="37">
-        <v>3.225E-3</v>
+        <v>3.5750000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MH5</v>
+        <v>EUR_YC3MRH_FUT3MM5</v>
       </c>
       <c r="E11" s="10">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>5.1250000000000462E-3</v>
+        <v>4.1249999999999343E-3</v>
       </c>
       <c r="F11" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -10215,29 +10215,29 @@
       </c>
       <c r="G11" s="9">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42081</v>
+        <v>42172</v>
       </c>
       <c r="H11" s="8">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>42173</v>
+        <v>42264</v>
       </c>
       <c r="I11" s="3">
-        <v>0.99461712438178396</v>
+        <v>0.99454000768750406</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L11" s="37">
-        <v>3.6749999999999999E-3</v>
+        <v>4.1250000000000002E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MM5</v>
+        <v>EUR_YC3MRH_FUT3MU5</v>
       </c>
       <c r="E12" s="10">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>5.8249999999999691E-3</v>
+        <v>4.9250000000000682E-3</v>
       </c>
       <c r="F12" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -10245,29 +10245,29 @@
       </c>
       <c r="G12" s="9">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42172</v>
+        <v>42263</v>
       </c>
       <c r="H12" s="8">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42264</v>
+        <v>42354</v>
       </c>
       <c r="I12" s="3">
-        <v>0.99315381481156628</v>
+        <v>0.99331580989011115</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L12" s="37">
-        <v>4.3249999999999999E-3</v>
+        <v>4.9249999999999997E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D13" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MU5</v>
+        <v>EUR_YC3MRH_FUT3MZ5</v>
       </c>
       <c r="E13" s="10">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>6.525000000000003E-3</v>
+        <v>5.8750000000000746E-3</v>
       </c>
       <c r="F13" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -10275,29 +10275,29 @@
       </c>
       <c r="G13" s="9">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42263</v>
+        <v>42354</v>
       </c>
       <c r="H13" s="8">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42354</v>
+        <v>42445</v>
       </c>
       <c r="I13" s="3">
-        <v>0.99153540386150263</v>
+        <v>0.99184285437368624</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="L13" s="37">
-        <v>5.1749999999999999E-3</v>
+        <v>5.875E-3</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D14" s="11" t="str">
-        <v>EUR_YC3MRH_FUT3MZ5</v>
+        <v>EUR_YC3MRH_AB3E3Y</v>
       </c>
       <c r="E14" s="10">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>7.3250000000000259E-3</v>
+        <v>5.2700000000000004E-3</v>
       </c>
       <c r="F14" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -10305,29 +10305,29 @@
       </c>
       <c r="G14" s="9">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>42354</v>
+        <v>41660</v>
       </c>
       <c r="H14" s="8">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42445</v>
+        <v>42758</v>
       </c>
       <c r="I14" s="3">
-        <v>0.98970287277145352</v>
+        <v>0.98429792952349793</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>126</v>
       </c>
       <c r="L14" s="37">
-        <v>4.7400000000000003E-3</v>
+        <v>5.2700000000000004E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E3Y</v>
+        <v>EUR_YC3MRH_AB3E4Y</v>
       </c>
       <c r="E15" s="10">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>6.2100000000000002E-3</v>
+        <v>7.4900000000000001E-3</v>
       </c>
       <c r="F15" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -10339,25 +10339,25 @@
       </c>
       <c r="H15" s="8">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42758</v>
+        <v>43122</v>
       </c>
       <c r="I15" s="3">
-        <v>0.98152866418254336</v>
+        <v>0.9704350271775819</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>127</v>
       </c>
       <c r="L15" s="37">
-        <v>7.0099999999999997E-3</v>
+        <v>7.4900000000000001E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E4Y</v>
+        <v>EUR_YC3MRH_AB3E5Y</v>
       </c>
       <c r="E16" s="10">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>8.3800000000000003E-3</v>
+        <v>9.8099999999999993E-3</v>
       </c>
       <c r="F16" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -10369,25 +10369,25 @@
       </c>
       <c r="H16" s="8">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>43122</v>
+        <v>43486</v>
       </c>
       <c r="I16" s="3">
-        <v>0.96699321354579781</v>
+        <v>0.95196455415332748</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>128</v>
       </c>
       <c r="L16" s="37">
-        <v>9.4400000000000005E-3</v>
+        <v>9.8099999999999993E-3</v>
       </c>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D17" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E5Y</v>
+        <v>EUR_YC3MRH_AB3E6Y</v>
       </c>
       <c r="E17" s="10">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>1.065E-2</v>
+        <v>1.201E-2</v>
       </c>
       <c r="F17" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -10399,25 +10399,25 @@
       </c>
       <c r="H17" s="8">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>43486</v>
+        <v>43851</v>
       </c>
       <c r="I17" s="3">
-        <v>0.94798424670544834</v>
+        <v>0.93002250871029335</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>129</v>
       </c>
       <c r="L17" s="37">
-        <v>1.176E-2</v>
+        <v>1.201E-2</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D18" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E6Y</v>
+        <v>EUR_YC3MRH_AB3E7Y</v>
       </c>
       <c r="E18" s="10">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.2629999999999999E-2</v>
+        <v>1.405E-2</v>
       </c>
       <c r="F18" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -10429,25 +10429,25 @@
       </c>
       <c r="H18" s="8">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>43851</v>
+        <v>44217</v>
       </c>
       <c r="I18" s="3">
-        <v>0.92661062015753326</v>
+        <v>0.90541515745241696</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>130</v>
       </c>
       <c r="L18" s="37">
-        <v>1.391E-2</v>
+        <v>1.405E-2</v>
       </c>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D19" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E7Y</v>
+        <v>EUR_YC3MRH_AB3E8Y</v>
       </c>
       <c r="E19" s="10">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>1.439E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="F19" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -10459,25 +10459,25 @@
       </c>
       <c r="H19" s="8">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>44217</v>
+        <v>44582</v>
       </c>
       <c r="I19" s="3">
-        <v>0.90338405827606372</v>
+        <v>0.87898506301363055</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>131</v>
       </c>
       <c r="L19" s="37">
-        <v>1.583E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D20" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E8Y</v>
+        <v>EUR_YC3MRH_AB3E9Y</v>
       </c>
       <c r="E20" s="10">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>1.5950000000000002E-2</v>
+        <v>1.755E-2</v>
       </c>
       <c r="F20" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -10489,25 +10489,25 @@
       </c>
       <c r="H20" s="8">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>44582</v>
+        <v>44949</v>
       </c>
       <c r="I20" s="3">
-        <v>0.87889173447947255</v>
+        <v>0.8514017959808502</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>132</v>
       </c>
       <c r="L20" s="37">
-        <v>1.753E-2</v>
+        <v>1.755E-2</v>
       </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D21" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E9Y</v>
+        <v>EUR_YC3MRH_AB3E10Y</v>
       </c>
       <c r="E21" s="10">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>1.7399999999999999E-2</v>
+        <v>1.9019999999999999E-2</v>
       </c>
       <c r="F21" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -10519,25 +10519,25 @@
       </c>
       <c r="H21" s="8">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>44949</v>
+        <v>45313</v>
       </c>
       <c r="I21" s="3">
-        <v>0.85295797086256664</v>
+        <v>0.82333870634032191</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>133</v>
       </c>
       <c r="L21" s="37">
-        <v>1.9060000000000001E-2</v>
+        <v>1.9019999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D22" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E10Y</v>
+        <v>EUR_YC3MRH_AB3E12Y</v>
       </c>
       <c r="E22" s="10">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>1.8710000000000001E-2</v>
+        <v>2.1400000000000002E-2</v>
       </c>
       <c r="F22" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -10549,25 +10549,25 @@
       </c>
       <c r="H22" s="8">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>45313</v>
+        <v>46043</v>
       </c>
       <c r="I22" s="3">
-        <v>0.82646731509808502</v>
+        <v>0.76782860382967666</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>134</v>
       </c>
       <c r="L22" s="37">
-        <v>2.1520000000000001E-2</v>
+        <v>2.1399999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D23" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E12Y</v>
+        <v>EUR_YC3MRH_AB3E15Y</v>
       </c>
       <c r="E23" s="10">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>2.0840000000000001E-2</v>
+        <v>2.3780000000000003E-2</v>
       </c>
       <c r="F23" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -10579,25 +10579,25 @@
       </c>
       <c r="H23" s="8">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>46043</v>
+        <v>47140</v>
       </c>
       <c r="I23" s="3">
-        <v>0.77395772498850468</v>
+        <v>0.69089780723857686</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>135</v>
       </c>
       <c r="L23" s="37">
-        <v>2.3959999999999999E-2</v>
+        <v>2.3779999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D24" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E15Y</v>
+        <v>EUR_YC3MRH_AB3E20Y</v>
       </c>
       <c r="E24" s="10">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>2.2889999999999997E-2</v>
+        <v>2.545E-2</v>
       </c>
       <c r="F24" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -10609,25 +10609,25 @@
       </c>
       <c r="H24" s="8">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>47140</v>
+        <v>48967</v>
       </c>
       <c r="I24" s="3">
-        <v>0.70188355983274198</v>
+        <v>0.58928894055572645</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>136</v>
       </c>
       <c r="L24" s="37">
-        <v>2.571E-2</v>
+        <v>2.545E-2</v>
       </c>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D25" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E20Y</v>
+        <v>EUR_YC3MRH_AB3E25Y</v>
       </c>
       <c r="E25" s="10">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>2.4119999999999999E-2</v>
+        <v>2.5939999999999998E-2</v>
       </c>
       <c r="F25" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -10639,25 +10639,25 @@
       </c>
       <c r="H25" s="8">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>48967</v>
+        <v>50791</v>
       </c>
       <c r="I25" s="3">
-        <v>0.60822627782844763</v>
+        <v>0.51129766137658039</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>137</v>
       </c>
       <c r="L25" s="37">
-        <v>2.6280000000000001E-2</v>
+        <v>2.5940000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D26" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E25Y</v>
+        <v>EUR_YC3MRH_AB3E30Y</v>
       </c>
       <c r="E26" s="10">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>2.4340000000000001E-2</v>
+        <v>2.6000000000000002E-2</v>
       </c>
       <c r="F26" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -10669,25 +10669,25 @@
       </c>
       <c r="H26" s="8">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>50791</v>
+        <v>52617</v>
       </c>
       <c r="I26" s="3">
-        <v>0.53613251189291333</v>
+        <v>0.44868754281442896</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>138</v>
       </c>
       <c r="L26" s="37">
-        <v>2.6450000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D27" s="11" t="str">
-        <v>EUR_YC3MRH_AB3E30Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS35Y</v>
       </c>
       <c r="E27" s="10">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>2.4310000000000002E-2</v>
+        <v>2.6120000000000001E-2</v>
       </c>
       <c r="F27" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -10699,25 +10699,25 @@
       </c>
       <c r="H27" s="8">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>52617</v>
+        <v>54444</v>
       </c>
       <c r="I27" s="3">
-        <v>0.47598176884021015</v>
+        <v>0.39202568677673444</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>139</v>
       </c>
       <c r="L27" s="37">
-        <v>2.6596999999999999E-2</v>
+        <v>2.6120000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D28" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS35Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS40Y</v>
       </c>
       <c r="E28" s="10">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.4505000000000002E-2</v>
+        <v>2.6315000000000002E-2</v>
       </c>
       <c r="F28" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -10729,25 +10729,25 @@
       </c>
       <c r="H28" s="8">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>54444</v>
+        <v>56270</v>
       </c>
       <c r="I28" s="3">
-        <v>0.41774965432003353</v>
+        <v>0.34007196302860065</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>140</v>
       </c>
       <c r="L28" s="37">
-        <v>2.683E-2</v>
+        <v>2.6315000000000002E-2</v>
       </c>
     </row>
     <row r="29" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D29" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS40Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS50Y</v>
       </c>
       <c r="E29" s="10">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.4820000000000002E-2</v>
+        <v>2.6554999999999999E-2</v>
       </c>
       <c r="F29" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -10759,25 +10759,25 @@
       </c>
       <c r="H29" s="8">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>56270</v>
+        <v>59922</v>
       </c>
       <c r="I29" s="3">
-        <v>0.36258214894487723</v>
+        <v>0.25649459475513936</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>141</v>
       </c>
       <c r="L29" s="37">
-        <v>2.7175000000000001E-2</v>
+        <v>2.6554999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D30" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS50Y</v>
+        <v>EUR_YC3MRH_AB3EBASIS60Y</v>
       </c>
       <c r="E30" s="10">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.5305000000000001E-2</v>
+        <v>2.6716000000000004E-2</v>
       </c>
       <c r="F30" s="10">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -10789,40 +10789,40 @@
       </c>
       <c r="H30" s="8">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>59922</v>
+        <v>63576</v>
       </c>
       <c r="I30" s="3">
-        <v>0.27156663703441392</v>
+        <v>0.19313772797651729</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>142</v>
       </c>
       <c r="L30" s="37">
-        <v>2.7481999999999999E-2</v>
+        <v>2.6716E-2</v>
       </c>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D31" s="11" t="str">
-        <v>EUR_YC3MRH_AB3EBASIS60Y</v>
-      </c>
-      <c r="E31" s="10">
+      <c r="D31" s="11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E31" s="10" t="e">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.564E-2</v>
-      </c>
-      <c r="F31" s="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F31" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="9">
+        <v>--</v>
+      </c>
+      <c r="G31" s="9" t="e">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41660</v>
-      </c>
-      <c r="H31" s="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H31" s="8" t="e">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>63576</v>
-      </c>
-      <c r="I31" s="3">
-        <v>0.2024386808921399</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I31" s="3" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L31" s="46"/>
     </row>
@@ -13198,7 +13198,7 @@
       </c>
       <c r="F3" s="101" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_SND#0002</v>
+        <v>EUR_YC3MRH_SND#0007</v>
       </c>
       <c r="G3" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -13225,7 +13225,7 @@
       </c>
       <c r="F4" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_SWD#0002</v>
+        <v>EUR_YC3MRH_SWD#0007</v>
       </c>
       <c r="G4" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -13252,7 +13252,7 @@
       </c>
       <c r="F5" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2WD#0002</v>
+        <v>EUR_YC3MRH_2WD#0007</v>
       </c>
       <c r="G5" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -13283,7 +13283,7 @@
       </c>
       <c r="F6" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3WD#0002</v>
+        <v>EUR_YC3MRH_3WD#0007</v>
       </c>
       <c r="G6" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -13310,7 +13310,7 @@
       </c>
       <c r="F7" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1MD#0002</v>
+        <v>EUR_YC3MRH_1MD#0007</v>
       </c>
       <c r="G7" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -13337,7 +13337,7 @@
       </c>
       <c r="F8" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2MD#0002</v>
+        <v>EUR_YC3MRH_2MD#0007</v>
       </c>
       <c r="G8" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -13364,7 +13364,7 @@
       </c>
       <c r="F9" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3MD#0002</v>
+        <v>EUR_YC3MRH_3MD#0007</v>
       </c>
       <c r="G9" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -13392,9 +13392,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13411,7 +13413,7 @@
     <col min="11" max="16384" width="9.140625" style="108"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="173" t="s">
         <v>169</v>
       </c>
@@ -13432,7 +13434,7 @@
       <c r="I1" s="150"/>
       <c r="J1" s="149"/>
     </row>
-    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="100"/>
       <c r="B2" s="103"/>
       <c r="C2" s="103"/>
@@ -13457,7 +13459,7 @@
       </c>
       <c r="J2" s="93"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="100"/>
       <c r="B3" s="145" t="s">
         <v>163</v>
@@ -13483,7 +13485,7 @@
       </c>
       <c r="H3" s="143" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_T3F1#0002</v>
+        <v>EUR_YC3MRH_T3F1#0007</v>
       </c>
       <c r="I3" s="142" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -13491,7 +13493,7 @@
       </c>
       <c r="J3" s="93"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="100"/>
       <c r="B4" s="136" t="s">
         <v>162</v>
@@ -13517,15 +13519,19 @@
       </c>
       <c r="H4" s="135" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_TOM3F1#0002</v>
+        <v>EUR_YC3MRH_TOM3F1#0007</v>
       </c>
       <c r="I4" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
         <v/>
       </c>
       <c r="J4" s="93"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L4" s="108" t="str">
+        <f>_xll.ohObjectCallerAddress(F4)</f>
+        <v>[EUR_Market.xlsm]FRA!R6C5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="100"/>
       <c r="B5" s="140" t="str">
         <f t="shared" ref="B5:B10" si="3">C5&amp;"M"</f>
@@ -13552,7 +13558,7 @@
       </c>
       <c r="H5" s="138" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1x4F#0002</v>
+        <v>EUR_YC3MRH_1x4F#0007</v>
       </c>
       <c r="I5" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -13560,7 +13566,7 @@
       </c>
       <c r="J5" s="93"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="100"/>
       <c r="B6" s="140" t="str">
         <f t="shared" si="3"/>
@@ -13587,7 +13593,7 @@
       </c>
       <c r="H6" s="138" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2x5F#0002</v>
+        <v>EUR_YC3MRH_2x5F#0007</v>
       </c>
       <c r="I6" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -13595,7 +13601,7 @@
       </c>
       <c r="J6" s="93"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="100"/>
       <c r="B7" s="140" t="str">
         <f t="shared" si="3"/>
@@ -13622,7 +13628,7 @@
       </c>
       <c r="H7" s="138" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3x6F#0002</v>
+        <v>EUR_YC3MRH_3x6F#0007</v>
       </c>
       <c r="I7" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -13630,7 +13636,7 @@
       </c>
       <c r="J7" s="93"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="100"/>
       <c r="B8" s="140" t="str">
         <f t="shared" si="3"/>
@@ -13657,7 +13663,7 @@
       </c>
       <c r="H8" s="138" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_4x7F#0002</v>
+        <v>EUR_YC3MRH_4x7F#0007</v>
       </c>
       <c r="I8" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -13665,7 +13671,7 @@
       </c>
       <c r="J8" s="93"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="100"/>
       <c r="B9" s="140" t="str">
         <f t="shared" si="3"/>
@@ -13692,7 +13698,7 @@
       </c>
       <c r="H9" s="138" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_5x8F#0002</v>
+        <v>EUR_YC3MRH_5x8F#0007</v>
       </c>
       <c r="I9" s="137" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -13700,7 +13706,7 @@
       </c>
       <c r="J9" s="93"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="100"/>
       <c r="B10" s="136" t="str">
         <f t="shared" si="3"/>
@@ -13727,7 +13733,7 @@
       </c>
       <c r="H10" s="135" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_6x9F#0002</v>
+        <v>EUR_YC3MRH_6x9F#0007</v>
       </c>
       <c r="I10" s="134" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -13735,7 +13741,7 @@
       </c>
       <c r="J10" s="93"/>
     </row>
-    <row r="11" spans="1:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="92"/>
       <c r="B11" s="91"/>
       <c r="C11" s="91"/>
@@ -13747,7 +13753,7 @@
       <c r="I11" s="133"/>
       <c r="J11" s="90"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D13" s="108"/>
       <c r="E13" s="108"/>
       <c r="H13" s="108"/>
@@ -13762,9 +13768,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13782,7 +13790,7 @@
     <col min="12" max="16384" width="9.140625" style="89"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="168" t="s">
         <v>168</v>
       </c>
@@ -13802,7 +13810,7 @@
       <c r="J1" s="169"/>
       <c r="K1" s="93"/>
     </row>
-    <row r="2" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="168"/>
       <c r="B2" s="103" t="s">
         <v>167</v>
@@ -13836,7 +13844,7 @@
       </c>
       <c r="K2" s="93"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="162"/>
       <c r="B3" s="166">
         <v>1</v>
@@ -13866,7 +13874,7 @@
       </c>
       <c r="I3" s="165" t="str">
         <f>_xll.qlFuturesRateHelper(H3,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MG4#0002</v>
+        <v>EUR_YC3MRH_FUT3MG4#0007</v>
       </c>
       <c r="J3" s="164" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -13874,8 +13882,12 @@
       </c>
       <c r="K3" s="93"/>
       <c r="L3" s="163"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="89" t="str">
+        <f>_xll.ohObjectCallerAddress(F3)</f>
+        <v>[EUR_Market.xlsm]Futures3M!R7C6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="162"/>
       <c r="B4" s="99">
         <v>2</v>
@@ -13904,7 +13916,7 @@
       </c>
       <c r="I4" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H4,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH4#0002</v>
+        <v>EUR_YC3MRH_FUT3MH4#0007</v>
       </c>
       <c r="J4" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -13913,7 +13925,7 @@
       <c r="K4" s="93"/>
       <c r="L4" s="163"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="162"/>
       <c r="B5" s="99">
         <v>3</v>
@@ -13942,7 +13954,7 @@
       </c>
       <c r="I5" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H5,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MJ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MJ4#0007</v>
       </c>
       <c r="J5" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -13951,7 +13963,7 @@
       <c r="K5" s="93"/>
       <c r="L5" s="163"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="162"/>
       <c r="B6" s="99">
         <v>4</v>
@@ -13980,7 +13992,7 @@
       </c>
       <c r="I6" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H6,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MK4#0002</v>
+        <v>EUR_YC3MRH_FUT3MK4#0007</v>
       </c>
       <c r="J6" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -13989,7 +14001,7 @@
       <c r="K6" s="93"/>
       <c r="L6" s="163"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="162"/>
       <c r="B7" s="99">
         <v>5</v>
@@ -14018,7 +14030,7 @@
       </c>
       <c r="I7" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H7,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM4#0002</v>
+        <v>EUR_YC3MRH_FUT3MM4#0007</v>
       </c>
       <c r="J7" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -14027,7 +14039,7 @@
       <c r="K7" s="93"/>
       <c r="L7" s="163"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="162"/>
       <c r="B8" s="99">
         <v>6</v>
@@ -14056,7 +14068,7 @@
       </c>
       <c r="I8" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H8,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MN4#0002</v>
+        <v>EUR_YC3MRH_FUT3MN4#0007</v>
       </c>
       <c r="J8" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -14065,7 +14077,7 @@
       <c r="K8" s="93"/>
       <c r="L8" s="163"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="162"/>
       <c r="B9" s="99">
         <v>7</v>
@@ -14094,7 +14106,7 @@
       </c>
       <c r="I9" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H9,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MQ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MQ4#0007</v>
       </c>
       <c r="J9" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -14103,7 +14115,7 @@
       <c r="K9" s="93"/>
       <c r="L9" s="163"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="162"/>
       <c r="B10" s="99">
         <v>8</v>
@@ -14132,7 +14144,7 @@
       </c>
       <c r="I10" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H10,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU4#0002</v>
+        <v>EUR_YC3MRH_FUT3MU4#0007</v>
       </c>
       <c r="J10" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -14141,7 +14153,7 @@
       <c r="K10" s="93"/>
       <c r="L10" s="163"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="162"/>
       <c r="B11" s="99">
         <v>9</v>
@@ -14170,7 +14182,7 @@
       </c>
       <c r="I11" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H11,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MV4#0002</v>
+        <v>EUR_YC3MRH_FUT3MV4#0007</v>
       </c>
       <c r="J11" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -14179,7 +14191,7 @@
       <c r="K11" s="93"/>
       <c r="L11" s="163"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="162"/>
       <c r="B12" s="99">
         <v>10</v>
@@ -14208,7 +14220,7 @@
       </c>
       <c r="I12" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H12,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MX4#0002</v>
+        <v>EUR_YC3MRH_FUT3MX4#0007</v>
       </c>
       <c r="J12" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -14217,7 +14229,7 @@
       <c r="K12" s="93"/>
       <c r="L12" s="163"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="162"/>
       <c r="B13" s="99">
         <v>11</v>
@@ -14246,7 +14258,7 @@
       </c>
       <c r="I13" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H13,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ4#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ4#0007</v>
       </c>
       <c r="J13" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -14255,7 +14267,7 @@
       <c r="K13" s="93"/>
       <c r="L13" s="163"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="162"/>
       <c r="B14" s="99">
         <v>12</v>
@@ -14284,7 +14296,7 @@
       </c>
       <c r="I14" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H14,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MF5#0002</v>
+        <v>EUR_YC3MRH_FUT3MF5#0007</v>
       </c>
       <c r="J14" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -14293,7 +14305,7 @@
       <c r="K14" s="93"/>
       <c r="L14" s="163"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="162"/>
       <c r="B15" s="99">
         <v>13</v>
@@ -14322,7 +14334,7 @@
       </c>
       <c r="I15" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H15,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH5#0002</v>
+        <v>EUR_YC3MRH_FUT3MH5#0007</v>
       </c>
       <c r="J15" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -14331,7 +14343,7 @@
       <c r="K15" s="93"/>
       <c r="L15" s="163"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="162"/>
       <c r="B16" s="99">
         <v>14</v>
@@ -14360,7 +14372,7 @@
       </c>
       <c r="I16" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H16,$F16,$D16,$E16,$G16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM5#0002</v>
+        <v>EUR_YC3MRH_FUT3MM5#0007</v>
       </c>
       <c r="J16" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -14398,7 +14410,7 @@
       </c>
       <c r="I17" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H17,$F17,$D17,$E17,$G17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU5#0002</v>
+        <v>EUR_YC3MRH_FUT3MU5#0007</v>
       </c>
       <c r="J17" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -14436,7 +14448,7 @@
       </c>
       <c r="I18" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H18,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ5#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ5#0007</v>
       </c>
       <c r="J18" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -14474,7 +14486,7 @@
       </c>
       <c r="I19" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H19,$F19,$D19,$E19,$G19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH6#0002</v>
+        <v>EUR_YC3MRH_FUT3MH6#0007</v>
       </c>
       <c r="J19" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -14512,7 +14524,7 @@
       </c>
       <c r="I20" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H20,$F20,$D20,$E20,$G20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM6#0002</v>
+        <v>EUR_YC3MRH_FUT3MM6#0007</v>
       </c>
       <c r="J20" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -14550,7 +14562,7 @@
       </c>
       <c r="I21" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H21,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU6#0002</v>
+        <v>EUR_YC3MRH_FUT3MU6#0007</v>
       </c>
       <c r="J21" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -14588,7 +14600,7 @@
       </c>
       <c r="I22" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H22,$F22,$D22,$E22,$G22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ6#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ6#0007</v>
       </c>
       <c r="J22" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -14626,7 +14638,7 @@
       </c>
       <c r="I23" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H23,$F23,$D23,$E23,$G23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH7#0002</v>
+        <v>EUR_YC3MRH_FUT3MH7#0007</v>
       </c>
       <c r="J23" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
@@ -14664,7 +14676,7 @@
       </c>
       <c r="I24" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H24,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM7#0002</v>
+        <v>EUR_YC3MRH_FUT3MM7#0007</v>
       </c>
       <c r="J24" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I24)</f>
@@ -14702,7 +14714,7 @@
       </c>
       <c r="I25" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H25,$F25,$D25,$E25,$G25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU7#0002</v>
+        <v>EUR_YC3MRH_FUT3MU7#0007</v>
       </c>
       <c r="J25" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I25)</f>
@@ -14740,7 +14752,7 @@
       </c>
       <c r="I26" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H26,$F26,$D26,$E26,$G26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ7#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ7#0007</v>
       </c>
       <c r="J26" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
@@ -14778,7 +14790,7 @@
       </c>
       <c r="I27" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H27,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH8#0002</v>
+        <v>EUR_YC3MRH_FUT3MH8#0007</v>
       </c>
       <c r="J27" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I27)</f>
@@ -14816,7 +14828,7 @@
       </c>
       <c r="I28" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H28,$F28,$D28,$E28,$G28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM8#0002</v>
+        <v>EUR_YC3MRH_FUT3MM8#0007</v>
       </c>
       <c r="J28" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I28)</f>
@@ -14854,7 +14866,7 @@
       </c>
       <c r="I29" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H29,$F29,$D29,$E29,$G29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU8#0002</v>
+        <v>EUR_YC3MRH_FUT3MU8#0007</v>
       </c>
       <c r="J29" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
@@ -14892,7 +14904,7 @@
       </c>
       <c r="I30" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H30,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ8#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ8#0007</v>
       </c>
       <c r="J30" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I30)</f>
@@ -14930,7 +14942,7 @@
       </c>
       <c r="I31" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H31,$F31,$D31,$E31,$G31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH9#0002</v>
+        <v>EUR_YC3MRH_FUT3MH9#0007</v>
       </c>
       <c r="J31" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I31)</f>
@@ -14968,7 +14980,7 @@
       </c>
       <c r="I32" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H32,$F32,$D32,$E32,$G32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM9#0002</v>
+        <v>EUR_YC3MRH_FUT3MM9#0007</v>
       </c>
       <c r="J32" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
@@ -15006,7 +15018,7 @@
       </c>
       <c r="I33" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H33,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU9#0002</v>
+        <v>EUR_YC3MRH_FUT3MU9#0007</v>
       </c>
       <c r="J33" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I33)</f>
@@ -15044,7 +15056,7 @@
       </c>
       <c r="I34" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H34,$F34,$D34,$E34,$G34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ9#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ9#0007</v>
       </c>
       <c r="J34" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I34)</f>
@@ -15082,7 +15094,7 @@
       </c>
       <c r="I35" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H35,$F35,$D35,$E35,$G35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH0#0002</v>
+        <v>EUR_YC3MRH_FUT3MH0#0007</v>
       </c>
       <c r="J35" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
@@ -15120,7 +15132,7 @@
       </c>
       <c r="I36" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H36,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM0#0002</v>
+        <v>EUR_YC3MRH_FUT3MM0#0007</v>
       </c>
       <c r="J36" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
@@ -15158,7 +15170,7 @@
       </c>
       <c r="I37" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H37,$F37,$D37,$E37,$G37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU0#0002</v>
+        <v>EUR_YC3MRH_FUT3MU0#0007</v>
       </c>
       <c r="J37" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I37)</f>
@@ -15196,7 +15208,7 @@
       </c>
       <c r="I38" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H38,$F38,$D38,$E38,$G38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ0#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ0#0007</v>
       </c>
       <c r="J38" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
@@ -15234,7 +15246,7 @@
       </c>
       <c r="I39" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H39,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH1#0002</v>
+        <v>EUR_YC3MRH_FUT3MH1#0007</v>
       </c>
       <c r="J39" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I39)</f>
@@ -15272,7 +15284,7 @@
       </c>
       <c r="I40" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H40,$F40,$D40,$E40,$G40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM1#0002</v>
+        <v>EUR_YC3MRH_FUT3MM1#0007</v>
       </c>
       <c r="J40" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I40)</f>
@@ -15309,7 +15321,7 @@
       </c>
       <c r="I41" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H41,$F41,$D41,$E41,$G41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MU1#0002</v>
+        <v>EUR_YC3MRH_FUT3MU1#0007</v>
       </c>
       <c r="J41" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
@@ -15346,7 +15358,7 @@
       </c>
       <c r="I42" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H42,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MZ1#0002</v>
+        <v>EUR_YC3MRH_FUT3MZ1#0007</v>
       </c>
       <c r="J42" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I42)</f>
@@ -15383,7 +15395,7 @@
       </c>
       <c r="I43" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H43,$F43,$D43,$E43,$G43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MH2#0002</v>
+        <v>EUR_YC3MRH_FUT3MH2#0007</v>
       </c>
       <c r="J43" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I43)</f>
@@ -15420,7 +15432,7 @@
       </c>
       <c r="I44" s="158" t="str">
         <f>_xll.qlFuturesRateHelper(H44,$F44,$D44,$E44,$G44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_FUT3MM2#0002</v>
+        <v>EUR_YC3MRH_FUT3MM2#0007</v>
       </c>
       <c r="J44" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(I44)</f>
@@ -15451,9 +15463,11 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15478,7 +15492,7 @@
     <col min="19" max="16384" width="9.140625" style="108"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="173" t="s">
         <v>186</v>
       </c>
@@ -15496,7 +15510,7 @@
       <c r="M1" s="154"/>
       <c r="N1" s="198"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="100"/>
       <c r="B2" s="111"/>
       <c r="C2" s="111"/>
@@ -15520,7 +15534,7 @@
       <c r="M2" s="111"/>
       <c r="N2" s="176"/>
     </row>
-    <row r="3" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="100"/>
       <c r="B3" s="107" t="s">
         <v>180</v>
@@ -15557,7 +15571,7 @@
       </c>
       <c r="N3" s="176"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="112"/>
       <c r="B4" s="111"/>
       <c r="C4" s="111"/>
@@ -15574,7 +15588,7 @@
       </c>
       <c r="L4" s="195" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC3MRH_AB3E_ibor3M#0002</v>
+        <v>EUR_YC3MRH_AB3E_ibor3M#0007</v>
       </c>
       <c r="M4" s="194" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -15582,7 +15596,7 @@
       </c>
       <c r="N4" s="176"/>
     </row>
-    <row r="5" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="112"/>
       <c r="B5" s="111"/>
       <c r="C5" s="111"/>
@@ -15598,7 +15612,7 @@
       <c r="M5" s="111"/>
       <c r="N5" s="176"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="100"/>
       <c r="B6" s="181" t="s">
         <v>163</v>
@@ -15638,7 +15652,7 @@
       </c>
       <c r="L6" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E1Y#0002</v>
+        <v>EUR_YC3MRH_AB3E1Y#0007</v>
       </c>
       <c r="M6" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -15654,8 +15668,12 @@
       <c r="R6" s="191" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T6" s="108" t="str">
+        <f>_xll.ohObjectCallerAddress(J6)</f>
+        <v>[EUR_Market.xlsm]Swap3M!R6C6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="100"/>
       <c r="B7" s="181" t="s">
         <v>163</v>
@@ -15693,7 +15711,7 @@
       </c>
       <c r="L7" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E15M#0002</v>
+        <v>EUR_YC3MRH_AB3E15M#0007</v>
       </c>
       <c r="M7" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -15710,7 +15728,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="100"/>
       <c r="B8" s="181" t="s">
         <v>163</v>
@@ -15748,7 +15766,7 @@
       </c>
       <c r="L8" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E18M#0002</v>
+        <v>EUR_YC3MRH_AB3E18M#0007</v>
       </c>
       <c r="M8" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -15765,7 +15783,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="100"/>
       <c r="B9" s="181" t="s">
         <v>163</v>
@@ -15803,7 +15821,7 @@
       </c>
       <c r="L9" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E21M#0002</v>
+        <v>EUR_YC3MRH_AB3E21M#0007</v>
       </c>
       <c r="M9" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -15820,7 +15838,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
       <c r="B10" s="181" t="s">
         <v>163</v>
@@ -15858,7 +15876,7 @@
       </c>
       <c r="L10" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E2Y#0002</v>
+        <v>EUR_YC3MRH_AB3E2Y#0007</v>
       </c>
       <c r="M10" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -15875,7 +15893,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="100"/>
       <c r="B11" s="181" t="s">
         <v>163</v>
@@ -15913,7 +15931,7 @@
       </c>
       <c r="L11" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E3Y#0002</v>
+        <v>EUR_YC3MRH_AB3E3Y#0007</v>
       </c>
       <c r="M11" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -15921,7 +15939,7 @@
       </c>
       <c r="N11" s="176"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="100"/>
       <c r="B12" s="181" t="s">
         <v>163</v>
@@ -15959,7 +15977,7 @@
       </c>
       <c r="L12" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E4Y#0002</v>
+        <v>EUR_YC3MRH_AB3E4Y#0007</v>
       </c>
       <c r="M12" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -15967,7 +15985,7 @@
       </c>
       <c r="N12" s="176"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="100"/>
       <c r="B13" s="181" t="s">
         <v>163</v>
@@ -16005,7 +16023,7 @@
       </c>
       <c r="L13" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E5Y#0002</v>
+        <v>EUR_YC3MRH_AB3E5Y#0007</v>
       </c>
       <c r="M13" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -16013,7 +16031,7 @@
       </c>
       <c r="N13" s="176"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="100"/>
       <c r="B14" s="181" t="s">
         <v>163</v>
@@ -16051,7 +16069,7 @@
       </c>
       <c r="L14" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E6Y#0002</v>
+        <v>EUR_YC3MRH_AB3E6Y#0007</v>
       </c>
       <c r="M14" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -16059,7 +16077,7 @@
       </c>
       <c r="N14" s="176"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="100"/>
       <c r="B15" s="181" t="s">
         <v>163</v>
@@ -16097,7 +16115,7 @@
       </c>
       <c r="L15" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E7Y#0002</v>
+        <v>EUR_YC3MRH_AB3E7Y#0007</v>
       </c>
       <c r="M15" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -16105,7 +16123,7 @@
       </c>
       <c r="N15" s="176"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="100"/>
       <c r="B16" s="181" t="s">
         <v>163</v>
@@ -16143,7 +16161,7 @@
       </c>
       <c r="L16" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E8Y#0002</v>
+        <v>EUR_YC3MRH_AB3E8Y#0007</v>
       </c>
       <c r="M16" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -16189,7 +16207,7 @@
       </c>
       <c r="L17" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E9Y#0002</v>
+        <v>EUR_YC3MRH_AB3E9Y#0007</v>
       </c>
       <c r="M17" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -16235,7 +16253,7 @@
       </c>
       <c r="L18" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E10Y#0002</v>
+        <v>EUR_YC3MRH_AB3E10Y#0007</v>
       </c>
       <c r="M18" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -16281,7 +16299,7 @@
       </c>
       <c r="L19" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E11Y#0002</v>
+        <v>EUR_YC3MRH_AB3E11Y#0007</v>
       </c>
       <c r="M19" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -16327,7 +16345,7 @@
       </c>
       <c r="L20" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E12Y#0002</v>
+        <v>EUR_YC3MRH_AB3E12Y#0007</v>
       </c>
       <c r="M20" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -16373,7 +16391,7 @@
       </c>
       <c r="L21" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E13Y#0002</v>
+        <v>EUR_YC3MRH_AB3E13Y#0007</v>
       </c>
       <c r="M21" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -16419,7 +16437,7 @@
       </c>
       <c r="L22" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E14Y#0002</v>
+        <v>EUR_YC3MRH_AB3E14Y#0007</v>
       </c>
       <c r="M22" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -16465,7 +16483,7 @@
       </c>
       <c r="L23" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E15Y#0002</v>
+        <v>EUR_YC3MRH_AB3E15Y#0007</v>
       </c>
       <c r="M23" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -16511,7 +16529,7 @@
       </c>
       <c r="L24" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E16Y#0002</v>
+        <v>EUR_YC3MRH_AB3E16Y#0007</v>
       </c>
       <c r="M24" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -16557,7 +16575,7 @@
       </c>
       <c r="L25" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E17Y#0002</v>
+        <v>EUR_YC3MRH_AB3E17Y#0007</v>
       </c>
       <c r="M25" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -16603,7 +16621,7 @@
       </c>
       <c r="L26" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E18Y#0002</v>
+        <v>EUR_YC3MRH_AB3E18Y#0007</v>
       </c>
       <c r="M26" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -16649,7 +16667,7 @@
       </c>
       <c r="L27" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E19Y#0002</v>
+        <v>EUR_YC3MRH_AB3E19Y#0007</v>
       </c>
       <c r="M27" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -16695,7 +16713,7 @@
       </c>
       <c r="L28" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E20Y#0002</v>
+        <v>EUR_YC3MRH_AB3E20Y#0007</v>
       </c>
       <c r="M28" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -16741,7 +16759,7 @@
       </c>
       <c r="L29" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E21Y#0002</v>
+        <v>EUR_YC3MRH_AB3E21Y#0007</v>
       </c>
       <c r="M29" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -16787,7 +16805,7 @@
       </c>
       <c r="L30" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E22Y#0002</v>
+        <v>EUR_YC3MRH_AB3E22Y#0007</v>
       </c>
       <c r="M30" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -16833,7 +16851,7 @@
       </c>
       <c r="L31" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E23Y#0002</v>
+        <v>EUR_YC3MRH_AB3E23Y#0007</v>
       </c>
       <c r="M31" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -16879,7 +16897,7 @@
       </c>
       <c r="L32" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E24Y#0002</v>
+        <v>EUR_YC3MRH_AB3E24Y#0007</v>
       </c>
       <c r="M32" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -16925,7 +16943,7 @@
       </c>
       <c r="L33" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E25Y#0002</v>
+        <v>EUR_YC3MRH_AB3E25Y#0007</v>
       </c>
       <c r="M33" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -16971,7 +16989,7 @@
       </c>
       <c r="L34" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E26Y#0002</v>
+        <v>EUR_YC3MRH_AB3E26Y#0007</v>
       </c>
       <c r="M34" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -17017,7 +17035,7 @@
       </c>
       <c r="L35" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E27Y#0002</v>
+        <v>EUR_YC3MRH_AB3E27Y#0007</v>
       </c>
       <c r="M35" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -17063,7 +17081,7 @@
       </c>
       <c r="L36" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E28Y#0002</v>
+        <v>EUR_YC3MRH_AB3E28Y#0007</v>
       </c>
       <c r="M36" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -17109,7 +17127,7 @@
       </c>
       <c r="L37" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E29Y#0002</v>
+        <v>EUR_YC3MRH_AB3E29Y#0007</v>
       </c>
       <c r="M37" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -17155,7 +17173,7 @@
       </c>
       <c r="L38" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E30Y#0002</v>
+        <v>EUR_YC3MRH_AB3E30Y#0007</v>
       </c>
       <c r="M38" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -17201,7 +17219,7 @@
       </c>
       <c r="L39" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E35Y#0002</v>
+        <v>EUR_YC3MRH_AB3E35Y#0007</v>
       </c>
       <c r="M39" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -17247,7 +17265,7 @@
       </c>
       <c r="L40" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E40Y#0002</v>
+        <v>EUR_YC3MRH_AB3E40Y#0007</v>
       </c>
       <c r="M40" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -17293,7 +17311,7 @@
       </c>
       <c r="L41" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E50Y#0002</v>
+        <v>EUR_YC3MRH_AB3E50Y#0007</v>
       </c>
       <c r="M41" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -17339,7 +17357,7 @@
       </c>
       <c r="L42" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3E60Y#0002</v>
+        <v>EUR_YC3MRH_AB3E60Y#0007</v>
       </c>
       <c r="M42" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -17397,7 +17415,7 @@
       </c>
       <c r="L44" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S12#0002</v>
+        <v>EUR_YC3MRH_1S12#0007</v>
       </c>
       <c r="M44" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -17442,7 +17460,7 @@
       </c>
       <c r="L45" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2S12#0002</v>
+        <v>EUR_YC3MRH_2S12#0007</v>
       </c>
       <c r="M45" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -17487,7 +17505,7 @@
       </c>
       <c r="L46" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3S12#0002</v>
+        <v>EUR_YC3MRH_3S12#0007</v>
       </c>
       <c r="M46" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -17532,7 +17550,7 @@
       </c>
       <c r="L47" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_4S12#0002</v>
+        <v>EUR_YC3MRH_4S12#0007</v>
       </c>
       <c r="M47" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -17577,7 +17595,7 @@
       </c>
       <c r="L48" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S24#0002</v>
+        <v>EUR_YC3MRH_1S24#0007</v>
       </c>
       <c r="M48" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -17622,7 +17640,7 @@
       </c>
       <c r="L49" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2S24#0002</v>
+        <v>EUR_YC3MRH_2S24#0007</v>
       </c>
       <c r="M49" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -17667,7 +17685,7 @@
       </c>
       <c r="L50" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S36#0002</v>
+        <v>EUR_YC3MRH_1S36#0007</v>
       </c>
       <c r="M50" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -17718,9 +17736,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17745,7 +17765,7 @@
     <col min="19" max="16384" width="9.140625" style="108"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="173" t="s">
         <v>187</v>
       </c>
@@ -17763,7 +17783,7 @@
       <c r="M1" s="154"/>
       <c r="N1" s="198"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="100"/>
       <c r="B2" s="111"/>
       <c r="C2" s="111"/>
@@ -17787,7 +17807,7 @@
       <c r="M2" s="111"/>
       <c r="N2" s="176"/>
     </row>
-    <row r="3" spans="1:18" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="100"/>
       <c r="B3" s="107" t="s">
         <v>180</v>
@@ -17824,7 +17844,7 @@
       </c>
       <c r="N3" s="176"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="112"/>
       <c r="B4" s="111"/>
       <c r="C4" s="111"/>
@@ -17841,7 +17861,7 @@
       </c>
       <c r="L4" s="195" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC3MRH_AB3EBASIS_ibor3M#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS_ibor3M#0007</v>
       </c>
       <c r="M4" s="194" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -17849,7 +17869,7 @@
       </c>
       <c r="N4" s="176"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="112"/>
       <c r="B5" s="111"/>
       <c r="C5" s="111"/>
@@ -17865,7 +17885,7 @@
       <c r="M5" s="111"/>
       <c r="N5" s="176"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="100"/>
       <c r="B6" s="207" t="s">
         <v>163</v>
@@ -17905,15 +17925,19 @@
       </c>
       <c r="L6" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS1Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS1Y#0007</v>
       </c>
       <c r="M6" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
         <v/>
       </c>
       <c r="N6" s="176"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T6" s="108" t="str">
+        <f>_xll.ohObjectCallerAddress(J6)</f>
+        <v>'[EUR_Market.xlsm]3M (4)'!R3C10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="100"/>
       <c r="B7" s="181" t="str">
         <f t="shared" ref="B7:B42" si="4">B6</f>
@@ -17954,7 +17978,7 @@
       </c>
       <c r="L7" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS15M#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS15M#0007</v>
       </c>
       <c r="M7" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -17962,7 +17986,7 @@
       </c>
       <c r="N7" s="176"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="100"/>
       <c r="B8" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18003,7 +18027,7 @@
       </c>
       <c r="L8" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS18M#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS18M#0007</v>
       </c>
       <c r="M8" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -18011,7 +18035,7 @@
       </c>
       <c r="N8" s="176"/>
     </row>
-    <row r="9" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="100"/>
       <c r="B9" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18052,7 +18076,7 @@
       </c>
       <c r="L9" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS21M#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS21M#0007</v>
       </c>
       <c r="M9" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -18060,7 +18084,7 @@
       </c>
       <c r="N9" s="176"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="100"/>
       <c r="B10" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18101,7 +18125,7 @@
       </c>
       <c r="L10" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS2Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS2Y#0007</v>
       </c>
       <c r="M10" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -18118,7 +18142,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="100"/>
       <c r="B11" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18159,7 +18183,7 @@
       </c>
       <c r="L11" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS3Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS3Y#0007</v>
       </c>
       <c r="M11" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -18176,7 +18200,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="100"/>
       <c r="B12" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18217,7 +18241,7 @@
       </c>
       <c r="L12" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS4Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS4Y#0007</v>
       </c>
       <c r="M12" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -18234,7 +18258,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="100"/>
       <c r="B13" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18275,7 +18299,7 @@
       </c>
       <c r="L13" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS5Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS5Y#0007</v>
       </c>
       <c r="M13" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -18292,7 +18316,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="100"/>
       <c r="B14" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18333,7 +18357,7 @@
       </c>
       <c r="L14" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS6Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS6Y#0007</v>
       </c>
       <c r="M14" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -18350,7 +18374,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="100"/>
       <c r="B15" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18391,7 +18415,7 @@
       </c>
       <c r="L15" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS7Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS7Y#0007</v>
       </c>
       <c r="M15" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -18402,7 +18426,7 @@
       <c r="Q15" s="175"/>
       <c r="R15" s="175"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="100"/>
       <c r="B16" s="181" t="str">
         <f t="shared" si="4"/>
@@ -18443,7 +18467,7 @@
       </c>
       <c r="L16" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS8Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS8Y#0007</v>
       </c>
       <c r="M16" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -18492,7 +18516,7 @@
       </c>
       <c r="L17" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS9Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS9Y#0007</v>
       </c>
       <c r="M17" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -18541,7 +18565,7 @@
       </c>
       <c r="L18" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS10Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS10Y#0007</v>
       </c>
       <c r="M18" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -18590,7 +18614,7 @@
       </c>
       <c r="L19" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS11Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS11Y#0007</v>
       </c>
       <c r="M19" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -18639,7 +18663,7 @@
       </c>
       <c r="L20" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS12Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS12Y#0007</v>
       </c>
       <c r="M20" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -18688,7 +18712,7 @@
       </c>
       <c r="L21" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS13Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS13Y#0007</v>
       </c>
       <c r="M21" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -18737,7 +18761,7 @@
       </c>
       <c r="L22" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS14Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS14Y#0007</v>
       </c>
       <c r="M22" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -18786,7 +18810,7 @@
       </c>
       <c r="L23" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS15Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS15Y#0007</v>
       </c>
       <c r="M23" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -18835,7 +18859,7 @@
       </c>
       <c r="L24" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS16Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS16Y#0007</v>
       </c>
       <c r="M24" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -18884,7 +18908,7 @@
       </c>
       <c r="L25" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS17Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS17Y#0007</v>
       </c>
       <c r="M25" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -18933,7 +18957,7 @@
       </c>
       <c r="L26" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS18Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS18Y#0007</v>
       </c>
       <c r="M26" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -18982,7 +19006,7 @@
       </c>
       <c r="L27" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS19Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS19Y#0007</v>
       </c>
       <c r="M27" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -19031,7 +19055,7 @@
       </c>
       <c r="L28" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS20Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS20Y#0007</v>
       </c>
       <c r="M28" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -19080,7 +19104,7 @@
       </c>
       <c r="L29" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS21Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS21Y#0007</v>
       </c>
       <c r="M29" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -19129,7 +19153,7 @@
       </c>
       <c r="L30" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS22Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS22Y#0007</v>
       </c>
       <c r="M30" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -19178,7 +19202,7 @@
       </c>
       <c r="L31" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS23Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS23Y#0007</v>
       </c>
       <c r="M31" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -19227,7 +19251,7 @@
       </c>
       <c r="L32" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS24Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS24Y#0007</v>
       </c>
       <c r="M32" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -19276,7 +19300,7 @@
       </c>
       <c r="L33" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS25Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS25Y#0007</v>
       </c>
       <c r="M33" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -19325,7 +19349,7 @@
       </c>
       <c r="L34" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS26Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS26Y#0007</v>
       </c>
       <c r="M34" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -19374,7 +19398,7 @@
       </c>
       <c r="L35" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS27Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS27Y#0007</v>
       </c>
       <c r="M35" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -19423,7 +19447,7 @@
       </c>
       <c r="L36" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS28Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS28Y#0007</v>
       </c>
       <c r="M36" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -19472,7 +19496,7 @@
       </c>
       <c r="L37" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS29Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS29Y#0007</v>
       </c>
       <c r="M37" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -19521,7 +19545,7 @@
       </c>
       <c r="L38" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS30Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS30Y#0007</v>
       </c>
       <c r="M38" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -19570,7 +19594,7 @@
       </c>
       <c r="L39" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS35Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS35Y#0007</v>
       </c>
       <c r="M39" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -19619,7 +19643,7 @@
       </c>
       <c r="L40" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS40Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS40Y#0007</v>
       </c>
       <c r="M40" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -19668,7 +19692,7 @@
       </c>
       <c r="L41" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS50Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS50Y#0007</v>
       </c>
       <c r="M41" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -19717,7 +19741,7 @@
       </c>
       <c r="L42" s="178" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_AB3EBASIS60Y#0002</v>
+        <v>EUR_YC3MRH_AB3EBASIS60Y#0007</v>
       </c>
       <c r="M42" s="177" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>